<commit_message>
finished down and upsampling finished analysis_master data injection, started first loop
</commit_message>
<xml_diff>
--- a/settings.xlsx
+++ b/settings.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24332"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26924"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://charitede-my.sharepoint.com/personal/lev_petrov_charite_de/Documents/DOCTORATE/Cytomata/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="20" documentId="11_F25DC773A252ABDACC104856411A5CB85ADE58E9" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C995146E-EA22-4560-9613-6C450B57977E}"/>
+  <xr:revisionPtr revIDLastSave="91" documentId="11_F25DC773A252ABDACC104856411A5CB85ADE58E9" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{91DD4601-2EF2-488E-BC87-8FBEF99DDD6D}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="5985" yWindow="840" windowWidth="28800" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="46">
   <si>
     <t>setting</t>
   </si>
@@ -129,16 +129,57 @@
     <t>Pre-gated subsets of events that you want to be analyzed. These should be the exact names of folders in fcs/4_subsets/.</t>
   </si>
   <si>
-    <t>Whether to down- or upsample events PER SAMPLE using a given factor. You might want to downsample if studying e.g. granulocytes (on whole blood) to reduce computational burden and oversample if interested in finding rare populations. Downsampling could also be used to reduce the dominance of the oversized samples, while oversampling could be used to enhance the representation of the undersized ones. The cutoff for downsampling is 50% of the most abundant sample (samples are not reduced in size beyond that threshold). The cutoff for oversampling is 50% of the most abundant sample (samples are not increased in size beyond that threshold). Accepts multiple values separated by comma if different needed for each data_subset. Order is given by data_subset order.</t>
+    <t>normalization settings</t>
+  </si>
+  <si>
+    <t>0 (off) or 1 (on).</t>
+  </si>
+  <si>
+    <t>do_normalization</t>
+  </si>
+  <si>
+    <t>database injection settings</t>
+  </si>
+  <si>
+    <t>do_database_injection</t>
+  </si>
+  <si>
+    <t>analysis settings</t>
+  </si>
+  <si>
+    <t>clustering settings</t>
+  </si>
+  <si>
+    <t>UMAP settings</t>
+  </si>
+  <si>
+    <t>do_analysis</t>
+  </si>
+  <si>
+    <t>Whether to down- or upsample events PER SAMPLE using a given factor. You might want to downsample if studying e.g. granulocytes (on whole blood) to reduce computational burden and oversample if interested in finding rare populations. Downsampling could also be used to reduce the dominance of the oversized samples, while oversampling could be used to enhance the representation of the undersized ones. The cutoff for downsampling is the average sample size across all samples (samples are not reduced in size beyond that threshold). The cutoff for oversampling is the average sample size across all samples (samples are not increased in size beyond that threshold). Accepts multiple values separated by comma if different needed for each data_subset. Order is given by data_subset order.</t>
+  </si>
+  <si>
+    <t>event_cutoff</t>
+  </si>
+  <si>
+    <t>minimal sample size to be included. Samples that are too small can  lead to outliers in cluster abundances. 0 can be selected to ommit filtering by event size.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="16"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -153,7 +194,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="12">
     <border>
       <left/>
       <right/>
@@ -161,17 +202,176 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -453,174 +653,260 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C14"/>
+  <dimension ref="A1:C23"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+    <sheetView tabSelected="1" topLeftCell="A15" workbookViewId="0">
+      <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="23.109375" style="1" customWidth="1"/>
-    <col min="2" max="2" width="28.44140625" style="1" customWidth="1"/>
+    <col min="1" max="1" width="23.140625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="28.42578125" style="1" customWidth="1"/>
     <col min="3" max="3" width="59" style="2" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:3" ht="21.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="4" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A2" s="1" t="s">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="B2" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="C2" s="7" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A3" s="1" t="s">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" s="8" t="s">
         <v>4</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="C3" s="2" t="s">
+      <c r="C3" s="9" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A4" s="1" t="s">
+    <row r="4" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+      <c r="A4" s="8" t="s">
         <v>5</v>
       </c>
       <c r="B4" s="1">
         <v>1</v>
       </c>
-      <c r="C4" s="2" t="s">
+      <c r="C4" s="9" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A5" s="1" t="s">
+    <row r="5" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="B5" s="1" t="s">
+      <c r="B5" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="C5" s="2" t="s">
+      <c r="C5" s="12" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="6" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A6" s="1" t="s">
+    <row r="6" spans="1:3" ht="21.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="16" t="s">
+        <v>34</v>
+      </c>
+      <c r="B6" s="16"/>
+      <c r="C6" s="16"/>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="B7" s="6">
+        <v>0</v>
+      </c>
+      <c r="C7" s="7" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="B6" s="1" t="s">
+      <c r="B8" s="11" t="s">
         <v>19</v>
       </c>
-      <c r="C6" s="2" t="s">
+      <c r="C8" s="12" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="7" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A7" s="1" t="s">
+    <row r="9" spans="1:3" ht="21.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="16" t="s">
+        <v>37</v>
+      </c>
+      <c r="B9" s="16"/>
+      <c r="C9" s="16"/>
+    </row>
+    <row r="10" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="13" t="s">
+        <v>38</v>
+      </c>
+      <c r="B10" s="14">
+        <v>0</v>
+      </c>
+      <c r="C10" s="15" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" ht="21.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="16" t="s">
+        <v>39</v>
+      </c>
+      <c r="B11" s="16"/>
+      <c r="C11" s="16"/>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="B12" s="6">
+        <v>1</v>
+      </c>
+      <c r="C12" s="7" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A13" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="B7" s="1" t="s">
+      <c r="B13" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="C7" s="2" t="s">
+      <c r="C13" s="9" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="8" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A8" s="1" t="s">
+    <row r="14" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A14" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="B8" s="1" t="s">
+      <c r="B14" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="C8" s="2" t="s">
+      <c r="C14" s="9" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="9" spans="1:3" ht="172.8" x14ac:dyDescent="0.3">
-      <c r="A9" s="1" t="s">
+    <row r="15" spans="1:3" ht="210" x14ac:dyDescent="0.25">
+      <c r="A15" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="B9" s="1">
+      <c r="B15" s="1">
         <v>1</v>
       </c>
-      <c r="C9" s="2" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A10" s="1" t="s">
+      <c r="C15" s="9" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+      <c r="A16" s="8" t="s">
+        <v>44</v>
+      </c>
+      <c r="B16" s="1">
+        <v>100</v>
+      </c>
+      <c r="C16" s="9" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="B10" s="1">
+      <c r="B17" s="11">
         <v>0</v>
       </c>
-      <c r="C10" s="2" t="s">
+      <c r="C17" s="12" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="11" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A11" s="1" t="s">
+    <row r="18" spans="1:3" ht="21.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A18" s="16" t="s">
+        <v>40</v>
+      </c>
+      <c r="B18" s="16"/>
+      <c r="C18" s="16"/>
+    </row>
+    <row r="19" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+      <c r="A19" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="B11" s="1" t="s">
+      <c r="B19" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="C11" s="2" t="s">
+      <c r="C19" s="7" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="12" spans="1:3" ht="72" x14ac:dyDescent="0.3">
-      <c r="A12" s="1" t="s">
+    <row r="20" spans="1:3" ht="75.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A20" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="B12" s="1">
+      <c r="B20" s="11">
         <v>30</v>
       </c>
-      <c r="C12" s="2" t="s">
+      <c r="C20" s="12" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="13" spans="1:3" ht="72" x14ac:dyDescent="0.3">
-      <c r="A13" s="1" t="s">
+    <row r="21" spans="1:3" ht="21.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A21" s="16" t="s">
+        <v>41</v>
+      </c>
+      <c r="B21" s="16"/>
+      <c r="C21" s="16"/>
+    </row>
+    <row r="22" spans="1:3" ht="75" x14ac:dyDescent="0.25">
+      <c r="A22" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="B13" s="1">
+      <c r="B22" s="6">
         <v>15</v>
       </c>
-      <c r="C13" s="2" t="s">
+      <c r="C22" s="7" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="14" spans="1:3" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A14" s="1" t="s">
+    <row r="23" spans="1:3" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A23" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="B14" s="1">
+      <c r="B23" s="11">
         <v>0.1</v>
       </c>
-      <c r="C14" s="2" t="s">
+      <c r="C23" s="12" t="s">
         <v>29</v>
       </c>
     </row>
   </sheetData>
+  <mergeCells count="5">
+    <mergeCell ref="A18:C18"/>
+    <mergeCell ref="A21:C21"/>
+    <mergeCell ref="A11:C11"/>
+    <mergeCell ref="A9:C9"/>
+    <mergeCell ref="A6:C6"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
prepared calls for scripts, feature pre-selection, variance-feature removal, z-scaling
</commit_message>
<xml_diff>
--- a/settings.xlsx
+++ b/settings.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://charitede-my.sharepoint.com/personal/lev_petrov_charite_de/Documents/DOCTORATE/Cytomata/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="91" documentId="11_F25DC773A252ABDACC104856411A5CB85ADE58E9" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{91DD4601-2EF2-488E-BC87-8FBEF99DDD6D}"/>
+  <xr:revisionPtr revIDLastSave="92" documentId="11_F25DC773A252ABDACC104856411A5CB85ADE58E9" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{4CE2C7D2-6FC7-4DEB-90B6-FF216ACDF055}"/>
   <bookViews>
-    <workbookView xWindow="5985" yWindow="840" windowWidth="28800" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="15" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="47">
   <si>
     <t>setting</t>
   </si>
@@ -163,6 +163,9 @@
   </si>
   <si>
     <t>minimal sample size to be included. Samples that are too small can  lead to outliers in cluster abundances. 0 can be selected to ommit filtering by event size.</t>
+  </si>
+  <si>
+    <t>1, 15</t>
   </si>
 </sst>
 </file>
@@ -656,7 +659,7 @@
   <dimension ref="A1:C23"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A15" workbookViewId="0">
-      <selection activeCell="D15" sqref="D15"/>
+      <selection activeCell="A18" sqref="A18:C18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -834,8 +837,8 @@
       <c r="A17" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="B17" s="11">
-        <v>0</v>
+      <c r="B17" s="11" t="s">
+        <v>46</v>
       </c>
       <c r="C17" s="12" t="s">
         <v>30</v>

</xml_diff>

<commit_message>
var. misc. fixes. folder structure now has version control for analysis plots sample count barcharts, also for resampled events
</commit_message>
<xml_diff>
--- a/settings.xlsx
+++ b/settings.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26924"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24332"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://charitede-my.sharepoint.com/personal/lev_petrov_charite_de/Documents/DOCTORATE/Cytomata/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="92" documentId="11_F25DC773A252ABDACC104856411A5CB85ADE58E9" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{4CE2C7D2-6FC7-4DEB-90B6-FF216ACDF055}"/>
+  <xr:revisionPtr revIDLastSave="118" documentId="11_F25DC773A252ABDACC104856411A5CB85ADE58E9" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{1D430BB5-C2D3-45EF-B9FC-37C937929CCA}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="15" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="57480" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="54">
   <si>
     <t>setting</t>
   </si>
@@ -166,6 +166,27 @@
   </si>
   <si>
     <t>1, 15</t>
+  </si>
+  <si>
+    <t>plotting settings</t>
+  </si>
+  <si>
+    <t>figure_object_scaling</t>
+  </si>
+  <si>
+    <t>figure_text_scaling</t>
+  </si>
+  <si>
+    <t>increase factor for bigger objects (points, lines) in figures, or decrease for smaller, try to avoid drastic changes, because it is a multiplicative factor</t>
+  </si>
+  <si>
+    <t>automatic_palette</t>
+  </si>
+  <si>
+    <t>if you want to set a custom palette for your group stratification, set this to 0 and change values in "analysis_plot_settings.R"</t>
+  </si>
+  <si>
+    <t>increase factor for bigger text, labels and legends in figures, or decrease for smaller, try to avoid drastic changes, because it is a multiplicative factor</t>
   </si>
 </sst>
 </file>
@@ -326,7 +347,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -373,7 +394,16 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -656,20 +686,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C23"/>
+  <dimension ref="A1:C27"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A15" workbookViewId="0">
-      <selection activeCell="A18" sqref="A18:C18"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="23.140625" style="1" customWidth="1"/>
-    <col min="2" max="2" width="28.42578125" style="1" customWidth="1"/>
+    <col min="1" max="1" width="23.109375" style="1" customWidth="1"/>
+    <col min="2" max="2" width="28.44140625" style="1" customWidth="1"/>
     <col min="3" max="3" width="59" style="2" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="21.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" ht="21.6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -680,7 +710,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" s="5" t="s">
         <v>3</v>
       </c>
@@ -691,7 +721,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" s="8" t="s">
         <v>4</v>
       </c>
@@ -702,7 +732,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A4" s="8" t="s">
         <v>5</v>
       </c>
@@ -713,7 +743,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="5" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A5" s="10" t="s">
         <v>6</v>
       </c>
@@ -724,14 +754,14 @@
         <v>32</v>
       </c>
     </row>
-    <row r="6" spans="1:3" ht="21.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="16" t="s">
+    <row r="6" spans="1:3" ht="21.6" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A6" s="18" t="s">
         <v>34</v>
       </c>
-      <c r="B6" s="16"/>
-      <c r="C6" s="16"/>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B6" s="18"/>
+      <c r="C6" s="18"/>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" s="5" t="s">
         <v>36</v>
       </c>
@@ -742,7 +772,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="8" spans="1:3" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:3" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A8" s="10" t="s">
         <v>7</v>
       </c>
@@ -753,14 +783,14 @@
         <v>24</v>
       </c>
     </row>
-    <row r="9" spans="1:3" ht="21.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="16" t="s">
+    <row r="9" spans="1:3" ht="21.6" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A9" s="18" t="s">
         <v>37</v>
       </c>
-      <c r="B9" s="16"/>
-      <c r="C9" s="16"/>
-    </row>
-    <row r="10" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B9" s="18"/>
+      <c r="C9" s="18"/>
+    </row>
+    <row r="10" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A10" s="13" t="s">
         <v>38</v>
       </c>
@@ -771,14 +801,14 @@
         <v>35</v>
       </c>
     </row>
-    <row r="11" spans="1:3" ht="21.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="16" t="s">
+    <row r="11" spans="1:3" ht="21.6" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A11" s="18" t="s">
         <v>39</v>
       </c>
-      <c r="B11" s="16"/>
-      <c r="C11" s="16"/>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B11" s="18"/>
+      <c r="C11" s="18"/>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A12" s="5" t="s">
         <v>42</v>
       </c>
@@ -789,7 +819,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="13" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A13" s="8" t="s">
         <v>8</v>
       </c>
@@ -800,7 +830,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="14" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A14" s="8" t="s">
         <v>9</v>
       </c>
@@ -811,7 +841,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="15" spans="1:3" ht="210" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:3" ht="172.8" x14ac:dyDescent="0.3">
       <c r="A15" s="8" t="s">
         <v>10</v>
       </c>
@@ -822,7 +852,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="16" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A16" s="8" t="s">
         <v>44</v>
       </c>
@@ -833,7 +863,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="17" spans="1:3" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:3" ht="43.8" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A17" s="10" t="s">
         <v>11</v>
       </c>
@@ -844,71 +874,112 @@
         <v>30</v>
       </c>
     </row>
-    <row r="18" spans="1:3" ht="21.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="16" t="s">
+    <row r="18" spans="1:3" ht="21.6" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A18" s="19" t="s">
+        <v>47</v>
+      </c>
+      <c r="B18" s="19"/>
+      <c r="C18" s="19"/>
+    </row>
+    <row r="19" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A19" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="B19" s="6">
+        <v>1</v>
+      </c>
+      <c r="C19" s="7" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A20" s="8" t="s">
+        <v>49</v>
+      </c>
+      <c r="B20" s="16">
+        <v>1</v>
+      </c>
+      <c r="C20" s="9" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A21" s="10" t="s">
+        <v>51</v>
+      </c>
+      <c r="B21" s="11">
+        <v>1</v>
+      </c>
+      <c r="C21" s="12" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" ht="21.6" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A22" s="17" t="s">
         <v>40</v>
       </c>
-      <c r="B18" s="16"/>
-      <c r="C18" s="16"/>
-    </row>
-    <row r="19" spans="1:3" ht="45" x14ac:dyDescent="0.25">
-      <c r="A19" s="5" t="s">
+      <c r="B22" s="17"/>
+      <c r="C22" s="17"/>
+    </row>
+    <row r="23" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A23" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="B19" s="6" t="s">
+      <c r="B23" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="C19" s="7" t="s">
+      <c r="C23" s="7" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="20" spans="1:3" ht="75.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="10" t="s">
+    <row r="24" spans="1:3" ht="72.599999999999994" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A24" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="B20" s="11">
+      <c r="B24" s="11">
         <v>30</v>
       </c>
-      <c r="C20" s="12" t="s">
+      <c r="C24" s="12" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="21" spans="1:3" ht="21.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="16" t="s">
+    <row r="25" spans="1:3" ht="21.6" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A25" s="18" t="s">
         <v>41</v>
       </c>
-      <c r="B21" s="16"/>
-      <c r="C21" s="16"/>
-    </row>
-    <row r="22" spans="1:3" ht="75" x14ac:dyDescent="0.25">
-      <c r="A22" s="5" t="s">
+      <c r="B25" s="18"/>
+      <c r="C25" s="18"/>
+    </row>
+    <row r="26" spans="1:3" ht="72" x14ac:dyDescent="0.3">
+      <c r="A26" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="B22" s="6">
+      <c r="B26" s="6">
         <v>15</v>
       </c>
-      <c r="C22" s="7" t="s">
+      <c r="C26" s="7" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="23" spans="1:3" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="10" t="s">
+    <row r="27" spans="1:3" ht="58.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A27" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="B23" s="11">
+      <c r="B27" s="11">
         <v>0.1</v>
       </c>
-      <c r="C23" s="12" t="s">
+      <c r="C27" s="12" t="s">
         <v>29</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="5">
-    <mergeCell ref="A18:C18"/>
-    <mergeCell ref="A21:C21"/>
+  <mergeCells count="6">
+    <mergeCell ref="A22:C22"/>
+    <mergeCell ref="A25:C25"/>
     <mergeCell ref="A11:C11"/>
     <mergeCell ref="A9:C9"/>
     <mergeCell ref="A6:C6"/>
+    <mergeCell ref="A18:C18"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
commiting unsynced changes from end of 2023. clustering implementation groundwork
</commit_message>
<xml_diff>
--- a/settings.xlsx
+++ b/settings.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24332"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27029"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://charitede-my.sharepoint.com/personal/lev_petrov_charite_de/Documents/DOCTORATE/Cytomata/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="118" documentId="11_F25DC773A252ABDACC104856411A5CB85ADE58E9" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{1D430BB5-C2D3-45EF-B9FC-37C937929CCA}"/>
+  <xr:revisionPtr revIDLastSave="154" documentId="11_F25DC773A252ABDACC104856411A5CB85ADE58E9" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B292E3B9-F949-4A8B-A874-1E52A096428E}"/>
   <bookViews>
-    <workbookView xWindow="57480" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView minimized="1" xWindow="-27030" yWindow="660" windowWidth="27135" windowHeight="14310" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="58">
   <si>
     <t>setting</t>
   </si>
@@ -108,9 +108,6 @@
     <t>fs = FlowSOM with automatic cluster merging (default), fs_manual = FlowSOM with set k, manual merging possible, pg = PhenoGraph (attention, slow!)</t>
   </si>
   <si>
-    <t>If fs, final number of clusters before automatic merging. If fs_manual, final number of clusters before manual merging. If pg, number of nearest neighbors parameter. Accepts multiple values, separated by comma, if different values are needed for each data_subset. Order is given by data_subset vector.</t>
-  </si>
-  <si>
     <t>UMAPs n_neighbors. Low value leads to better resolution of local structure, high - to better capture of global structure. Default value is 15. Accepts multiple values, separated by comma of different values are needed for each data_subset. Order is given by data_subset vector.</t>
   </si>
   <si>
@@ -187,13 +184,28 @@
   </si>
   <si>
     <t>increase factor for bigger text, labels and legends in figures, or decrease for smaller, try to avoid drastic changes, because it is a multiplicative factor</t>
+  </si>
+  <si>
+    <t>If fs, number of clusters after hierarchical and before automatic merging. If fs_manual, final number of clusters after hierarchical merging. If pg, number of nearest neighbors parameter. Accepts multiple values, separated by comma, if different values are needed for each data_subset. Order is given by data_subset vector.</t>
+  </si>
+  <si>
+    <t>fs_n_dims</t>
+  </si>
+  <si>
+    <t>controls the size of SOM. e.g. 10 gives a total of 100 nodes in SOM (xdim of 10 and ydim of 10), 20 results in 400 etc. default value is 10.</t>
+  </si>
+  <si>
+    <t>ccp_delta_cutoff</t>
+  </si>
+  <si>
+    <t>used for automatic detection of optimal number of clusters in "fs" clustering engine. minimal increase in CDF area under the curve after adding one more cluster. When increase reaches a plateu, maximum clustering consensus has probably been reached.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -209,6 +221,12 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9CDCFE"/>
+      <name val="Consolas"/>
+      <family val="3"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -347,7 +365,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -394,8 +412,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -686,20 +710,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C27"/>
+  <dimension ref="A1:G29"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="K13" sqref="K13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="23.109375" style="1" customWidth="1"/>
-    <col min="2" max="2" width="28.44140625" style="1" customWidth="1"/>
+    <col min="1" max="1" width="23.140625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="28.42578125" style="1" customWidth="1"/>
     <col min="3" max="3" width="59" style="2" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="21.6" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:3" ht="21.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -710,7 +734,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
         <v>3</v>
       </c>
@@ -718,10 +742,10 @@
         <v>16</v>
       </c>
       <c r="C2" s="7" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="8" t="s">
         <v>4</v>
       </c>
@@ -729,97 +753,97 @@
         <v>17</v>
       </c>
       <c r="C3" s="9" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4" s="11" t="s">
+        <v>18</v>
+      </c>
+      <c r="C4" s="12" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A4" s="8" t="s">
+    <row r="5" spans="1:3" ht="21.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="20" t="s">
+        <v>33</v>
+      </c>
+      <c r="B5" s="20"/>
+      <c r="C5" s="20"/>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="B6" s="6">
+        <v>0</v>
+      </c>
+      <c r="C6" s="7" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="B7" s="11" t="s">
+        <v>19</v>
+      </c>
+      <c r="C7" s="12" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" ht="21.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="20" t="s">
+        <v>36</v>
+      </c>
+      <c r="B8" s="20"/>
+      <c r="C8" s="20"/>
+    </row>
+    <row r="9" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="13" t="s">
+        <v>37</v>
+      </c>
+      <c r="B9" s="14">
+        <v>0</v>
+      </c>
+      <c r="C9" s="15" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" ht="21.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="20" t="s">
+        <v>38</v>
+      </c>
+      <c r="B10" s="20"/>
+      <c r="C10" s="20"/>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="B11" s="6">
+        <v>1</v>
+      </c>
+      <c r="C11" s="7" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+      <c r="A12" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="B4" s="1">
+      <c r="B12" s="1">
         <v>1</v>
       </c>
-      <c r="C4" s="9" t="s">
+      <c r="C12" s="9" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="5" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A5" s="10" t="s">
-        <v>6</v>
-      </c>
-      <c r="B5" s="11" t="s">
-        <v>18</v>
-      </c>
-      <c r="C5" s="12" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" ht="21.6" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A6" s="18" t="s">
-        <v>34</v>
-      </c>
-      <c r="B6" s="18"/>
-      <c r="C6" s="18"/>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A7" s="5" t="s">
-        <v>36</v>
-      </c>
-      <c r="B7" s="6">
-        <v>0</v>
-      </c>
-      <c r="C7" s="7" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A8" s="10" t="s">
-        <v>7</v>
-      </c>
-      <c r="B8" s="11" t="s">
-        <v>19</v>
-      </c>
-      <c r="C8" s="12" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" ht="21.6" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A9" s="18" t="s">
-        <v>37</v>
-      </c>
-      <c r="B9" s="18"/>
-      <c r="C9" s="18"/>
-    </row>
-    <row r="10" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A10" s="13" t="s">
-        <v>38</v>
-      </c>
-      <c r="B10" s="14">
-        <v>0</v>
-      </c>
-      <c r="C10" s="15" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" ht="21.6" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A11" s="18" t="s">
-        <v>39</v>
-      </c>
-      <c r="B11" s="18"/>
-      <c r="C11" s="18"/>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A12" s="5" t="s">
-        <v>42</v>
-      </c>
-      <c r="B12" s="6">
-        <v>1</v>
-      </c>
-      <c r="C12" s="7" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A13" s="8" t="s">
         <v>8</v>
       </c>
@@ -830,7 +854,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="14" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A14" s="8" t="s">
         <v>9</v>
       </c>
@@ -838,10 +862,10 @@
         <v>21</v>
       </c>
       <c r="C14" s="9" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" ht="172.8" x14ac:dyDescent="0.3">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" ht="210" x14ac:dyDescent="0.25">
       <c r="A15" s="8" t="s">
         <v>10</v>
       </c>
@@ -849,79 +873,79 @@
         <v>1</v>
       </c>
       <c r="C15" s="9" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+      <c r="A16" s="8" t="s">
         <v>43</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A16" s="8" t="s">
-        <v>44</v>
       </c>
       <c r="B16" s="1">
         <v>100</v>
       </c>
       <c r="C16" s="9" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" ht="43.8" thickBot="1" x14ac:dyDescent="0.35">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="10" t="s">
         <v>11</v>
       </c>
       <c r="B17" s="11" t="s">
+        <v>45</v>
+      </c>
+      <c r="C17" s="12" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" ht="21.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A18" s="21" t="s">
         <v>46</v>
       </c>
-      <c r="C17" s="12" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" ht="21.6" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A18" s="19" t="s">
+      <c r="B18" s="21"/>
+      <c r="C18" s="21"/>
+    </row>
+    <row r="19" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="A19" s="5" t="s">
         <v>47</v>
-      </c>
-      <c r="B18" s="19"/>
-      <c r="C18" s="19"/>
-    </row>
-    <row r="19" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A19" s="5" t="s">
-        <v>48</v>
       </c>
       <c r="B19" s="6">
         <v>1</v>
       </c>
       <c r="C19" s="7" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="A20" s="8" t="s">
+        <v>48</v>
+      </c>
+      <c r="B20" s="1">
+        <v>1</v>
+      </c>
+      <c r="C20" s="9" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A21" s="10" t="s">
         <v>50</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A20" s="8" t="s">
-        <v>49</v>
-      </c>
-      <c r="B20" s="16">
-        <v>1</v>
-      </c>
-      <c r="C20" s="9" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A21" s="10" t="s">
-        <v>51</v>
       </c>
       <c r="B21" s="11">
         <v>1</v>
       </c>
       <c r="C21" s="12" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3" ht="21.6" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A22" s="17" t="s">
-        <v>40</v>
-      </c>
-      <c r="B22" s="17"/>
-      <c r="C22" s="17"/>
-    </row>
-    <row r="23" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" ht="21.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A22" s="19" t="s">
+        <v>39</v>
+      </c>
+      <c r="B22" s="19"/>
+      <c r="C22" s="19"/>
+    </row>
+    <row r="23" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A23" s="5" t="s">
         <v>12</v>
       </c>
@@ -932,53 +956,76 @@
         <v>26</v>
       </c>
     </row>
-    <row r="24" spans="1:3" ht="72.599999999999994" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A24" s="10" t="s">
+    <row r="24" spans="1:7" ht="90" x14ac:dyDescent="0.25">
+      <c r="A24" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="B24" s="11">
+      <c r="B24" s="1">
         <v>30</v>
       </c>
-      <c r="C24" s="12" t="s">
+      <c r="C24" s="16" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="A25" s="8" t="s">
+        <v>54</v>
+      </c>
+      <c r="B25" s="1">
+        <v>10</v>
+      </c>
+      <c r="C25" s="16" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" ht="75.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A26" s="10" t="s">
+        <v>56</v>
+      </c>
+      <c r="B26" s="11">
+        <v>0.01</v>
+      </c>
+      <c r="C26" s="17" t="s">
+        <v>57</v>
+      </c>
+      <c r="G26" s="18"/>
+    </row>
+    <row r="27" spans="1:7" ht="21.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A27" s="20" t="s">
+        <v>40</v>
+      </c>
+      <c r="B27" s="20"/>
+      <c r="C27" s="20"/>
+    </row>
+    <row r="28" spans="1:7" ht="75" x14ac:dyDescent="0.25">
+      <c r="A28" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="B28" s="6">
+        <v>15</v>
+      </c>
+      <c r="C28" s="7" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="25" spans="1:3" ht="21.6" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A25" s="18" t="s">
-        <v>41</v>
-      </c>
-      <c r="B25" s="18"/>
-      <c r="C25" s="18"/>
-    </row>
-    <row r="26" spans="1:3" ht="72" x14ac:dyDescent="0.3">
-      <c r="A26" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="B26" s="6">
+    <row r="29" spans="1:7" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A29" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="C26" s="7" t="s">
+      <c r="B29" s="11">
+        <v>0.1</v>
+      </c>
+      <c r="C29" s="12" t="s">
         <v>28</v>
-      </c>
-    </row>
-    <row r="27" spans="1:3" ht="58.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A27" s="10" t="s">
-        <v>15</v>
-      </c>
-      <c r="B27" s="11">
-        <v>0.1</v>
-      </c>
-      <c r="C27" s="12" t="s">
-        <v>29</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="6">
     <mergeCell ref="A22:C22"/>
-    <mergeCell ref="A25:C25"/>
-    <mergeCell ref="A11:C11"/>
-    <mergeCell ref="A9:C9"/>
-    <mergeCell ref="A6:C6"/>
+    <mergeCell ref="A27:C27"/>
+    <mergeCell ref="A10:C10"/>
+    <mergeCell ref="A8:C8"/>
+    <mergeCell ref="A5:C5"/>
     <mergeCell ref="A18:C18"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
added update_settings function and exclude_channels setting (for flagging of channels in panel.csv)
</commit_message>
<xml_diff>
--- a/settings.xlsx
+++ b/settings.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27628"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://charitede-my.sharepoint.com/personal/lev_petrov_charite_de/Documents/DOCTORATE/Cytomata/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="154" documentId="11_F25DC773A252ABDACC104856411A5CB85ADE58E9" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B292E3B9-F949-4A8B-A874-1E52A096428E}"/>
+  <xr:revisionPtr revIDLastSave="180" documentId="11_F25DC773A252ABDACC104856411A5CB85ADE58E9" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{44857EA5-BBE2-4D98-909F-3A29C74F0761}"/>
   <bookViews>
-    <workbookView minimized="1" xWindow="-27030" yWindow="660" windowWidth="27135" windowHeight="14310" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-27930" yWindow="1185" windowWidth="22185" windowHeight="15690" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="61">
   <si>
     <t>setting</t>
   </si>
@@ -123,9 +123,6 @@
     <t>Used to find meta-table in meta_folder.</t>
   </si>
   <si>
-    <t>Pre-gated subsets of events that you want to be analyzed. These should be the exact names of folders in fcs/4_subsets/.</t>
-  </si>
-  <si>
     <t>normalization settings</t>
   </si>
   <si>
@@ -199,6 +196,18 @@
   </si>
   <si>
     <t>used for automatic detection of optimal number of clusters in "fs" clustering engine. minimal increase in CDF area under the curve after adding one more cluster. When increase reaches a plateu, maximum clustering consensus has probably been reached.</t>
+  </si>
+  <si>
+    <t>excluded_channels</t>
+  </si>
+  <si>
+    <t>B2M, DNA, Bead, LD, Live, Dead, ID, Cell-ID, Cell_ID</t>
+  </si>
+  <si>
+    <t>Pre-gated subsets of events that you want to analyze. These should be the exact names of folders in fcs/4_subsets/. Separated by comma.</t>
+  </si>
+  <si>
+    <t>Patterns present in the names of pre-processing channels that will be used to remove them. Input separated by comma. This can be adjusted in the panel.csv file afterwards.</t>
   </si>
 </sst>
 </file>
@@ -365,7 +374,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -420,6 +429,9 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -710,10 +722,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G29"/>
+  <dimension ref="A1:G30"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="K13" sqref="K13"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I5" sqref="I5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -756,277 +768,288 @@
         <v>30</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="10" t="s">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="B4" s="11" t="s">
+      <c r="B4" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="C4" s="12" t="s">
+      <c r="C4" s="9" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="5" spans="1:3" ht="21.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="20" t="s">
+    <row r="5" spans="1:3" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="10" t="s">
+        <v>57</v>
+      </c>
+      <c r="B5" s="19" t="s">
+        <v>58</v>
+      </c>
+      <c r="C5" s="12" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" ht="21.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="21" t="s">
+        <v>32</v>
+      </c>
+      <c r="B6" s="21"/>
+      <c r="C6" s="21"/>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="B7" s="6">
+        <v>0</v>
+      </c>
+      <c r="C7" s="7" t="s">
         <v>33</v>
       </c>
-      <c r="B5" s="20"/>
-      <c r="C5" s="20"/>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6" s="5" t="s">
+    </row>
+    <row r="8" spans="1:3" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="B8" s="11" t="s">
+        <v>19</v>
+      </c>
+      <c r="C8" s="12" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" ht="21.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="21" t="s">
         <v>35</v>
       </c>
-      <c r="B6" s="6">
+      <c r="B9" s="21"/>
+      <c r="C9" s="21"/>
+    </row>
+    <row r="10" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="13" t="s">
+        <v>36</v>
+      </c>
+      <c r="B10" s="14">
         <v>0</v>
       </c>
-      <c r="C6" s="7" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="10" t="s">
-        <v>7</v>
-      </c>
-      <c r="B7" s="11" t="s">
-        <v>19</v>
-      </c>
-      <c r="C7" s="12" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" ht="21.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="20" t="s">
-        <v>36</v>
-      </c>
-      <c r="B8" s="20"/>
-      <c r="C8" s="20"/>
-    </row>
-    <row r="9" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="13" t="s">
+      <c r="C10" s="15" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" ht="21.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="21" t="s">
         <v>37</v>
       </c>
-      <c r="B9" s="14">
-        <v>0</v>
-      </c>
-      <c r="C9" s="15" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" ht="21.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="20" t="s">
-        <v>38</v>
-      </c>
-      <c r="B10" s="20"/>
-      <c r="C10" s="20"/>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A11" s="5" t="s">
-        <v>41</v>
-      </c>
-      <c r="B11" s="6">
+      <c r="B11" s="21"/>
+      <c r="C11" s="21"/>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="B12" s="6">
         <v>1</v>
       </c>
-      <c r="C11" s="7" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" ht="45" x14ac:dyDescent="0.25">
-      <c r="A12" s="8" t="s">
+      <c r="C12" s="7" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+      <c r="A13" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="B12" s="1">
+      <c r="B13" s="1">
         <v>1</v>
       </c>
-      <c r="C12" s="9" t="s">
+      <c r="C13" s="9" t="s">
         <v>25</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A13" s="8" t="s">
-        <v>8</v>
-      </c>
-      <c r="B13" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="C13" s="9" t="s">
-        <v>23</v>
       </c>
     </row>
     <row r="14" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A14" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C14" s="9" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+      <c r="A15" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="B14" s="1" t="s">
+      <c r="B15" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="C14" s="9" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" ht="210" x14ac:dyDescent="0.25">
-      <c r="A15" s="8" t="s">
+      <c r="C15" s="9" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" ht="210" x14ac:dyDescent="0.25">
+      <c r="A16" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="B15" s="1">
+      <c r="B16" s="1">
         <v>1</v>
       </c>
-      <c r="C15" s="9" t="s">
+      <c r="C16" s="9" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="A17" s="8" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="16" spans="1:3" ht="45" x14ac:dyDescent="0.25">
-      <c r="A16" s="8" t="s">
+      <c r="B17" s="1">
+        <v>100</v>
+      </c>
+      <c r="C17" s="9" t="s">
         <v>43</v>
       </c>
-      <c r="B16" s="1">
-        <v>100</v>
-      </c>
-      <c r="C16" s="9" t="s">
+    </row>
+    <row r="18" spans="1:7" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A18" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="B18" s="11" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="17" spans="1:7" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="10" t="s">
-        <v>11</v>
-      </c>
-      <c r="B17" s="11" t="s">
+      <c r="C18" s="12" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" ht="21.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A19" s="22" t="s">
         <v>45</v>
       </c>
-      <c r="C17" s="12" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="18" spans="1:7" ht="21.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="21" t="s">
+      <c r="B19" s="22"/>
+      <c r="C19" s="22"/>
+    </row>
+    <row r="20" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="A20" s="5" t="s">
         <v>46</v>
       </c>
-      <c r="B18" s="21"/>
-      <c r="C18" s="21"/>
-    </row>
-    <row r="19" spans="1:7" ht="45" x14ac:dyDescent="0.25">
-      <c r="A19" s="5" t="s">
+      <c r="B20" s="6">
+        <v>1</v>
+      </c>
+      <c r="C20" s="7" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="A21" s="8" t="s">
         <v>47</v>
       </c>
-      <c r="B19" s="6">
+      <c r="B21" s="1">
         <v>1</v>
       </c>
-      <c r="C19" s="7" t="s">
+      <c r="C21" s="9" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A22" s="10" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="20" spans="1:7" ht="45" x14ac:dyDescent="0.25">
-      <c r="A20" s="8" t="s">
-        <v>48</v>
-      </c>
-      <c r="B20" s="1">
+      <c r="B22" s="11">
         <v>1</v>
       </c>
-      <c r="C20" s="9" t="s">
+      <c r="C22" s="12" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" ht="21.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A23" s="20" t="s">
+        <v>38</v>
+      </c>
+      <c r="B23" s="20"/>
+      <c r="C23" s="20"/>
+    </row>
+    <row r="24" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="A24" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="B24" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="C24" s="7" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" ht="90" x14ac:dyDescent="0.25">
+      <c r="A25" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="B25" s="1">
+        <v>30</v>
+      </c>
+      <c r="C25" s="16" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="21" spans="1:7" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="10" t="s">
-        <v>50</v>
-      </c>
-      <c r="B21" s="11">
-        <v>1</v>
-      </c>
-      <c r="C21" s="12" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="22" spans="1:7" ht="21.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="19" t="s">
+    <row r="26" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="A26" s="8" t="s">
+        <v>53</v>
+      </c>
+      <c r="B26" s="1">
+        <v>10</v>
+      </c>
+      <c r="C26" s="16" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" ht="75.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A27" s="10" t="s">
+        <v>55</v>
+      </c>
+      <c r="B27" s="11">
+        <v>0.01</v>
+      </c>
+      <c r="C27" s="17" t="s">
+        <v>56</v>
+      </c>
+      <c r="G27" s="18"/>
+    </row>
+    <row r="28" spans="1:7" ht="21.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A28" s="21" t="s">
         <v>39</v>
       </c>
-      <c r="B22" s="19"/>
-      <c r="C22" s="19"/>
-    </row>
-    <row r="23" spans="1:7" ht="45" x14ac:dyDescent="0.25">
-      <c r="A23" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="B23" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="C23" s="7" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="24" spans="1:7" ht="90" x14ac:dyDescent="0.25">
-      <c r="A24" s="8" t="s">
-        <v>13</v>
-      </c>
-      <c r="B24" s="1">
-        <v>30</v>
-      </c>
-      <c r="C24" s="16" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="25" spans="1:7" ht="45" x14ac:dyDescent="0.25">
-      <c r="A25" s="8" t="s">
-        <v>54</v>
-      </c>
-      <c r="B25" s="1">
-        <v>10</v>
-      </c>
-      <c r="C25" s="16" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="26" spans="1:7" ht="75.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="10" t="s">
-        <v>56</v>
-      </c>
-      <c r="B26" s="11">
-        <v>0.01</v>
-      </c>
-      <c r="C26" s="17" t="s">
-        <v>57</v>
-      </c>
-      <c r="G26" s="18"/>
-    </row>
-    <row r="27" spans="1:7" ht="21.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="20" t="s">
-        <v>40</v>
-      </c>
-      <c r="B27" s="20"/>
-      <c r="C27" s="20"/>
-    </row>
-    <row r="28" spans="1:7" ht="75" x14ac:dyDescent="0.25">
-      <c r="A28" s="5" t="s">
+      <c r="B28" s="21"/>
+      <c r="C28" s="21"/>
+    </row>
+    <row r="29" spans="1:7" ht="75" x14ac:dyDescent="0.25">
+      <c r="A29" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="B28" s="6">
+      <c r="B29" s="6">
         <v>15</v>
       </c>
-      <c r="C28" s="7" t="s">
+      <c r="C29" s="7" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="29" spans="1:7" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A29" s="10" t="s">
+    <row r="30" spans="1:7" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A30" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="B29" s="11">
+      <c r="B30" s="11">
         <v>0.1</v>
       </c>
-      <c r="C29" s="12" t="s">
+      <c r="C30" s="12" t="s">
         <v>28</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="6">
-    <mergeCell ref="A22:C22"/>
-    <mergeCell ref="A27:C27"/>
-    <mergeCell ref="A10:C10"/>
-    <mergeCell ref="A8:C8"/>
-    <mergeCell ref="A5:C5"/>
-    <mergeCell ref="A18:C18"/>
+    <mergeCell ref="A23:C23"/>
+    <mergeCell ref="A28:C28"/>
+    <mergeCell ref="A11:C11"/>
+    <mergeCell ref="A9:C9"/>
+    <mergeCell ref="A6:C6"/>
+    <mergeCell ref="A19:C19"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
added first run mode check. check_sampling_rate improved (added sampling_rate_changed integer for clustering to default back to "do_clustering", added check_feature_input and first_run feature selection logging, feature_input_changed integer for clustering to default back to "do_clustering"
</commit_message>
<xml_diff>
--- a/settings.xlsx
+++ b/settings.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://charitede-my.sharepoint.com/personal/lev_petrov_charite_de/Documents/DOCTORATE/Cytomata/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="180" documentId="11_F25DC773A252ABDACC104856411A5CB85ADE58E9" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{44857EA5-BBE2-4D98-909F-3A29C74F0761}"/>
+  <xr:revisionPtr revIDLastSave="181" documentId="11_F25DC773A252ABDACC104856411A5CB85ADE58E9" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{4E239B27-7D85-4774-845D-0A3F44936CB5}"/>
   <bookViews>
     <workbookView xWindow="-27930" yWindow="1185" windowWidth="22185" windowHeight="15690" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -159,9 +159,6 @@
     <t>minimal sample size to be included. Samples that are too small can  lead to outliers in cluster abundances. 0 can be selected to ommit filtering by event size.</t>
   </si>
   <si>
-    <t>1, 15</t>
-  </si>
-  <si>
     <t>plotting settings</t>
   </si>
   <si>
@@ -208,6 +205,9 @@
   </si>
   <si>
     <t>Patterns present in the names of pre-processing channels that will be used to remove them. Input separated by comma. This can be adjusted in the panel.csv file afterwards.</t>
+  </si>
+  <si>
+    <t>1, 20</t>
   </si>
 </sst>
 </file>
@@ -725,7 +725,7 @@
   <dimension ref="A1:G30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I5" sqref="I5"/>
+      <selection activeCell="J7" sqref="J7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -781,13 +781,13 @@
     </row>
     <row r="5" spans="1:3" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="10" t="s">
+        <v>56</v>
+      </c>
+      <c r="B5" s="19" t="s">
         <v>57</v>
       </c>
-      <c r="B5" s="19" t="s">
-        <v>58</v>
-      </c>
       <c r="C5" s="12" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="6" spans="1:3" ht="21.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -885,7 +885,7 @@
         <v>21</v>
       </c>
       <c r="C15" s="9" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="16" spans="1:3" ht="210" x14ac:dyDescent="0.25">
@@ -915,7 +915,7 @@
         <v>11</v>
       </c>
       <c r="B18" s="11" t="s">
-        <v>44</v>
+        <v>60</v>
       </c>
       <c r="C18" s="12" t="s">
         <v>29</v>
@@ -923,42 +923,42 @@
     </row>
     <row r="19" spans="1:7" ht="21.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A19" s="22" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B19" s="22"/>
       <c r="C19" s="22"/>
     </row>
     <row r="20" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A20" s="5" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B20" s="6">
         <v>1</v>
       </c>
       <c r="C20" s="7" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="21" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A21" s="8" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B21" s="1">
         <v>1</v>
       </c>
       <c r="C21" s="9" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="22" spans="1:7" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A22" s="10" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B22" s="11">
         <v>1</v>
       </c>
       <c r="C22" s="12" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="23" spans="1:7" ht="21.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -987,29 +987,29 @@
         <v>30</v>
       </c>
       <c r="C25" s="16" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="26" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A26" s="8" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B26" s="1">
         <v>10</v>
       </c>
       <c r="C26" s="16" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="27" spans="1:7" ht="75.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A27" s="10" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B27" s="11">
         <v>0.01</v>
       </c>
       <c r="C27" s="17" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="G27" s="18"/>
     </row>

</xml_diff>

<commit_message>
improved folder_manager Added "answer" variable reset after every function assigning it Fixed palette calculation to be deterministic (seed wasn’t being applied globally for some reason)
</commit_message>
<xml_diff>
--- a/settings.xlsx
+++ b/settings.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://charitede-my.sharepoint.com/personal/lev_petrov_charite_de/Documents/DOCTORATE/Cytomata/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="181" documentId="11_F25DC773A252ABDACC104856411A5CB85ADE58E9" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{4E239B27-7D85-4774-845D-0A3F44936CB5}"/>
+  <xr:revisionPtr revIDLastSave="185" documentId="11_F25DC773A252ABDACC104856411A5CB85ADE58E9" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{EB69B38B-8B2F-4DA4-B04D-21784D009C37}"/>
   <bookViews>
-    <workbookView xWindow="-27930" yWindow="1185" windowWidth="22185" windowHeight="15690" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-27240" yWindow="1185" windowWidth="27030" windowHeight="15690" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -78,15 +78,9 @@
     <t>~/DOCTORATE/Cytomata_data/</t>
   </si>
   <si>
-    <t>dev_project_panel_1</t>
-  </si>
-  <si>
     <t>meta</t>
   </si>
   <si>
-    <t>HC-4, HC-100</t>
-  </si>
-  <si>
     <t>sev_age_timepoint, inf_age_timepoint</t>
   </si>
   <si>
@@ -208,6 +202,12 @@
   </si>
   <si>
     <t>1, 20</t>
+  </si>
+  <si>
+    <t>small_dev_project_panel_1</t>
+  </si>
+  <si>
+    <t>HC-100</t>
   </si>
 </sst>
 </file>
@@ -725,7 +725,7 @@
   <dimension ref="A1:G30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J7" sqref="J7"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -754,7 +754,7 @@
         <v>16</v>
       </c>
       <c r="C2" s="7" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
@@ -762,10 +762,10 @@
         <v>4</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>17</v>
+        <v>59</v>
       </c>
       <c r="C3" s="9" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
@@ -773,39 +773,39 @@
         <v>6</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C4" s="9" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
     </row>
     <row r="5" spans="1:3" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="10" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B5" s="19" t="s">
+        <v>55</v>
+      </c>
+      <c r="C5" s="12" t="s">
         <v>57</v>
-      </c>
-      <c r="C5" s="12" t="s">
-        <v>59</v>
       </c>
     </row>
     <row r="6" spans="1:3" ht="21.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="21" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="B6" s="21"/>
       <c r="C6" s="21"/>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" s="5" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="B7" s="6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C7" s="7" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
     </row>
     <row r="8" spans="1:3" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -813,46 +813,46 @@
         <v>7</v>
       </c>
       <c r="B8" s="11" t="s">
-        <v>19</v>
+        <v>60</v>
       </c>
       <c r="C8" s="12" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
     </row>
     <row r="9" spans="1:3" ht="21.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="21" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="B9" s="21"/>
       <c r="C9" s="21"/>
     </row>
     <row r="10" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="13" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="B10" s="14">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C10" s="15" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
     </row>
     <row r="11" spans="1:3" ht="21.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="21" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="B11" s="21"/>
       <c r="C11" s="21"/>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" s="5" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="B12" s="6">
         <v>1</v>
       </c>
       <c r="C12" s="7" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
     </row>
     <row r="13" spans="1:3" ht="45" x14ac:dyDescent="0.25">
@@ -863,7 +863,7 @@
         <v>1</v>
       </c>
       <c r="C13" s="9" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
     </row>
     <row r="14" spans="1:3" ht="30" x14ac:dyDescent="0.25">
@@ -871,10 +871,10 @@
         <v>8</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="C14" s="9" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
     </row>
     <row r="15" spans="1:3" ht="45" x14ac:dyDescent="0.25">
@@ -882,10 +882,10 @@
         <v>9</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="C15" s="9" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
     </row>
     <row r="16" spans="1:3" ht="210" x14ac:dyDescent="0.25">
@@ -896,18 +896,18 @@
         <v>1</v>
       </c>
       <c r="C16" s="9" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
     </row>
     <row r="17" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A17" s="8" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B17" s="1">
         <v>100</v>
       </c>
       <c r="C17" s="9" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
     </row>
     <row r="18" spans="1:7" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -915,55 +915,55 @@
         <v>11</v>
       </c>
       <c r="B18" s="11" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="C18" s="12" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
     </row>
     <row r="19" spans="1:7" ht="21.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A19" s="22" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="B19" s="22"/>
       <c r="C19" s="22"/>
     </row>
     <row r="20" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A20" s="5" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="B20" s="6">
         <v>1</v>
       </c>
       <c r="C20" s="7" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
     </row>
     <row r="21" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A21" s="8" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="B21" s="1">
         <v>1</v>
       </c>
       <c r="C21" s="9" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
     </row>
     <row r="22" spans="1:7" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A22" s="10" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="B22" s="11">
         <v>1</v>
       </c>
       <c r="C22" s="12" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
     </row>
     <row r="23" spans="1:7" ht="21.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A23" s="20" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B23" s="20"/>
       <c r="C23" s="20"/>
@@ -973,10 +973,10 @@
         <v>12</v>
       </c>
       <c r="B24" s="6" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="C24" s="7" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
     </row>
     <row r="25" spans="1:7" ht="90" x14ac:dyDescent="0.25">
@@ -987,35 +987,35 @@
         <v>30</v>
       </c>
       <c r="C25" s="16" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
     </row>
     <row r="26" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A26" s="8" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="B26" s="1">
         <v>10</v>
       </c>
       <c r="C26" s="16" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
     </row>
     <row r="27" spans="1:7" ht="75.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A27" s="10" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="B27" s="11">
         <v>0.01</v>
       </c>
       <c r="C27" s="17" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="G27" s="18"/>
     </row>
     <row r="28" spans="1:7" ht="21.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A28" s="21" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="B28" s="21"/>
       <c r="C28" s="21"/>
@@ -1028,7 +1028,7 @@
         <v>15</v>
       </c>
       <c r="C29" s="7" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
     </row>
     <row r="30" spans="1:7" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1039,7 +1039,7 @@
         <v>0.1</v>
       </c>
       <c r="C30" s="12" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
implemented a powerful summary_table function to calculate means, medians, counts and n_sizes. implemented calculate_cluster_proportions fucntion based on it
</commit_message>
<xml_diff>
--- a/settings.xlsx
+++ b/settings.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27628"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27726"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://charitede-my.sharepoint.com/personal/lev_petrov_charite_de/Documents/DOCTORATE/Cytomata/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="185" documentId="11_F25DC773A252ABDACC104856411A5CB85ADE58E9" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{EB69B38B-8B2F-4DA4-B04D-21784D009C37}"/>
+  <xr:revisionPtr revIDLastSave="188" documentId="11_F25DC773A252ABDACC104856411A5CB85ADE58E9" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{7BF836D1-576C-41D0-91D6-725C8E14BA47}"/>
   <bookViews>
-    <workbookView xWindow="-27240" yWindow="1185" windowWidth="27030" windowHeight="15690" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="1155" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="63">
   <si>
     <t>setting</t>
   </si>
@@ -208,6 +208,12 @@
   </si>
   <si>
     <t>HC-100</t>
+  </si>
+  <si>
+    <t>grouping_orders</t>
+  </si>
+  <si>
+    <t>Control order of groups. Input group names separated by comma. For multiple grouping columns - separate by semicolon.</t>
   </si>
 </sst>
 </file>
@@ -722,10 +728,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G30"/>
+  <dimension ref="A1:G31"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+    <sheetView tabSelected="1" topLeftCell="A14" workbookViewId="0">
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -879,177 +885,185 @@
     </row>
     <row r="15" spans="1:3" ht="45" x14ac:dyDescent="0.25">
       <c r="A15" s="8" t="s">
+        <v>61</v>
+      </c>
+      <c r="C15" s="9" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+      <c r="A16" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="B15" s="1" t="s">
+      <c r="B16" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="C15" s="9" t="s">
+      <c r="C16" s="9" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="16" spans="1:3" ht="210" x14ac:dyDescent="0.25">
-      <c r="A16" s="8" t="s">
+    <row r="17" spans="1:7" ht="210" x14ac:dyDescent="0.25">
+      <c r="A17" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="B16" s="1">
+      <c r="B17" s="1">
         <v>1</v>
       </c>
-      <c r="C16" s="9" t="s">
+      <c r="C17" s="9" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="17" spans="1:7" ht="45" x14ac:dyDescent="0.25">
-      <c r="A17" s="8" t="s">
+    <row r="18" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="A18" s="8" t="s">
         <v>40</v>
       </c>
-      <c r="B17" s="1">
+      <c r="B18" s="1">
         <v>100</v>
       </c>
-      <c r="C17" s="9" t="s">
+      <c r="C18" s="9" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="18" spans="1:7" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="10" t="s">
+    <row r="19" spans="1:7" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A19" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="B18" s="11" t="s">
+      <c r="B19" s="11" t="s">
         <v>58</v>
       </c>
-      <c r="C18" s="12" t="s">
+      <c r="C19" s="12" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="19" spans="1:7" ht="21.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="22" t="s">
+    <row r="20" spans="1:7" ht="21.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A20" s="22" t="s">
         <v>42</v>
       </c>
-      <c r="B19" s="22"/>
-      <c r="C19" s="22"/>
-    </row>
-    <row r="20" spans="1:7" ht="45" x14ac:dyDescent="0.25">
-      <c r="A20" s="5" t="s">
+      <c r="B20" s="22"/>
+      <c r="C20" s="22"/>
+    </row>
+    <row r="21" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="A21" s="5" t="s">
         <v>43</v>
       </c>
-      <c r="B20" s="6">
+      <c r="B21" s="6">
         <v>1</v>
       </c>
-      <c r="C20" s="7" t="s">
+      <c r="C21" s="7" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="21" spans="1:7" ht="45" x14ac:dyDescent="0.25">
-      <c r="A21" s="8" t="s">
+    <row r="22" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="A22" s="8" t="s">
         <v>44</v>
       </c>
-      <c r="B21" s="1">
+      <c r="B22" s="1">
         <v>1</v>
       </c>
-      <c r="C21" s="9" t="s">
+      <c r="C22" s="9" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="22" spans="1:7" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="10" t="s">
+    <row r="23" spans="1:7" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A23" s="10" t="s">
         <v>46</v>
       </c>
-      <c r="B22" s="11">
+      <c r="B23" s="11">
         <v>1</v>
       </c>
-      <c r="C22" s="12" t="s">
+      <c r="C23" s="12" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="23" spans="1:7" ht="21.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="20" t="s">
+    <row r="24" spans="1:7" ht="21.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A24" s="20" t="s">
         <v>36</v>
       </c>
-      <c r="B23" s="20"/>
-      <c r="C23" s="20"/>
-    </row>
-    <row r="24" spans="1:7" ht="45" x14ac:dyDescent="0.25">
-      <c r="A24" s="5" t="s">
+      <c r="B24" s="20"/>
+      <c r="C24" s="20"/>
+    </row>
+    <row r="25" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="A25" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="B24" s="6" t="s">
+      <c r="B25" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="C24" s="7" t="s">
+      <c r="C25" s="7" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="25" spans="1:7" ht="90" x14ac:dyDescent="0.25">
-      <c r="A25" s="8" t="s">
+    <row r="26" spans="1:7" ht="90" x14ac:dyDescent="0.25">
+      <c r="A26" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="B25" s="1">
+      <c r="B26" s="1">
         <v>30</v>
       </c>
-      <c r="C25" s="16" t="s">
+      <c r="C26" s="16" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="26" spans="1:7" ht="45" x14ac:dyDescent="0.25">
-      <c r="A26" s="8" t="s">
+    <row r="27" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="A27" s="8" t="s">
         <v>50</v>
       </c>
-      <c r="B26" s="1">
+      <c r="B27" s="1">
         <v>10</v>
       </c>
-      <c r="C26" s="16" t="s">
+      <c r="C27" s="16" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="27" spans="1:7" ht="75.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="10" t="s">
+    <row r="28" spans="1:7" ht="75.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A28" s="10" t="s">
         <v>52</v>
       </c>
-      <c r="B27" s="11">
+      <c r="B28" s="11">
         <v>0.01</v>
       </c>
-      <c r="C27" s="17" t="s">
+      <c r="C28" s="17" t="s">
         <v>53</v>
       </c>
-      <c r="G27" s="18"/>
-    </row>
-    <row r="28" spans="1:7" ht="21.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A28" s="21" t="s">
+      <c r="G28" s="18"/>
+    </row>
+    <row r="29" spans="1:7" ht="21.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A29" s="21" t="s">
         <v>37</v>
       </c>
-      <c r="B28" s="21"/>
-      <c r="C28" s="21"/>
-    </row>
-    <row r="29" spans="1:7" ht="75" x14ac:dyDescent="0.25">
-      <c r="A29" s="5" t="s">
+      <c r="B29" s="21"/>
+      <c r="C29" s="21"/>
+    </row>
+    <row r="30" spans="1:7" ht="75" x14ac:dyDescent="0.25">
+      <c r="A30" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="B29" s="6">
+      <c r="B30" s="6">
         <v>15</v>
       </c>
-      <c r="C29" s="7" t="s">
+      <c r="C30" s="7" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="30" spans="1:7" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A30" s="10" t="s">
+    <row r="31" spans="1:7" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A31" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="B30" s="11">
+      <c r="B31" s="11">
         <v>0.1</v>
       </c>
-      <c r="C30" s="12" t="s">
+      <c r="C31" s="12" t="s">
         <v>26</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="6">
-    <mergeCell ref="A23:C23"/>
-    <mergeCell ref="A28:C28"/>
+    <mergeCell ref="A24:C24"/>
+    <mergeCell ref="A29:C29"/>
     <mergeCell ref="A11:C11"/>
     <mergeCell ref="A9:C9"/>
     <mergeCell ref="A6:C6"/>
-    <mergeCell ref="A19:C19"/>
+    <mergeCell ref="A20:C20"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
painfully implemented testing and boxplot engines
</commit_message>
<xml_diff>
--- a/settings.xlsx
+++ b/settings.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://charitede-my.sharepoint.com/personal/lev_petrov_charite_de/Documents/DOCTORATE/Cytomata/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="188" documentId="11_F25DC773A252ABDACC104856411A5CB85ADE58E9" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{7BF836D1-576C-41D0-91D6-725C8E14BA47}"/>
+  <xr:revisionPtr revIDLastSave="189" documentId="11_F25DC773A252ABDACC104856411A5CB85ADE58E9" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{DA840CA6-4FFA-46F3-B7E4-CAB32C6C4A93}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="1155" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -81,9 +81,6 @@
     <t>meta</t>
   </si>
   <si>
-    <t>sev_age_timepoint, inf_age_timepoint</t>
-  </si>
-  <si>
     <t>CD4_T</t>
   </si>
   <si>
@@ -214,6 +211,9 @@
   </si>
   <si>
     <t>Control order of groups. Input group names separated by comma. For multiple grouping columns - separate by semicolon.</t>
+  </si>
+  <si>
+    <t>sev_age_timepoint, inf_age_timepoint, inf_age</t>
   </si>
 </sst>
 </file>
@@ -730,8 +730,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G31"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A14" workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -760,7 +760,7 @@
         <v>16</v>
       </c>
       <c r="C2" s="7" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
@@ -768,10 +768,10 @@
         <v>4</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C3" s="9" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
@@ -782,36 +782,36 @@
         <v>17</v>
       </c>
       <c r="C4" s="9" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="5" spans="1:3" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="10" t="s">
+        <v>53</v>
+      </c>
+      <c r="B5" s="19" t="s">
         <v>54</v>
       </c>
-      <c r="B5" s="19" t="s">
-        <v>55</v>
-      </c>
       <c r="C5" s="12" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="6" spans="1:3" ht="21.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="21" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B6" s="21"/>
       <c r="C6" s="21"/>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" s="5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B7" s="6">
         <v>1</v>
       </c>
       <c r="C7" s="7" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="8" spans="1:3" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -819,46 +819,46 @@
         <v>7</v>
       </c>
       <c r="B8" s="11" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C8" s="12" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="9" spans="1:3" ht="21.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="21" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B9" s="21"/>
       <c r="C9" s="21"/>
     </row>
     <row r="10" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="13" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B10" s="14">
         <v>1</v>
       </c>
       <c r="C10" s="15" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="11" spans="1:3" ht="21.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="21" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B11" s="21"/>
       <c r="C11" s="21"/>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" s="5" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B12" s="6">
         <v>1</v>
       </c>
       <c r="C12" s="7" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="13" spans="1:3" ht="45" x14ac:dyDescent="0.25">
@@ -869,7 +869,7 @@
         <v>1</v>
       </c>
       <c r="C13" s="9" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="14" spans="1:3" ht="30" x14ac:dyDescent="0.25">
@@ -877,18 +877,18 @@
         <v>8</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>18</v>
+        <v>62</v>
       </c>
       <c r="C14" s="9" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="15" spans="1:3" ht="45" x14ac:dyDescent="0.25">
       <c r="A15" s="8" t="s">
+        <v>60</v>
+      </c>
+      <c r="C15" s="9" t="s">
         <v>61</v>
-      </c>
-      <c r="C15" s="9" t="s">
-        <v>62</v>
       </c>
     </row>
     <row r="16" spans="1:3" ht="45" x14ac:dyDescent="0.25">
@@ -896,10 +896,10 @@
         <v>9</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C16" s="9" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="17" spans="1:7" ht="210" x14ac:dyDescent="0.25">
@@ -910,18 +910,18 @@
         <v>1</v>
       </c>
       <c r="C17" s="9" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="18" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A18" s="8" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B18" s="1">
         <v>100</v>
       </c>
       <c r="C18" s="9" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="19" spans="1:7" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -929,55 +929,55 @@
         <v>11</v>
       </c>
       <c r="B19" s="11" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C19" s="12" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="20" spans="1:7" ht="21.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A20" s="22" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B20" s="22"/>
       <c r="C20" s="22"/>
     </row>
     <row r="21" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A21" s="5" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B21" s="6">
         <v>1</v>
       </c>
       <c r="C21" s="7" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="22" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A22" s="8" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B22" s="1">
         <v>1</v>
       </c>
       <c r="C22" s="9" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="23" spans="1:7" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A23" s="10" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B23" s="11">
         <v>1</v>
       </c>
       <c r="C23" s="12" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="24" spans="1:7" ht="21.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A24" s="20" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B24" s="20"/>
       <c r="C24" s="20"/>
@@ -987,10 +987,10 @@
         <v>12</v>
       </c>
       <c r="B25" s="6" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C25" s="7" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="26" spans="1:7" ht="90" x14ac:dyDescent="0.25">
@@ -1001,35 +1001,35 @@
         <v>30</v>
       </c>
       <c r="C26" s="16" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="27" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A27" s="8" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B27" s="1">
         <v>10</v>
       </c>
       <c r="C27" s="16" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="28" spans="1:7" ht="75.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A28" s="10" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B28" s="11">
         <v>0.01</v>
       </c>
       <c r="C28" s="17" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="G28" s="18"/>
     </row>
     <row r="29" spans="1:7" ht="21.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A29" s="21" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B29" s="21"/>
       <c r="C29" s="21"/>
@@ -1042,7 +1042,7 @@
         <v>15</v>
       </c>
       <c r="C30" s="7" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="31" spans="1:7" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1053,7 +1053,7 @@
         <v>0.1</v>
       </c>
       <c r="C31" s="12" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added group order control, manual palette control. fixed testing heatmap for edge cases (two groups only)
</commit_message>
<xml_diff>
--- a/settings.xlsx
+++ b/settings.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27726"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27830"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://charitede-my.sharepoint.com/personal/lev_petrov_charite_de/Documents/DOCTORATE/Cytomata/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="189" documentId="11_F25DC773A252ABDACC104856411A5CB85ADE58E9" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{DA840CA6-4FFA-46F3-B7E4-CAB32C6C4A93}"/>
+  <xr:revisionPtr revIDLastSave="202" documentId="11_F25DC773A252ABDACC104856411A5CB85ADE58E9" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{EAD6DAA3-7B3E-4EED-90CC-B3AAA5EB1E6B}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="1155" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="64">
   <si>
     <t>setting</t>
   </si>
@@ -210,10 +210,13 @@
     <t>grouping_orders</t>
   </si>
   <si>
-    <t>Control order of groups. Input group names separated by comma. For multiple grouping columns - separate by semicolon.</t>
-  </si>
-  <si>
     <t>sev_age_timepoint, inf_age_timepoint, inf_age</t>
+  </si>
+  <si>
+    <t>Control order of groups. Input group names separated by comma. For multiple grouping columns - separate by semicolon. If you do not want to input order for any specific grouping column - write NA.</t>
+  </si>
+  <si>
+    <t>NA; control child, control, infected child, infected adult, infected child d14, infected adult d14, infected child d180, infected adult d180; control child, control adult, infected child, infected adult</t>
   </si>
 </sst>
 </file>
@@ -380,7 +383,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -397,9 +400,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -412,18 +412,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -447,6 +441,12 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -730,14 +730,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G31"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="23.140625" style="1" customWidth="1"/>
-    <col min="2" max="2" width="28.42578125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="71.28515625" style="2" customWidth="1"/>
     <col min="3" max="3" width="59" style="2" customWidth="1"/>
   </cols>
   <sheetData>
@@ -745,7 +745,7 @@
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="B1" s="4" t="s">
         <v>1</v>
       </c>
       <c r="C1" s="4" t="s">
@@ -756,303 +756,306 @@
       <c r="A2" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="6" t="s">
+      <c r="B2" s="20" t="s">
         <v>16</v>
       </c>
-      <c r="C2" s="7" t="s">
+      <c r="C2" s="6" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" s="8" t="s">
+      <c r="A3" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="B3" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="C3" s="9" t="s">
+      <c r="C3" s="8" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" s="8" t="s">
+      <c r="A4" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="B4" s="1" t="s">
+      <c r="B4" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="C4" s="9" t="s">
+      <c r="C4" s="8" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="5" spans="1:3" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="10" t="s">
+      <c r="A5" s="9" t="s">
         <v>53</v>
       </c>
-      <c r="B5" s="19" t="s">
+      <c r="B5" s="16" t="s">
         <v>54</v>
       </c>
-      <c r="C5" s="12" t="s">
+      <c r="C5" s="10" t="s">
         <v>56</v>
       </c>
     </row>
     <row r="6" spans="1:3" ht="21.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="21" t="s">
+      <c r="A6" s="18" t="s">
         <v>29</v>
       </c>
-      <c r="B6" s="21"/>
-      <c r="C6" s="21"/>
+      <c r="B6" s="18"/>
+      <c r="C6" s="18"/>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="B7" s="6">
+      <c r="B7" s="20">
         <v>1</v>
       </c>
-      <c r="C7" s="7" t="s">
+      <c r="C7" s="6" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="8" spans="1:3" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="10" t="s">
+      <c r="A8" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="B8" s="11" t="s">
+      <c r="B8" s="16" t="s">
         <v>59</v>
       </c>
-      <c r="C8" s="12" t="s">
+      <c r="C8" s="10" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="9" spans="1:3" ht="21.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="21" t="s">
+      <c r="A9" s="18" t="s">
         <v>32</v>
       </c>
-      <c r="B9" s="21"/>
-      <c r="C9" s="21"/>
+      <c r="B9" s="18"/>
+      <c r="C9" s="18"/>
     </row>
     <row r="10" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="13" t="s">
+      <c r="A10" s="11" t="s">
         <v>33</v>
       </c>
-      <c r="B10" s="14">
+      <c r="B10" s="21">
         <v>1</v>
       </c>
-      <c r="C10" s="15" t="s">
+      <c r="C10" s="12" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="11" spans="1:3" ht="21.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="21" t="s">
+      <c r="A11" s="18" t="s">
         <v>34</v>
       </c>
-      <c r="B11" s="21"/>
-      <c r="C11" s="21"/>
+      <c r="B11" s="18"/>
+      <c r="C11" s="18"/>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" s="5" t="s">
         <v>37</v>
       </c>
-      <c r="B12" s="6">
+      <c r="B12" s="20">
         <v>1</v>
       </c>
-      <c r="C12" s="7" t="s">
+      <c r="C12" s="6" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="13" spans="1:3" ht="45" x14ac:dyDescent="0.25">
-      <c r="A13" s="8" t="s">
+      <c r="A13" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="B13" s="1">
+      <c r="B13" s="2">
         <v>1</v>
       </c>
-      <c r="C13" s="9" t="s">
+      <c r="C13" s="8" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="14" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A14" s="8" t="s">
+      <c r="A14" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="B14" s="1" t="s">
+      <c r="B14" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="C14" s="8" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" ht="60" x14ac:dyDescent="0.25">
+      <c r="A15" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="C15" s="8" t="s">
         <v>62</v>
       </c>
-      <c r="C14" s="9" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" ht="45" x14ac:dyDescent="0.25">
-      <c r="A15" s="8" t="s">
-        <v>60</v>
-      </c>
-      <c r="C15" s="9" t="s">
-        <v>61</v>
-      </c>
     </row>
     <row r="16" spans="1:3" ht="45" x14ac:dyDescent="0.25">
-      <c r="A16" s="8" t="s">
+      <c r="A16" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="B16" s="1" t="s">
+      <c r="B16" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="C16" s="9" t="s">
+      <c r="C16" s="8" t="s">
         <v>55</v>
       </c>
     </row>
     <row r="17" spans="1:7" ht="210" x14ac:dyDescent="0.25">
-      <c r="A17" s="8" t="s">
+      <c r="A17" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="B17" s="1">
+      <c r="B17" s="2">
         <v>1</v>
       </c>
-      <c r="C17" s="9" t="s">
+      <c r="C17" s="8" t="s">
         <v>38</v>
       </c>
     </row>
     <row r="18" spans="1:7" ht="45" x14ac:dyDescent="0.25">
-      <c r="A18" s="8" t="s">
+      <c r="A18" s="7" t="s">
         <v>39</v>
       </c>
-      <c r="B18" s="1">
+      <c r="B18" s="2">
         <v>100</v>
       </c>
-      <c r="C18" s="9" t="s">
+      <c r="C18" s="8" t="s">
         <v>40</v>
       </c>
     </row>
     <row r="19" spans="1:7" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="10" t="s">
+      <c r="A19" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="B19" s="11" t="s">
+      <c r="B19" s="16" t="s">
         <v>57</v>
       </c>
-      <c r="C19" s="12" t="s">
+      <c r="C19" s="10" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="20" spans="1:7" ht="21.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="22" t="s">
+      <c r="A20" s="19" t="s">
         <v>41</v>
       </c>
-      <c r="B20" s="22"/>
-      <c r="C20" s="22"/>
+      <c r="B20" s="19"/>
+      <c r="C20" s="19"/>
     </row>
     <row r="21" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A21" s="5" t="s">
         <v>42</v>
       </c>
-      <c r="B21" s="6">
+      <c r="B21" s="20">
         <v>1</v>
       </c>
-      <c r="C21" s="7" t="s">
+      <c r="C21" s="6" t="s">
         <v>44</v>
       </c>
     </row>
     <row r="22" spans="1:7" ht="45" x14ac:dyDescent="0.25">
-      <c r="A22" s="8" t="s">
+      <c r="A22" s="7" t="s">
         <v>43</v>
       </c>
-      <c r="B22" s="1">
+      <c r="B22" s="2">
         <v>1</v>
       </c>
-      <c r="C22" s="9" t="s">
+      <c r="C22" s="8" t="s">
         <v>47</v>
       </c>
     </row>
     <row r="23" spans="1:7" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="10" t="s">
+      <c r="A23" s="9" t="s">
         <v>45</v>
       </c>
-      <c r="B23" s="11">
+      <c r="B23" s="16">
         <v>1</v>
       </c>
-      <c r="C23" s="12" t="s">
+      <c r="C23" s="10" t="s">
         <v>46</v>
       </c>
     </row>
     <row r="24" spans="1:7" ht="21.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A24" s="20" t="s">
+      <c r="A24" s="17" t="s">
         <v>35</v>
       </c>
-      <c r="B24" s="20"/>
-      <c r="C24" s="20"/>
+      <c r="B24" s="17"/>
+      <c r="C24" s="17"/>
     </row>
     <row r="25" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A25" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="B25" s="6" t="s">
+      <c r="B25" s="20" t="s">
         <v>19</v>
       </c>
-      <c r="C25" s="7" t="s">
+      <c r="C25" s="6" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="26" spans="1:7" ht="90" x14ac:dyDescent="0.25">
-      <c r="A26" s="8" t="s">
+      <c r="A26" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="B26" s="1">
+      <c r="B26" s="2">
         <v>30</v>
       </c>
-      <c r="C26" s="16" t="s">
+      <c r="C26" s="13" t="s">
         <v>48</v>
       </c>
     </row>
     <row r="27" spans="1:7" ht="45" x14ac:dyDescent="0.25">
-      <c r="A27" s="8" t="s">
+      <c r="A27" s="7" t="s">
         <v>49</v>
       </c>
-      <c r="B27" s="1">
+      <c r="B27" s="2">
         <v>10</v>
       </c>
-      <c r="C27" s="16" t="s">
+      <c r="C27" s="13" t="s">
         <v>50</v>
       </c>
     </row>
     <row r="28" spans="1:7" ht="75.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A28" s="10" t="s">
+      <c r="A28" s="9" t="s">
         <v>51</v>
       </c>
-      <c r="B28" s="11">
+      <c r="B28" s="16">
         <v>0.01</v>
       </c>
-      <c r="C28" s="17" t="s">
+      <c r="C28" s="14" t="s">
         <v>52</v>
       </c>
-      <c r="G28" s="18"/>
+      <c r="G28" s="15"/>
     </row>
     <row r="29" spans="1:7" ht="21.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A29" s="21" t="s">
+      <c r="A29" s="18" t="s">
         <v>36</v>
       </c>
-      <c r="B29" s="21"/>
-      <c r="C29" s="21"/>
+      <c r="B29" s="18"/>
+      <c r="C29" s="18"/>
     </row>
     <row r="30" spans="1:7" ht="75" x14ac:dyDescent="0.25">
       <c r="A30" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="B30" s="6">
+      <c r="B30" s="20">
         <v>15</v>
       </c>
-      <c r="C30" s="7" t="s">
+      <c r="C30" s="6" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="31" spans="1:7" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A31" s="10" t="s">
+      <c r="A31" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="B31" s="11">
+      <c r="B31" s="16">
         <v>0.1</v>
       </c>
-      <c r="C31" s="12" t="s">
+      <c r="C31" s="10" t="s">
         <v>25</v>
       </c>
     </row>

</xml_diff>

<commit_message>
fixed a bunch of big bugs in analysis functions
</commit_message>
<xml_diff>
--- a/settings.xlsx
+++ b/settings.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://charitede-my.sharepoint.com/personal/lev_petrov_charite_de/Documents/DOCTORATE/Cytomata/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="216" documentId="11_F25DC773A252ABDACC104856411A5CB85ADE58E9" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C5162800-0828-4A59-913D-F261E20C2BFC}"/>
+  <xr:revisionPtr revIDLastSave="218" documentId="11_F25DC773A252ABDACC104856411A5CB85ADE58E9" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{691D1615-6DB9-4F2F-87C4-B53F50C676D5}"/>
   <bookViews>
-    <workbookView xWindow="-57720" yWindow="-11715" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-56010" yWindow="-10395" windowWidth="24495" windowHeight="11235" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -174,49 +174,49 @@
     <t>HC-050</t>
   </si>
   <si>
-    <t>antigen,anca_status</t>
-  </si>
-  <si>
-    <t>1, 30</t>
-  </si>
-  <si>
     <t>anca_panel_1</t>
   </si>
   <si>
-    <t>Patterns present in the names of pre-processing channels that will be used to remove them. Input separated by comma and whitespace (', '). This can be adjusted in the panel.csv file afterwards.</t>
-  </si>
-  <si>
-    <t>What ID your reference replicates have. Accepts multiple IDs, separated by comma and whitespace (', ').</t>
-  </si>
-  <si>
-    <t>Columns in meta-table that contain group stratification. Accepts multiple names, separated by comma and whitespace (', ').</t>
-  </si>
-  <si>
-    <t>Pre-gated subsets of events that you want to analyze. These should be the exact names of folders in fcs/4_subsets/. Separated by comma and whitespace (', ').</t>
-  </si>
-  <si>
-    <t>Whether to down- or upsample events PER SAMPLE using a given factor. You might want to downsample if studying e.g. granulocytes (on whole blood) to reduce computational burden and oversample if interested in finding rare populations. Downsampling could also be used to reduce the dominance of the oversized samples, while oversampling could be used to enhance the representation of the undersized ones. The cutoff for downsampling is the average sample size across all samples (samples are not reduced in size beyond that threshold). The cutoff for oversampling is the average sample size across all samples (samples are not increased in size beyond that threshold). Accepts multiple values separated by comma and whitespace (', ') if different needed for each data_subset. Order is given by data_subset order.</t>
-  </si>
-  <si>
-    <t>0 (off) or 1 (on). Second value can be entered for number of features to keep, separated by comma and whitespace (', '). Is done by default for top 20 features if subset_feature_selection.xlsx is not provided.</t>
-  </si>
-  <si>
-    <t>If fs, number of clusters after hierarchical and before automatic merging. If fs_manual, final number of clusters after hierarchical merging. If pg, number of nearest neighbors parameter. Accepts multiple values, separated by comma and whitespace (', '), if different values are needed for each data_subset. Order is given by data_subset vector.</t>
-  </si>
-  <si>
-    <t>UMAPs n_neighbors. Low value leads to better resolution of local structure, high - to better capture of global structure. Default value is 15. Accepts multiple values, separated by comma and whitespace (', ') of different values are needed for each data_subset. Order is given by data_subset vector.</t>
-  </si>
-  <si>
-    <t>UMAPs min_dist. Lower values lead to clumpier embeddings, higher make them more spread-out. Accepts multiple values, separated by comma and whitespace (', ') of different values are needed for each data_subset. Order is given by data_subset vector.</t>
+    <t>Patterns present in the names of pre-processing channels that will be used to remove them. Input separated by comma and whitespace (", "). This can be adjusted in the panel.csv file afterwards.</t>
+  </si>
+  <si>
+    <t>What ID your reference replicates have. Accepts multiple IDs, separated by comma and whitespace (", ").</t>
+  </si>
+  <si>
+    <t>Columns in meta-table that contain group stratification. Accepts multiple names, separated by comma and whitespace (", ").</t>
+  </si>
+  <si>
+    <t>Pre-gated subsets of events that you want to analyze. These should be the exact names of folders in fcs/4_subsets/. Separated by comma and whitespace (", ").</t>
+  </si>
+  <si>
+    <t>Whether to down- or upsample events PER SAMPLE using a given factor. You might want to downsample if studying e.g. granulocytes (on whole blood) to reduce computational burden and oversample if interested in finding rare populations. Downsampling could also be used to reduce the dominance of the oversized samples, while oversampling could be used to enhance the representation of the undersized ones. The cutoff for downsampling is the average sample size across all samples (samples are not reduced in size beyond that threshold). The cutoff for oversampling is the average sample size across all samples (samples are not increased in size beyond that threshold). Accepts multiple values separated by comma and whitespace (", ") if different needed for each data_subset. Order is given by data_subset order.</t>
+  </si>
+  <si>
+    <t>0 (off) or 1 (on). Second value can be entered for number of features to keep, separated by comma and whitespace (", "). Is done by default for top 20 features if subset_feature_selection.xlsx is not provided.</t>
+  </si>
+  <si>
+    <t>If fs, number of clusters after hierarchical and before automatic merging. If fs_manual, final number of clusters after hierarchical merging. If pg, number of nearest neighbors parameter. Accepts multiple values, separated by comma and whitespace (", "), if different values are needed for each data_subset. Order is given by data_subset vector.</t>
+  </si>
+  <si>
+    <t>UMAPs n_neighbors. Low value leads to better resolution of local structure, high - to better capture of global structure. Default value is 15. Accepts multiple values, separated by comma and whitespace (", ") of different values are needed for each data_subset. Order is given by data_subset vector.</t>
+  </si>
+  <si>
+    <t>UMAPs min_dist. Lower values lead to clumpier embeddings, higher make them more spread-out. Accepts multiple values, separated by comma and whitespace (", ") of different values are needed for each data_subset. Order is given by data_subset vector.</t>
+  </si>
+  <si>
+    <t>Control order of groups. Input group names separated by comma and whitespace (", "). For multiple grouping columns - separate by semicolon and whitespace (", "). If you do not want to input order for any specific grouping column - write NA.</t>
+  </si>
+  <si>
+    <t>HC, MPO, PR3; HC, ANCA</t>
   </si>
   <si>
     <t>CD4_T, B</t>
   </si>
   <si>
-    <t>HC, MPO, PR3; HC, ANCA</t>
-  </si>
-  <si>
-    <t>Control order of groups. Input group names separated by comma and whitespace (', '). For multiple grouping columns - separate by semicolon and whitespace ('; '). If you do not want to input order for any specific grouping column - write NA.</t>
+    <t>antigen, anca_status</t>
+  </si>
+  <si>
+    <t>0, 30</t>
   </si>
 </sst>
 </file>
@@ -730,8 +730,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G31"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="F15" sqref="F15"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -768,7 +768,7 @@
         <v>4</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="C3" s="8" t="s">
         <v>21</v>
@@ -793,7 +793,7 @@
         <v>46</v>
       </c>
       <c r="C5" s="10" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
     </row>
     <row r="6" spans="1:3" ht="21.6" thickBot="1" x14ac:dyDescent="0.35">
@@ -822,7 +822,7 @@
         <v>48</v>
       </c>
       <c r="C8" s="10" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
     </row>
     <row r="9" spans="1:3" ht="21.6" thickBot="1" x14ac:dyDescent="0.35">
@@ -877,10 +877,10 @@
         <v>8</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>49</v>
+        <v>62</v>
       </c>
       <c r="C14" s="8" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
     </row>
     <row r="15" spans="1:3" ht="57.6" x14ac:dyDescent="0.3">
@@ -888,10 +888,10 @@
         <v>47</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="C15" s="8" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
     </row>
     <row r="16" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
@@ -902,7 +902,7 @@
         <v>61</v>
       </c>
       <c r="C16" s="8" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
     </row>
     <row r="17" spans="1:7" ht="172.8" x14ac:dyDescent="0.3">
@@ -913,7 +913,7 @@
         <v>1</v>
       </c>
       <c r="C17" s="8" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
     </row>
     <row r="18" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
@@ -932,10 +932,10 @@
         <v>11</v>
       </c>
       <c r="B19" s="16" t="s">
-        <v>50</v>
+        <v>63</v>
       </c>
       <c r="C19" s="10" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
     </row>
     <row r="20" spans="1:7" ht="21.6" thickBot="1" x14ac:dyDescent="0.35">
@@ -996,7 +996,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="26" spans="1:7" ht="72" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:7" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A26" s="7" t="s">
         <v>13</v>
       </c>
@@ -1004,7 +1004,7 @@
         <v>30</v>
       </c>
       <c r="C26" s="13" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
     </row>
     <row r="27" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
@@ -1045,7 +1045,7 @@
         <v>15</v>
       </c>
       <c r="C30" s="6" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
     </row>
     <row r="31" spans="1:7" ht="58.2" thickBot="1" x14ac:dyDescent="0.35">
@@ -1056,7 +1056,7 @@
         <v>0.1</v>
       </c>
       <c r="C31" s="10" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
chore: Refactor analysis functions and update plot settings
</commit_message>
<xml_diff>
--- a/settings.xlsx
+++ b/settings.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://charitede-my.sharepoint.com/personal/lev_petrov_charite_de/Documents/DOCTORATE/Cytomata_data/anca_panel_3/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://charitede-my.sharepoint.com/personal/lev_petrov_charite_de/Documents/DOCTORATE/Cytomata/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="219" documentId="11_F25DC773A252ABDACC104856411A5CB85ADE58E9" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{ADD61B67-0CB2-434B-9601-AD824ED1A05B}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="14_{C8F7A666-B505-455E-A52A-3CA40E73FDF1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-56010" yWindow="-10395" windowWidth="24495" windowHeight="11235" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -174,49 +174,49 @@
     <t>HC-050</t>
   </si>
   <si>
-    <t>anca_panel_3</t>
-  </si>
-  <si>
-    <t>Monos_and_DCs</t>
+    <t>anca_panel_2</t>
+  </si>
+  <si>
+    <t>Granulos</t>
+  </si>
+  <si>
+    <t>Patterns present in the names of pre-processing channels that will be used to remove them. Input separated by comma and whitespace (', '). This can be adjusted in the panel.csv file afterwards.</t>
+  </si>
+  <si>
+    <t>What ID your reference replicates have. Accepts multiple IDs, separated by comma and whitespace (', ').</t>
+  </si>
+  <si>
+    <t>Columns in meta-table that contain group stratification. Accepts multiple names, separated by comma and whitespace (', ').</t>
+  </si>
+  <si>
+    <t>Pre-gated subsets of events that you want to analyze. These should be the exact names of folders in fcs/4_subsets/. Separated by comma and whitespace (', ').</t>
+  </si>
+  <si>
+    <t>Whether to down- or upsample events PER SAMPLE using a given factor. You might want to downsample if studying e.g. granulocytes (on whole blood) to reduce computational burden and oversample if interested in finding rare populations. Downsampling could also be used to reduce the dominance of the oversized samples, while oversampling could be used to enhance the representation of the undersized ones. The cutoff for downsampling is the average sample size across all samples (samples are not reduced in size beyond that threshold). The cutoff for oversampling is the average sample size across all samples (samples are not increased in size beyond that threshold). Accepts multiple values separated by comma and whitespace (', ') if different needed for each data_subset. Order is given by data_subset order.</t>
+  </si>
+  <si>
+    <t>0 (off) or 1 (on). Second value can be entered for number of features to keep, separated by comma and whitespace (', '). Is done by default for top 20 features if subset_feature_selection.xlsx is not provided.</t>
+  </si>
+  <si>
+    <t>If fs, number of clusters after hierarchical and before automatic merging. If fs_manual, final number of clusters after hierarchical merging. If pg, number of nearest neighbors parameter. Accepts multiple values, separated by comma and whitespace (', '), if different values are needed for each data_subset. Order is given by data_subset vector.</t>
+  </si>
+  <si>
+    <t>UMAPs n_neighbors. Low value leads to better resolution of local structure, high - to better capture of global structure. Default value is 15. Accepts multiple values, separated by comma and whitespace (', ') of different values are needed for each data_subset. Order is given by data_subset vector.</t>
+  </si>
+  <si>
+    <t>UMAPs min_dist. Lower values lead to clumpier embeddings, higher make them more spread-out. Accepts multiple values, separated by comma and whitespace (', ') of different values are needed for each data_subset. Order is given by data_subset vector.</t>
+  </si>
+  <si>
+    <t>Control order of groups. Input group names separated by comma and whitespace (', '). For multiple grouping columns - separate by semicolon and whitespace (', '). If you do not want to input order for any specific grouping column - write NA.</t>
+  </si>
+  <si>
+    <t>antigen, anca_status</t>
+  </si>
+  <si>
+    <t>HC, MPO, PR3; HC, ANCA</t>
   </si>
   <si>
     <t>0, 30</t>
-  </si>
-  <si>
-    <t>HC, MPO, PR3; HC, ANCA</t>
-  </si>
-  <si>
-    <t>antigen, anca_status</t>
-  </si>
-  <si>
-    <t>Patterns present in the names of pre-processing channels that will be used to remove them. Input separated by comma and whitespace (', '). This can be adjusted in the panel.csv file afterwards.</t>
-  </si>
-  <si>
-    <t>What ID your reference replicates have. Accepts multiple IDs, separated by comma and whitespace (', ').</t>
-  </si>
-  <si>
-    <t>Columns in meta-table that contain group stratification. Accepts multiple names, separated by comma and whitespace (', ').</t>
-  </si>
-  <si>
-    <t>Pre-gated subsets of events that you want to analyze. These should be the exact names of folders in fcs/4_subsets/. Separated by comma and whitespace (', ').</t>
-  </si>
-  <si>
-    <t>Whether to down- or upsample events PER SAMPLE using a given factor. You might want to downsample if studying e.g. granulocytes (on whole blood) to reduce computational burden and oversample if interested in finding rare populations. Downsampling could also be used to reduce the dominance of the oversized samples, while oversampling could be used to enhance the representation of the undersized ones. The cutoff for downsampling is the average sample size across all samples (samples are not reduced in size beyond that threshold). The cutoff for oversampling is the average sample size across all samples (samples are not increased in size beyond that threshold). Accepts multiple values separated by comma and whitespace (', ') if different needed for each data_subset. Order is given by data_subset order.</t>
-  </si>
-  <si>
-    <t>0 (off) or 1 (on). Second value can be entered for number of features to keep, separated by comma and whitespace (', '). Is done by default for top 20 features if subset_feature_selection.xlsx is not provided.</t>
-  </si>
-  <si>
-    <t>If fs, number of clusters after hierarchical and before automatic merging. If fs_manual, final number of clusters after hierarchical merging. If pg, number of nearest neighbors parameter. Accepts multiple values, separated by comma and whitespace (', '), if different values are needed for each data_subset. Order is given by data_subset vector.</t>
-  </si>
-  <si>
-    <t>UMAPs n_neighbors. Low value leads to better resolution of local structure, high - to better capture of global structure. Default value is 15. Accepts multiple values, separated by comma and whitespace (', ') of different values are needed for each data_subset. Order is given by data_subset vector.</t>
-  </si>
-  <si>
-    <t>UMAPs min_dist. Lower values lead to clumpier embeddings, higher make them more spread-out. Accepts multiple values, separated by comma and whitespace (', ') of different values are needed for each data_subset. Order is given by data_subset vector.</t>
-  </si>
-  <si>
-    <t>Control order of groups. Input group names separated by comma and whitespace (', '). For multiple grouping columns - separate by semicolon and whitespace (', '). If you do not want to input order for any specific grouping column - write NA.</t>
   </si>
 </sst>
 </file>
@@ -730,8 +730,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G31"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -793,7 +793,7 @@
         <v>46</v>
       </c>
       <c r="C5" s="10" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
     </row>
     <row r="6" spans="1:3" ht="21.6" thickBot="1" x14ac:dyDescent="0.35">
@@ -822,7 +822,7 @@
         <v>48</v>
       </c>
       <c r="C8" s="10" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
     </row>
     <row r="9" spans="1:3" ht="21.6" thickBot="1" x14ac:dyDescent="0.35">
@@ -866,7 +866,7 @@
         <v>5</v>
       </c>
       <c r="B13" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C13" s="8" t="s">
         <v>19</v>
@@ -877,21 +877,21 @@
         <v>8</v>
       </c>
       <c r="B14" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="C14" s="8" t="s">
         <v>53</v>
       </c>
-      <c r="C14" s="8" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
+    </row>
+    <row r="15" spans="1:3" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A15" s="7" t="s">
         <v>47</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>52</v>
+        <v>62</v>
       </c>
       <c r="C15" s="8" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
     </row>
     <row r="16" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
@@ -902,7 +902,7 @@
         <v>50</v>
       </c>
       <c r="C16" s="8" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
     </row>
     <row r="17" spans="1:7" ht="172.8" x14ac:dyDescent="0.3">
@@ -913,7 +913,7 @@
         <v>1</v>
       </c>
       <c r="C17" s="8" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
     </row>
     <row r="18" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
@@ -932,10 +932,10 @@
         <v>11</v>
       </c>
       <c r="B19" s="16" t="s">
-        <v>51</v>
+        <v>63</v>
       </c>
       <c r="C19" s="10" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
     </row>
     <row r="20" spans="1:7" ht="21.6" thickBot="1" x14ac:dyDescent="0.35">
@@ -996,7 +996,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="26" spans="1:7" ht="72" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:7" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A26" s="7" t="s">
         <v>13</v>
       </c>
@@ -1004,7 +1004,7 @@
         <v>30</v>
       </c>
       <c r="C26" s="13" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
     </row>
     <row r="27" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
@@ -1045,7 +1045,7 @@
         <v>15</v>
       </c>
       <c r="C30" s="6" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
     </row>
     <row r="31" spans="1:7" ht="58.2" thickBot="1" x14ac:dyDescent="0.35">
@@ -1056,7 +1056,7 @@
         <v>0.1</v>
       </c>
       <c r="C31" s="10" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fix, chore: fix heatmap ordering to be dynamic or based on exprs heatmap dendrogram_order; small refactoring of general functions;
</commit_message>
<xml_diff>
--- a/settings.xlsx
+++ b/settings.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://charitede-my.sharepoint.com/personal/lev_petrov_charite_de/Documents/DOCTORATE/Cytomata/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://charitede-my.sharepoint.com/personal/lev_petrov_charite_de/Documents/DOCTORATE/Cytomata_data/anca_panel_3/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="14_{C8F7A666-B505-455E-A52A-3CA40E73FDF1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="8" documentId="14_{5CD1A498-E873-4B30-8872-751E1B7C508A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F956C573-4AE3-48D9-B9DA-1DFC6995C026}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-57720" yWindow="-11715" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -174,10 +174,16 @@
     <t>HC-050</t>
   </si>
   <si>
-    <t>anca_panel_2</t>
-  </si>
-  <si>
-    <t>Granulos</t>
+    <t>anca_panel_3</t>
+  </si>
+  <si>
+    <t>0, 30</t>
+  </si>
+  <si>
+    <t>HC, MPO, PR3; HC, ANCA</t>
+  </si>
+  <si>
+    <t>antigen, anca_status</t>
   </si>
   <si>
     <t>Patterns present in the names of pre-processing channels that will be used to remove them. Input separated by comma and whitespace (', '). This can be adjusted in the panel.csv file afterwards.</t>
@@ -210,13 +216,7 @@
     <t>Control order of groups. Input group names separated by comma and whitespace (', '). For multiple grouping columns - separate by semicolon and whitespace (', '). If you do not want to input order for any specific grouping column - write NA.</t>
   </si>
   <si>
-    <t>antigen, anca_status</t>
-  </si>
-  <si>
-    <t>HC, MPO, PR3; HC, ANCA</t>
-  </si>
-  <si>
-    <t>0, 30</t>
+    <t>B</t>
   </si>
 </sst>
 </file>
@@ -730,8 +730,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G31"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -793,7 +793,7 @@
         <v>46</v>
       </c>
       <c r="C5" s="10" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
     </row>
     <row r="6" spans="1:3" ht="21.6" thickBot="1" x14ac:dyDescent="0.35">
@@ -822,7 +822,7 @@
         <v>48</v>
       </c>
       <c r="C8" s="10" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
     </row>
     <row r="9" spans="1:3" ht="21.6" thickBot="1" x14ac:dyDescent="0.35">
@@ -866,7 +866,7 @@
         <v>5</v>
       </c>
       <c r="B13" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C13" s="8" t="s">
         <v>19</v>
@@ -877,10 +877,10 @@
         <v>8</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>61</v>
+        <v>52</v>
       </c>
       <c r="C14" s="8" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
     </row>
     <row r="15" spans="1:3" ht="57.6" x14ac:dyDescent="0.3">
@@ -888,10 +888,10 @@
         <v>47</v>
       </c>
       <c r="B15" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="C15" s="8" t="s">
         <v>62</v>
-      </c>
-      <c r="C15" s="8" t="s">
-        <v>60</v>
       </c>
     </row>
     <row r="16" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
@@ -899,13 +899,13 @@
         <v>9</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>50</v>
+        <v>63</v>
       </c>
       <c r="C16" s="8" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="17" spans="1:7" ht="172.8" x14ac:dyDescent="0.3">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" ht="187.2" x14ac:dyDescent="0.3">
       <c r="A17" s="7" t="s">
         <v>10</v>
       </c>
@@ -913,7 +913,7 @@
         <v>1</v>
       </c>
       <c r="C17" s="8" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
     </row>
     <row r="18" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
@@ -932,10 +932,10 @@
         <v>11</v>
       </c>
       <c r="B19" s="16" t="s">
-        <v>63</v>
+        <v>50</v>
       </c>
       <c r="C19" s="10" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
     </row>
     <row r="20" spans="1:7" ht="21.6" thickBot="1" x14ac:dyDescent="0.35">
@@ -972,7 +972,7 @@
         <v>38</v>
       </c>
       <c r="B23" s="16">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C23" s="10" t="s">
         <v>39</v>
@@ -1004,7 +1004,7 @@
         <v>30</v>
       </c>
       <c r="C26" s="13" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
     </row>
     <row r="27" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
@@ -1023,7 +1023,7 @@
         <v>43</v>
       </c>
       <c r="B28" s="16">
-        <v>0.01</v>
+        <v>1.2E-2</v>
       </c>
       <c r="C28" s="14" t="s">
         <v>44</v>
@@ -1045,7 +1045,7 @@
         <v>15</v>
       </c>
       <c r="C30" s="6" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
     </row>
     <row r="31" spans="1:7" ht="58.2" thickBot="1" x14ac:dyDescent="0.35">
@@ -1056,7 +1056,7 @@
         <v>0.1</v>
       </c>
       <c r="C31" s="10" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add missing packages to the environment_setup
</commit_message>
<xml_diff>
--- a/settings.xlsx
+++ b/settings.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://charitede-my.sharepoint.com/personal/lev_petrov_charite_de/Documents/DOCTORATE/Cytomata_data/anca_panel_3/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="8" documentId="14_{5CD1A498-E873-4B30-8872-751E1B7C508A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F956C573-4AE3-48D9-B9DA-1DFC6995C026}"/>
+  <xr:revisionPtr revIDLastSave="9" documentId="14_{5CD1A498-E873-4B30-8872-751E1B7C508A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{AFB83027-AE09-42D8-B0F4-B1B6031C3A0F}"/>
   <bookViews>
-    <workbookView xWindow="-57720" yWindow="-11715" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -216,7 +216,7 @@
     <t>Control order of groups. Input group names separated by comma and whitespace (', '). For multiple grouping columns - separate by semicolon and whitespace (', '). If you do not want to input order for any specific grouping column - write NA.</t>
   </si>
   <si>
-    <t>B</t>
+    <t>B, CD4_T, Monos_and_DCs</t>
   </si>
 </sst>
 </file>
@@ -731,7 +731,7 @@
   <dimension ref="A1:G31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+      <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
chore: small fix for counts and cluster_proportions tables from calculate_abundances not saving
</commit_message>
<xml_diff>
--- a/settings.xlsx
+++ b/settings.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://charitede-my.sharepoint.com/personal/lev_petrov_charite_de/Documents/DOCTORATE/Cytomata_data/anca_panel_3/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="9" documentId="14_{5CD1A498-E873-4B30-8872-751E1B7C508A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{AFB83027-AE09-42D8-B0F4-B1B6031C3A0F}"/>
+  <xr:revisionPtr revIDLastSave="10" documentId="14_{5CD1A498-E873-4B30-8872-751E1B7C508A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{56C2BC43-201A-4B29-805C-CBABCC979360}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -730,8 +730,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G31"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
+    <sheetView tabSelected="1" topLeftCell="A18" workbookViewId="0">
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -866,7 +866,7 @@
         <v>5</v>
       </c>
       <c r="B13" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C13" s="8" t="s">
         <v>19</v>

</xml_diff>

<commit_message>
feature: add norm_mode setting to select between percentile-based and harmony normalization, add harmony normalization implementation
</commit_message>
<xml_diff>
--- a/settings.xlsx
+++ b/settings.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://charitede-my.sharepoint.com/personal/lev_petrov_charite_de/Documents/DOCTORATE/Cytomata_data/anca_panel_3/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="10" documentId="14_{5CD1A498-E873-4B30-8872-751E1B7C508A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{56C2BC43-201A-4B29-805C-CBABCC979360}"/>
+  <xr:revisionPtr revIDLastSave="13" documentId="14_{5CD1A498-E873-4B30-8872-751E1B7C508A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C3E73056-10E9-4FDC-912A-D4D8F07CE771}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -216,7 +216,7 @@
     <t>Control order of groups. Input group names separated by comma and whitespace (', '). For multiple grouping columns - separate by semicolon and whitespace (', '). If you do not want to input order for any specific grouping column - write NA.</t>
   </si>
   <si>
-    <t>B, CD4_T, Monos_and_DCs</t>
+    <t>Monos_and_DCs</t>
   </si>
 </sst>
 </file>
@@ -730,8 +730,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G31"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A18" workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
+      <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -866,7 +866,7 @@
         <v>5</v>
       </c>
       <c r="B13" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C13" s="8" t="s">
         <v>19</v>

</xml_diff>

<commit_message>
fix: dir structure checks to handle populated directories properly
</commit_message>
<xml_diff>
--- a/settings.xlsx
+++ b/settings.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://charitede-my.sharepoint.com/personal/lev_petrov_charite_de/Documents/DOCTORATE/Cytomata/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="20" documentId="14_{5CD1A498-E873-4B30-8872-751E1B7C508A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C6769CEC-C450-447A-98EF-9D2152D2CC99}"/>
+  <xr:revisionPtr revIDLastSave="7" documentId="13_ncr:1_{9C262F40-B724-47DA-807B-CA0883A1DDFB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B25339B4-8BFC-4D9D-98A2-55C45FA88A0D}"/>
   <bookViews>
     <workbookView xWindow="-57720" yWindow="-11715" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="64">
   <si>
     <t>setting</t>
   </si>
@@ -174,58 +174,49 @@
     <t>HC-050</t>
   </si>
   <si>
+    <t>anca_panel_1</t>
+  </si>
+  <si>
+    <t>Patterns present in the names of pre-processing channels that will be used to remove them. Input separated by comma and whitespace (", "). This can be adjusted in the panel.csv file afterwards.</t>
+  </si>
+  <si>
+    <t>What ID your reference replicates have. Accepts multiple IDs, separated by comma and whitespace (", ").</t>
+  </si>
+  <si>
+    <t>Columns in meta-table that contain group stratification. Accepts multiple names, separated by comma and whitespace (", ").</t>
+  </si>
+  <si>
+    <t>Pre-gated subsets of events that you want to analyze. These should be the exact names of folders in fcs/4_subsets/. Separated by comma and whitespace (", ").</t>
+  </si>
+  <si>
+    <t>Whether to down- or upsample events PER SAMPLE using a given factor. You might want to downsample if studying e.g. granulocytes (on whole blood) to reduce computational burden and oversample if interested in finding rare populations. Downsampling could also be used to reduce the dominance of the oversized samples, while oversampling could be used to enhance the representation of the undersized ones. The cutoff for downsampling is the average sample size across all samples (samples are not reduced in size beyond that threshold). The cutoff for oversampling is the average sample size across all samples (samples are not increased in size beyond that threshold). Accepts multiple values separated by comma and whitespace (", ") if different needed for each data_subset. Order is given by data_subset order.</t>
+  </si>
+  <si>
+    <t>0 (off) or 1 (on). Second value can be entered for number of features to keep, separated by comma and whitespace (", "). Is done by default for top 20 features if subset_feature_selection.xlsx is not provided.</t>
+  </si>
+  <si>
+    <t>If fs, number of clusters after hierarchical and before automatic merging. If fs_manual, final number of clusters after hierarchical merging. If pg, number of nearest neighbors parameter. Accepts multiple values, separated by comma and whitespace (", "), if different values are needed for each data_subset. Order is given by data_subset vector.</t>
+  </si>
+  <si>
+    <t>UMAPs n_neighbors. Low value leads to better resolution of local structure, high - to better capture of global structure. Default value is 15. Accepts multiple values, separated by comma and whitespace (", ") of different values are needed for each data_subset. Order is given by data_subset vector.</t>
+  </si>
+  <si>
+    <t>UMAPs min_dist. Lower values lead to clumpier embeddings, higher make them more spread-out. Accepts multiple values, separated by comma and whitespace (", ") of different values are needed for each data_subset. Order is given by data_subset vector.</t>
+  </si>
+  <si>
+    <t>Control order of groups. Input group names separated by comma and whitespace (", "). For multiple grouping columns - separate by semicolon and whitespace (", "). If you do not want to input order for any specific grouping column - write NA.</t>
+  </si>
+  <si>
+    <t>HC, MPO, PR3; HC, ANCA</t>
+  </si>
+  <si>
+    <t>antigen, anca_status</t>
+  </si>
+  <si>
     <t>0, 30</t>
   </si>
   <si>
-    <t>HC, MPO, PR3; HC, ANCA</t>
-  </si>
-  <si>
-    <t>antigen, anca_status</t>
-  </si>
-  <si>
-    <t>Patterns present in the names of pre-processing channels that will be used to remove them. Input separated by comma and whitespace (', '). This can be adjusted in the panel.csv file afterwards.</t>
-  </si>
-  <si>
-    <t>What ID your reference replicates have. Accepts multiple IDs, separated by comma and whitespace (', ').</t>
-  </si>
-  <si>
-    <t>Columns in meta-table that contain group stratification. Accepts multiple names, separated by comma and whitespace (', ').</t>
-  </si>
-  <si>
-    <t>Pre-gated subsets of events that you want to analyze. These should be the exact names of folders in fcs/4_subsets/. Separated by comma and whitespace (', ').</t>
-  </si>
-  <si>
-    <t>Whether to down- or upsample events PER SAMPLE using a given factor. You might want to downsample if studying e.g. granulocytes (on whole blood) to reduce computational burden and oversample if interested in finding rare populations. Downsampling could also be used to reduce the dominance of the oversized samples, while oversampling could be used to enhance the representation of the undersized ones. The cutoff for downsampling is the average sample size across all samples (samples are not reduced in size beyond that threshold). The cutoff for oversampling is the average sample size across all samples (samples are not increased in size beyond that threshold). Accepts multiple values separated by comma and whitespace (', ') if different needed for each data_subset. Order is given by data_subset order.</t>
-  </si>
-  <si>
-    <t>0 (off) or 1 (on). Second value can be entered for number of features to keep, separated by comma and whitespace (', '). Is done by default for top 20 features if subset_feature_selection.xlsx is not provided.</t>
-  </si>
-  <si>
-    <t>If fs, number of clusters after hierarchical and before automatic merging. If fs_manual, final number of clusters after hierarchical merging. If pg, number of nearest neighbors parameter. Accepts multiple values, separated by comma and whitespace (', '), if different values are needed for each data_subset. Order is given by data_subset vector.</t>
-  </si>
-  <si>
-    <t>UMAPs n_neighbors. Low value leads to better resolution of local structure, high - to better capture of global structure. Default value is 15. Accepts multiple values, separated by comma and whitespace (', ') of different values are needed for each data_subset. Order is given by data_subset vector.</t>
-  </si>
-  <si>
-    <t>UMAPs min_dist. Lower values lead to clumpier embeddings, higher make them more spread-out. Accepts multiple values, separated by comma and whitespace (', ') of different values are needed for each data_subset. Order is given by data_subset vector.</t>
-  </si>
-  <si>
-    <t>Control order of groups. Input group names separated by comma and whitespace (', '). For multiple grouping columns - separate by semicolon and whitespace (', '). If you do not want to input order for any specific grouping column - write NA.</t>
-  </si>
-  <si>
-    <t>Monos_and_DCs</t>
-  </si>
-  <si>
-    <t>anca_panel_3_temp</t>
-  </si>
-  <si>
-    <t>norm_mode</t>
-  </si>
-  <si>
-    <t>harmony</t>
-  </si>
-  <si>
-    <t>percentile or harmony</t>
+    <t>CD8_T</t>
   </si>
 </sst>
 </file>
@@ -392,7 +383,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -456,9 +447,6 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -740,10 +728,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G32"/>
+  <dimension ref="A1:G31"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="B28" sqref="B28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -780,7 +768,7 @@
         <v>4</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>63</v>
+        <v>49</v>
       </c>
       <c r="C3" s="8" t="s">
         <v>21</v>
@@ -805,7 +793,7 @@
         <v>46</v>
       </c>
       <c r="C5" s="10" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
     </row>
     <row r="6" spans="1:3" ht="21.6" thickBot="1" x14ac:dyDescent="0.35">
@@ -820,276 +808,265 @@
         <v>25</v>
       </c>
       <c r="B7" s="17">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C7" s="6" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A8" s="7" t="s">
-        <v>64</v>
-      </c>
-      <c r="B8" s="22" t="s">
-        <v>65</v>
-      </c>
-      <c r="C8" s="8" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A9" s="9" t="s">
+    <row r="8" spans="1:3" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A8" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="B9" s="16" t="s">
+      <c r="B8" s="16" t="s">
         <v>48</v>
       </c>
-      <c r="C9" s="10" t="s">
+      <c r="C8" s="10" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" ht="21.6" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A9" s="20" t="s">
+        <v>26</v>
+      </c>
+      <c r="B9" s="20"/>
+      <c r="C9" s="20"/>
+    </row>
+    <row r="10" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A10" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="B10" s="18">
+        <v>0</v>
+      </c>
+      <c r="C10" s="12" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" ht="21.6" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A11" s="20" t="s">
+        <v>28</v>
+      </c>
+      <c r="B11" s="20"/>
+      <c r="C11" s="20"/>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A12" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="B12" s="17">
+        <v>1</v>
+      </c>
+      <c r="C12" s="6" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A13" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="B13" s="2">
+        <v>0</v>
+      </c>
+      <c r="C13" s="8" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A14" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="C14" s="8" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A15" s="7" t="s">
+        <v>47</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="C15" s="8" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A16" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="C16" s="8" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="10" spans="1:3" ht="21.6" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A10" s="20" t="s">
-        <v>26</v>
-      </c>
-      <c r="B10" s="20"/>
-      <c r="C10" s="20"/>
-    </row>
-    <row r="11" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A11" s="11" t="s">
-        <v>27</v>
-      </c>
-      <c r="B11" s="18">
+    <row r="17" spans="1:7" ht="187.2" x14ac:dyDescent="0.3">
+      <c r="A17" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="B17" s="2">
+        <v>1</v>
+      </c>
+      <c r="C17" s="8" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A18" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="B18" s="2">
+        <v>100</v>
+      </c>
+      <c r="C18" s="8" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" ht="43.8" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A19" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="B19" s="16" t="s">
+        <v>62</v>
+      </c>
+      <c r="C19" s="10" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" ht="21.6" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A20" s="21" t="s">
+        <v>34</v>
+      </c>
+      <c r="B20" s="21"/>
+      <c r="C20" s="21"/>
+    </row>
+    <row r="21" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A21" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="B21" s="17">
+        <v>1</v>
+      </c>
+      <c r="C21" s="6" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A22" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="B22" s="2">
+        <v>1</v>
+      </c>
+      <c r="C22" s="8" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A23" s="9" t="s">
+        <v>38</v>
+      </c>
+      <c r="B23" s="16">
         <v>0</v>
       </c>
-      <c r="C11" s="12" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" ht="21.6" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A12" s="20" t="s">
-        <v>28</v>
-      </c>
-      <c r="B12" s="20"/>
-      <c r="C12" s="20"/>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A13" s="5" t="s">
-        <v>31</v>
-      </c>
-      <c r="B13" s="17">
-        <v>0</v>
-      </c>
-      <c r="C13" s="6" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A14" s="7" t="s">
-        <v>5</v>
-      </c>
-      <c r="B14" s="2">
-        <v>1</v>
-      </c>
-      <c r="C14" s="8" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A15" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="B15" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="C15" s="8" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A16" s="7" t="s">
-        <v>47</v>
-      </c>
-      <c r="B16" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="C16" s="8" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="17" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A17" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="B17" s="2" t="s">
-        <v>62</v>
-      </c>
-      <c r="C17" s="8" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="18" spans="1:7" ht="187.2" x14ac:dyDescent="0.3">
-      <c r="A18" s="7" t="s">
+      <c r="C23" s="10" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" ht="21.6" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A24" s="19" t="s">
+        <v>29</v>
+      </c>
+      <c r="B24" s="19"/>
+      <c r="C24" s="19"/>
+    </row>
+    <row r="25" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A25" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="B25" s="17" t="s">
+        <v>18</v>
+      </c>
+      <c r="C25" s="6" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" ht="86.4" x14ac:dyDescent="0.3">
+      <c r="A26" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="B26" s="2">
+        <v>30</v>
+      </c>
+      <c r="C26" s="13" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A27" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="B27" s="2">
         <v>10</v>
       </c>
-      <c r="B18" s="2">
-        <v>1</v>
-      </c>
-      <c r="C18" s="8" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="19" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A19" s="7" t="s">
-        <v>32</v>
-      </c>
-      <c r="B19" s="2">
-        <v>100</v>
-      </c>
-      <c r="C19" s="8" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="20" spans="1:7" ht="43.8" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A20" s="9" t="s">
-        <v>11</v>
-      </c>
-      <c r="B20" s="16" t="s">
-        <v>49</v>
-      </c>
-      <c r="C20" s="10" t="s">
+      <c r="C27" s="13" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" ht="58.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A28" s="9" t="s">
+        <v>43</v>
+      </c>
+      <c r="B28" s="16">
+        <v>0.02</v>
+      </c>
+      <c r="C28" s="14" t="s">
+        <v>44</v>
+      </c>
+      <c r="G28" s="15"/>
+    </row>
+    <row r="29" spans="1:7" ht="21.6" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A29" s="20" t="s">
+        <v>30</v>
+      </c>
+      <c r="B29" s="20"/>
+      <c r="C29" s="20"/>
+    </row>
+    <row r="30" spans="1:7" ht="72" x14ac:dyDescent="0.3">
+      <c r="A30" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="B30" s="17">
+        <v>15</v>
+      </c>
+      <c r="C30" s="6" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="21" spans="1:7" ht="21.6" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A21" s="21" t="s">
-        <v>34</v>
-      </c>
-      <c r="B21" s="21"/>
-      <c r="C21" s="21"/>
-    </row>
-    <row r="22" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A22" s="5" t="s">
-        <v>35</v>
-      </c>
-      <c r="B22" s="17">
-        <v>1</v>
-      </c>
-      <c r="C22" s="6" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="23" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A23" s="7" t="s">
-        <v>36</v>
-      </c>
-      <c r="B23" s="2">
-        <v>1</v>
-      </c>
-      <c r="C23" s="8" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="24" spans="1:7" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A24" s="9" t="s">
-        <v>38</v>
-      </c>
-      <c r="B24" s="16">
-        <v>0</v>
-      </c>
-      <c r="C24" s="10" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="25" spans="1:7" ht="21.6" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A25" s="19" t="s">
-        <v>29</v>
-      </c>
-      <c r="B25" s="19"/>
-      <c r="C25" s="19"/>
-    </row>
-    <row r="26" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A26" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="B26" s="17" t="s">
-        <v>18</v>
-      </c>
-      <c r="C26" s="6" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="27" spans="1:7" ht="86.4" x14ac:dyDescent="0.3">
-      <c r="A27" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="B27" s="2">
-        <v>30</v>
-      </c>
-      <c r="C27" s="13" t="s">
+    <row r="31" spans="1:7" ht="58.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A31" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="B31" s="16">
+        <v>0.1</v>
+      </c>
+      <c r="C31" s="10" t="s">
         <v>58</v>
-      </c>
-    </row>
-    <row r="28" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A28" s="7" t="s">
-        <v>41</v>
-      </c>
-      <c r="B28" s="2">
-        <v>10</v>
-      </c>
-      <c r="C28" s="13" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="29" spans="1:7" ht="58.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A29" s="9" t="s">
-        <v>43</v>
-      </c>
-      <c r="B29" s="16">
-        <v>1.2E-2</v>
-      </c>
-      <c r="C29" s="14" t="s">
-        <v>44</v>
-      </c>
-      <c r="G29" s="15"/>
-    </row>
-    <row r="30" spans="1:7" ht="21.6" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A30" s="20" t="s">
-        <v>30</v>
-      </c>
-      <c r="B30" s="20"/>
-      <c r="C30" s="20"/>
-    </row>
-    <row r="31" spans="1:7" ht="72" x14ac:dyDescent="0.3">
-      <c r="A31" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="B31" s="17">
-        <v>15</v>
-      </c>
-      <c r="C31" s="6" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="32" spans="1:7" ht="58.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A32" s="9" t="s">
-        <v>15</v>
-      </c>
-      <c r="B32" s="16">
-        <v>0.1</v>
-      </c>
-      <c r="C32" s="10" t="s">
-        <v>60</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="6">
-    <mergeCell ref="A25:C25"/>
-    <mergeCell ref="A30:C30"/>
-    <mergeCell ref="A12:C12"/>
-    <mergeCell ref="A10:C10"/>
+    <mergeCell ref="A24:C24"/>
+    <mergeCell ref="A29:C29"/>
+    <mergeCell ref="A11:C11"/>
+    <mergeCell ref="A9:C9"/>
     <mergeCell ref="A6:C6"/>
-    <mergeCell ref="A21:C21"/>
+    <mergeCell ref="A20:C20"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
fix: dplyr::summarize conflict fix in normalization_exploration_adjustment.R (line 90)
</commit_message>
<xml_diff>
--- a/settings.xlsx
+++ b/settings.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24332"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28526"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://charitede-my.sharepoint.com/personal/lev_petrov_charite_de/Documents/DOCTORATE/Cytomata/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://charitede-my.sharepoint.com/personal/lucas_arendholz_bih-charite_de/Documents/In_Silico/Cytomata/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="7" documentId="13_ncr:1_{9C262F40-B724-47DA-807B-CA0883A1DDFB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B25339B4-8BFC-4D9D-98A2-55C45FA88A0D}"/>
+  <xr:revisionPtr revIDLastSave="25" documentId="14_{5CD1A498-E873-4B30-8872-751E1B7C508A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A57A9D6D-1861-4F80-B619-4A17FA531146}"/>
   <bookViews>
-    <workbookView xWindow="-57720" yWindow="-11715" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="11424" yWindow="0" windowWidth="11712" windowHeight="12336" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="67">
   <si>
     <t>setting</t>
   </si>
@@ -75,9 +75,6 @@
     <t>umap_min_dist</t>
   </si>
   <si>
-    <t>~/DOCTORATE/Cytomata_data/</t>
-  </si>
-  <si>
     <t>meta</t>
   </si>
   <si>
@@ -171,40 +168,7 @@
     <t>grouping_orders</t>
   </si>
   <si>
-    <t>HC-050</t>
-  </si>
-  <si>
-    <t>anca_panel_1</t>
-  </si>
-  <si>
-    <t>Patterns present in the names of pre-processing channels that will be used to remove them. Input separated by comma and whitespace (", "). This can be adjusted in the panel.csv file afterwards.</t>
-  </si>
-  <si>
-    <t>What ID your reference replicates have. Accepts multiple IDs, separated by comma and whitespace (", ").</t>
-  </si>
-  <si>
-    <t>Columns in meta-table that contain group stratification. Accepts multiple names, separated by comma and whitespace (", ").</t>
-  </si>
-  <si>
-    <t>Pre-gated subsets of events that you want to analyze. These should be the exact names of folders in fcs/4_subsets/. Separated by comma and whitespace (", ").</t>
-  </si>
-  <si>
-    <t>Whether to down- or upsample events PER SAMPLE using a given factor. You might want to downsample if studying e.g. granulocytes (on whole blood) to reduce computational burden and oversample if interested in finding rare populations. Downsampling could also be used to reduce the dominance of the oversized samples, while oversampling could be used to enhance the representation of the undersized ones. The cutoff for downsampling is the average sample size across all samples (samples are not reduced in size beyond that threshold). The cutoff for oversampling is the average sample size across all samples (samples are not increased in size beyond that threshold). Accepts multiple values separated by comma and whitespace (", ") if different needed for each data_subset. Order is given by data_subset order.</t>
-  </si>
-  <si>
-    <t>0 (off) or 1 (on). Second value can be entered for number of features to keep, separated by comma and whitespace (", "). Is done by default for top 20 features if subset_feature_selection.xlsx is not provided.</t>
-  </si>
-  <si>
-    <t>If fs, number of clusters after hierarchical and before automatic merging. If fs_manual, final number of clusters after hierarchical merging. If pg, number of nearest neighbors parameter. Accepts multiple values, separated by comma and whitespace (", "), if different values are needed for each data_subset. Order is given by data_subset vector.</t>
-  </si>
-  <si>
-    <t>UMAPs n_neighbors. Low value leads to better resolution of local structure, high - to better capture of global structure. Default value is 15. Accepts multiple values, separated by comma and whitespace (", ") of different values are needed for each data_subset. Order is given by data_subset vector.</t>
-  </si>
-  <si>
-    <t>UMAPs min_dist. Lower values lead to clumpier embeddings, higher make them more spread-out. Accepts multiple values, separated by comma and whitespace (", ") of different values are needed for each data_subset. Order is given by data_subset vector.</t>
-  </si>
-  <si>
-    <t>Control order of groups. Input group names separated by comma and whitespace (", "). For multiple grouping columns - separate by semicolon and whitespace (", "). If you do not want to input order for any specific grouping column - write NA.</t>
+    <t>0, 30</t>
   </si>
   <si>
     <t>HC, MPO, PR3; HC, ANCA</t>
@@ -213,10 +177,55 @@
     <t>antigen, anca_status</t>
   </si>
   <si>
-    <t>0, 30</t>
-  </si>
-  <si>
-    <t>CD8_T</t>
+    <t>Patterns present in the names of pre-processing channels that will be used to remove them. Input separated by comma and whitespace (', '). This can be adjusted in the panel.csv file afterwards.</t>
+  </si>
+  <si>
+    <t>What ID your reference replicates have. Accepts multiple IDs, separated by comma and whitespace (', ').</t>
+  </si>
+  <si>
+    <t>Columns in meta-table that contain group stratification. Accepts multiple names, separated by comma and whitespace (', ').</t>
+  </si>
+  <si>
+    <t>Pre-gated subsets of events that you want to analyze. These should be the exact names of folders in fcs/4_subsets/. Separated by comma and whitespace (', ').</t>
+  </si>
+  <si>
+    <t>Whether to down- or upsample events PER SAMPLE using a given factor. You might want to downsample if studying e.g. granulocytes (on whole blood) to reduce computational burden and oversample if interested in finding rare populations. Downsampling could also be used to reduce the dominance of the oversized samples, while oversampling could be used to enhance the representation of the undersized ones. The cutoff for downsampling is the average sample size across all samples (samples are not reduced in size beyond that threshold). The cutoff for oversampling is the average sample size across all samples (samples are not increased in size beyond that threshold). Accepts multiple values separated by comma and whitespace (', ') if different needed for each data_subset. Order is given by data_subset order.</t>
+  </si>
+  <si>
+    <t>0 (off) or 1 (on). Second value can be entered for number of features to keep, separated by comma and whitespace (', '). Is done by default for top 20 features if subset_feature_selection.xlsx is not provided.</t>
+  </si>
+  <si>
+    <t>If fs, number of clusters after hierarchical and before automatic merging. If fs_manual, final number of clusters after hierarchical merging. If pg, number of nearest neighbors parameter. Accepts multiple values, separated by comma and whitespace (', '), if different values are needed for each data_subset. Order is given by data_subset vector.</t>
+  </si>
+  <si>
+    <t>UMAPs n_neighbors. Low value leads to better resolution of local structure, high - to better capture of global structure. Default value is 15. Accepts multiple values, separated by comma and whitespace (', ') of different values are needed for each data_subset. Order is given by data_subset vector.</t>
+  </si>
+  <si>
+    <t>UMAPs min_dist. Lower values lead to clumpier embeddings, higher make them more spread-out. Accepts multiple values, separated by comma and whitespace (', ') of different values are needed for each data_subset. Order is given by data_subset vector.</t>
+  </si>
+  <si>
+    <t>Control order of groups. Input group names separated by comma and whitespace (', '). For multiple grouping columns - separate by semicolon and whitespace (', '). If you do not want to input order for any specific grouping column - write NA.</t>
+  </si>
+  <si>
+    <t>B, CD4_T, Monos_and_DCs</t>
+  </si>
+  <si>
+    <t>NKSG_IACS_panel_3</t>
+  </si>
+  <si>
+    <t>C:/Users/lucas/OneDrive - Charité - Universitätsmedizin Berlin/#NKSG - Post-Covid19/CyTOF_analysis/Cytomata-master/Cytomata_data/</t>
+  </si>
+  <si>
+    <t>HC-04</t>
+  </si>
+  <si>
+    <t>norm_mode</t>
+  </si>
+  <si>
+    <t>percentile</t>
+  </si>
+  <si>
+    <t>percentile or harmony. harmony looks weird, will fix.</t>
   </si>
 </sst>
 </file>
@@ -383,7 +392,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -447,6 +456,9 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -728,10 +740,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G31"/>
+  <dimension ref="A1:G32"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="B28" sqref="B28"/>
+    <sheetView tabSelected="1" topLeftCell="B2" workbookViewId="0">
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -752,15 +764,15 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A2" s="5" t="s">
         <v>3</v>
       </c>
       <c r="B2" s="17" t="s">
-        <v>16</v>
+        <v>62</v>
       </c>
       <c r="C2" s="6" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
@@ -768,10 +780,10 @@
         <v>4</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>49</v>
+        <v>61</v>
       </c>
       <c r="C3" s="8" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
@@ -779,18 +791,18 @@
         <v>6</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C4" s="8" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="5" spans="1:3" ht="43.8" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A5" s="9" t="s">
+        <v>44</v>
+      </c>
+      <c r="B5" s="16" t="s">
         <v>45</v>
-      </c>
-      <c r="B5" s="16" t="s">
-        <v>46</v>
       </c>
       <c r="C5" s="10" t="s">
         <v>50</v>
@@ -798,275 +810,286 @@
     </row>
     <row r="6" spans="1:3" ht="21.6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A6" s="20" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B6" s="20"/>
       <c r="C6" s="20"/>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="B7" s="17">
+        <v>1</v>
+      </c>
+      <c r="C7" s="6" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A8" s="7" t="s">
+        <v>64</v>
+      </c>
+      <c r="B8" s="22" t="s">
+        <v>65</v>
+      </c>
+      <c r="C8" s="8" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A9" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="B9" s="16" t="s">
+        <v>63</v>
+      </c>
+      <c r="C9" s="10" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" ht="21.6" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A10" s="20" t="s">
         <v>25</v>
       </c>
-      <c r="B7" s="17">
+      <c r="B10" s="20"/>
+      <c r="C10" s="20"/>
+    </row>
+    <row r="11" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A11" s="11" t="s">
+        <v>26</v>
+      </c>
+      <c r="B11" s="18">
+        <v>1</v>
+      </c>
+      <c r="C11" s="12" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" ht="21.6" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A12" s="20" t="s">
+        <v>27</v>
+      </c>
+      <c r="B12" s="20"/>
+      <c r="C12" s="20"/>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A13" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="B13" s="17">
+        <v>1</v>
+      </c>
+      <c r="C13" s="6" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A14" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="B14" s="2">
+        <v>1</v>
+      </c>
+      <c r="C14" s="8" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A15" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="C15" s="8" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A16" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="C16" s="8" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A17" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="B17" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="C17" s="8" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" ht="187.2" x14ac:dyDescent="0.3">
+      <c r="A18" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="B18" s="2">
+        <v>1</v>
+      </c>
+      <c r="C18" s="8" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A19" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="B19" s="2">
+        <v>100</v>
+      </c>
+      <c r="C19" s="8" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" ht="43.8" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A20" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="B20" s="16" t="s">
+        <v>47</v>
+      </c>
+      <c r="C20" s="10" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" ht="21.6" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A21" s="21" t="s">
+        <v>33</v>
+      </c>
+      <c r="B21" s="21"/>
+      <c r="C21" s="21"/>
+    </row>
+    <row r="22" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A22" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="B22" s="17">
+        <v>1</v>
+      </c>
+      <c r="C22" s="6" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A23" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="B23" s="2">
+        <v>1</v>
+      </c>
+      <c r="C23" s="8" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A24" s="9" t="s">
+        <v>37</v>
+      </c>
+      <c r="B24" s="16">
         <v>0</v>
       </c>
-      <c r="C7" s="6" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A8" s="9" t="s">
-        <v>7</v>
-      </c>
-      <c r="B8" s="16" t="s">
-        <v>48</v>
-      </c>
-      <c r="C8" s="10" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" ht="21.6" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A9" s="20" t="s">
-        <v>26</v>
-      </c>
-      <c r="B9" s="20"/>
-      <c r="C9" s="20"/>
-    </row>
-    <row r="10" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A10" s="11" t="s">
-        <v>27</v>
-      </c>
-      <c r="B10" s="18">
-        <v>0</v>
-      </c>
-      <c r="C10" s="12" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" ht="21.6" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A11" s="20" t="s">
+      <c r="C24" s="10" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" ht="21.6" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A25" s="19" t="s">
         <v>28</v>
       </c>
-      <c r="B11" s="20"/>
-      <c r="C11" s="20"/>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A12" s="5" t="s">
-        <v>31</v>
-      </c>
-      <c r="B12" s="17">
-        <v>1</v>
-      </c>
-      <c r="C12" s="6" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A13" s="7" t="s">
-        <v>5</v>
-      </c>
-      <c r="B13" s="2">
-        <v>0</v>
-      </c>
-      <c r="C13" s="8" t="s">
+      <c r="B25" s="19"/>
+      <c r="C25" s="19"/>
+    </row>
+    <row r="26" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A26" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="B26" s="17" t="s">
+        <v>17</v>
+      </c>
+      <c r="C26" s="6" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="14" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A14" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="B14" s="2" t="s">
-        <v>61</v>
-      </c>
-      <c r="C14" s="8" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A15" s="7" t="s">
-        <v>47</v>
-      </c>
-      <c r="B15" s="2" t="s">
-        <v>60</v>
-      </c>
-      <c r="C15" s="8" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A16" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="B16" s="2" t="s">
-        <v>63</v>
-      </c>
-      <c r="C16" s="8" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="17" spans="1:7" ht="187.2" x14ac:dyDescent="0.3">
-      <c r="A17" s="7" t="s">
+    <row r="27" spans="1:7" ht="86.4" x14ac:dyDescent="0.3">
+      <c r="A27" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="B27" s="2">
+        <v>30</v>
+      </c>
+      <c r="C27" s="13" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A28" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="B28" s="2">
         <v>10</v>
       </c>
-      <c r="B17" s="2">
-        <v>1</v>
-      </c>
-      <c r="C17" s="8" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="18" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A18" s="7" t="s">
-        <v>32</v>
-      </c>
-      <c r="B18" s="2">
-        <v>100</v>
-      </c>
-      <c r="C18" s="8" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="19" spans="1:7" ht="43.8" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A19" s="9" t="s">
-        <v>11</v>
-      </c>
-      <c r="B19" s="16" t="s">
-        <v>62</v>
-      </c>
-      <c r="C19" s="10" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="20" spans="1:7" ht="21.6" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A20" s="21" t="s">
-        <v>34</v>
-      </c>
-      <c r="B20" s="21"/>
-      <c r="C20" s="21"/>
-    </row>
-    <row r="21" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A21" s="5" t="s">
-        <v>35</v>
-      </c>
-      <c r="B21" s="17">
-        <v>1</v>
-      </c>
-      <c r="C21" s="6" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="22" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A22" s="7" t="s">
-        <v>36</v>
-      </c>
-      <c r="B22" s="2">
-        <v>1</v>
-      </c>
-      <c r="C22" s="8" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="23" spans="1:7" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A23" s="9" t="s">
-        <v>38</v>
-      </c>
-      <c r="B23" s="16">
-        <v>0</v>
-      </c>
-      <c r="C23" s="10" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="24" spans="1:7" ht="21.6" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A24" s="19" t="s">
+      <c r="C28" s="13" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" ht="58.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A29" s="9" t="s">
+        <v>42</v>
+      </c>
+      <c r="B29" s="16">
+        <v>1.2E-2</v>
+      </c>
+      <c r="C29" s="14" t="s">
+        <v>43</v>
+      </c>
+      <c r="G29" s="15"/>
+    </row>
+    <row r="30" spans="1:7" ht="21.6" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A30" s="20" t="s">
         <v>29</v>
       </c>
-      <c r="B24" s="19"/>
-      <c r="C24" s="19"/>
-    </row>
-    <row r="25" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A25" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="B25" s="17" t="s">
-        <v>18</v>
-      </c>
-      <c r="C25" s="6" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="26" spans="1:7" ht="86.4" x14ac:dyDescent="0.3">
-      <c r="A26" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="B26" s="2">
-        <v>30</v>
-      </c>
-      <c r="C26" s="13" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="27" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A27" s="7" t="s">
-        <v>41</v>
-      </c>
-      <c r="B27" s="2">
-        <v>10</v>
-      </c>
-      <c r="C27" s="13" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="28" spans="1:7" ht="58.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A28" s="9" t="s">
-        <v>43</v>
-      </c>
-      <c r="B28" s="16">
-        <v>0.02</v>
-      </c>
-      <c r="C28" s="14" t="s">
-        <v>44</v>
-      </c>
-      <c r="G28" s="15"/>
-    </row>
-    <row r="29" spans="1:7" ht="21.6" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A29" s="20" t="s">
-        <v>30</v>
-      </c>
-      <c r="B29" s="20"/>
-      <c r="C29" s="20"/>
-    </row>
-    <row r="30" spans="1:7" ht="72" x14ac:dyDescent="0.3">
-      <c r="A30" s="5" t="s">
+      <c r="B30" s="20"/>
+      <c r="C30" s="20"/>
+    </row>
+    <row r="31" spans="1:7" ht="72" x14ac:dyDescent="0.3">
+      <c r="A31" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="B30" s="17">
+      <c r="B31" s="17">
         <v>15</v>
       </c>
-      <c r="C30" s="6" t="s">
+      <c r="C31" s="6" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="31" spans="1:7" ht="58.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A31" s="9" t="s">
+    <row r="32" spans="1:7" ht="58.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A32" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="B31" s="16">
+      <c r="B32" s="16">
         <v>0.1</v>
       </c>
-      <c r="C31" s="10" t="s">
+      <c r="C32" s="10" t="s">
         <v>58</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="6">
-    <mergeCell ref="A24:C24"/>
-    <mergeCell ref="A29:C29"/>
-    <mergeCell ref="A11:C11"/>
-    <mergeCell ref="A9:C9"/>
+    <mergeCell ref="A25:C25"/>
+    <mergeCell ref="A30:C30"/>
+    <mergeCell ref="A12:C12"/>
+    <mergeCell ref="A10:C10"/>
     <mergeCell ref="A6:C6"/>
-    <mergeCell ref="A20:C20"/>
+    <mergeCell ref="A21:C21"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
fix: add dplyr:: to all summarize or summarise found in codebase; refactor debar_dir check in general_functions
</commit_message>
<xml_diff>
--- a/settings.xlsx
+++ b/settings.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://charitede-my.sharepoint.com/personal/lev_petrov_charite_de/Documents/DOCTORATE/Cytomata/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="7" documentId="13_ncr:1_{9C262F40-B724-47DA-807B-CA0883A1DDFB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B25339B4-8BFC-4D9D-98A2-55C45FA88A0D}"/>
+  <xr:revisionPtr revIDLastSave="21" documentId="13_ncr:1_{9C262F40-B724-47DA-807B-CA0883A1DDFB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{45416216-9AE5-49C5-8A35-2C2E330F3C3F}"/>
   <bookViews>
-    <workbookView xWindow="-57720" yWindow="-11715" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1440" yWindow="1008" windowWidth="21600" windowHeight="11232" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="67">
   <si>
     <t>setting</t>
   </si>
@@ -174,9 +174,6 @@
     <t>HC-050</t>
   </si>
   <si>
-    <t>anca_panel_1</t>
-  </si>
-  <si>
     <t>Patterns present in the names of pre-processing channels that will be used to remove them. Input separated by comma and whitespace (", "). This can be adjusted in the panel.csv file afterwards.</t>
   </si>
   <si>
@@ -207,16 +204,28 @@
     <t>Control order of groups. Input group names separated by comma and whitespace (", "). For multiple grouping columns - separate by semicolon and whitespace (", "). If you do not want to input order for any specific grouping column - write NA.</t>
   </si>
   <si>
-    <t>HC, MPO, PR3; HC, ANCA</t>
-  </si>
-  <si>
-    <t>antigen, anca_status</t>
-  </si>
-  <si>
     <t>0, 30</t>
   </si>
   <si>
-    <t>CD8_T</t>
+    <t>iahp_panel_1</t>
+  </si>
+  <si>
+    <t>visit</t>
+  </si>
+  <si>
+    <t>S1.1, S1.2, HC</t>
+  </si>
+  <si>
+    <t>Monos_and_DCs, CD4_T, CD8_T, B</t>
+  </si>
+  <si>
+    <t>norm_mode</t>
+  </si>
+  <si>
+    <t>percentile</t>
+  </si>
+  <si>
+    <t>percentile or harmony. Harmony is weird right now, use percentile.</t>
   </si>
 </sst>
 </file>
@@ -383,7 +392,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -447,6 +456,9 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -728,10 +740,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G31"/>
+  <dimension ref="A1:G32"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="B28" sqref="B28"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -768,7 +780,7 @@
         <v>4</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>49</v>
+        <v>60</v>
       </c>
       <c r="C3" s="8" t="s">
         <v>21</v>
@@ -793,7 +805,7 @@
         <v>46</v>
       </c>
       <c r="C5" s="10" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="6" spans="1:3" ht="21.6" thickBot="1" x14ac:dyDescent="0.35">
@@ -808,7 +820,7 @@
         <v>25</v>
       </c>
       <c r="B7" s="17">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C7" s="6" t="s">
         <v>24</v>
@@ -822,251 +834,262 @@
         <v>48</v>
       </c>
       <c r="C8" s="10" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A9" s="22" t="s">
+        <v>64</v>
+      </c>
+      <c r="B9" s="16" t="s">
+        <v>65</v>
+      </c>
+      <c r="C9" s="16" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" ht="21.6" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A10" s="20" t="s">
+        <v>26</v>
+      </c>
+      <c r="B10" s="20"/>
+      <c r="C10" s="20"/>
+    </row>
+    <row r="11" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A11" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="B11" s="18">
+        <v>1</v>
+      </c>
+      <c r="C11" s="12" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" ht="21.6" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A12" s="20" t="s">
+        <v>28</v>
+      </c>
+      <c r="B12" s="20"/>
+      <c r="C12" s="20"/>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A13" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="B13" s="17">
+        <v>0</v>
+      </c>
+      <c r="C13" s="6" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A14" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="B14" s="2">
+        <v>1</v>
+      </c>
+      <c r="C14" s="8" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A15" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="C15" s="8" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="9" spans="1:3" ht="21.6" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A9" s="20" t="s">
-        <v>26</v>
-      </c>
-      <c r="B9" s="20"/>
-      <c r="C9" s="20"/>
-    </row>
-    <row r="10" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A10" s="11" t="s">
-        <v>27</v>
-      </c>
-      <c r="B10" s="18">
+    <row r="16" spans="1:3" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A16" s="7" t="s">
+        <v>47</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="C16" s="8" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A17" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="B17" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="C17" s="8" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" ht="187.2" x14ac:dyDescent="0.3">
+      <c r="A18" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="B18" s="2">
+        <v>1</v>
+      </c>
+      <c r="C18" s="8" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A19" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="B19" s="2">
+        <v>100</v>
+      </c>
+      <c r="C19" s="8" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" ht="43.8" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A20" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="B20" s="16" t="s">
+        <v>59</v>
+      </c>
+      <c r="C20" s="10" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" ht="21.6" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A21" s="21" t="s">
+        <v>34</v>
+      </c>
+      <c r="B21" s="21"/>
+      <c r="C21" s="21"/>
+    </row>
+    <row r="22" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A22" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="B22" s="17">
+        <v>1</v>
+      </c>
+      <c r="C22" s="6" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A23" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="B23" s="2">
+        <v>1</v>
+      </c>
+      <c r="C23" s="8" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A24" s="9" t="s">
+        <v>38</v>
+      </c>
+      <c r="B24" s="16">
         <v>0</v>
       </c>
-      <c r="C10" s="12" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" ht="21.6" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A11" s="20" t="s">
-        <v>28</v>
-      </c>
-      <c r="B11" s="20"/>
-      <c r="C11" s="20"/>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A12" s="5" t="s">
-        <v>31</v>
-      </c>
-      <c r="B12" s="17">
-        <v>1</v>
-      </c>
-      <c r="C12" s="6" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A13" s="7" t="s">
-        <v>5</v>
-      </c>
-      <c r="B13" s="2">
-        <v>0</v>
-      </c>
-      <c r="C13" s="8" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A14" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="B14" s="2" t="s">
-        <v>61</v>
-      </c>
-      <c r="C14" s="8" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A15" s="7" t="s">
-        <v>47</v>
-      </c>
-      <c r="B15" s="2" t="s">
-        <v>60</v>
-      </c>
-      <c r="C15" s="8" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A16" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="B16" s="2" t="s">
-        <v>63</v>
-      </c>
-      <c r="C16" s="8" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="17" spans="1:7" ht="187.2" x14ac:dyDescent="0.3">
-      <c r="A17" s="7" t="s">
+      <c r="C24" s="10" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" ht="21.6" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A25" s="19" t="s">
+        <v>29</v>
+      </c>
+      <c r="B25" s="19"/>
+      <c r="C25" s="19"/>
+    </row>
+    <row r="26" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A26" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="B26" s="17" t="s">
+        <v>18</v>
+      </c>
+      <c r="C26" s="6" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" ht="86.4" x14ac:dyDescent="0.3">
+      <c r="A27" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="B27" s="2">
+        <v>30</v>
+      </c>
+      <c r="C27" s="13" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A28" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="B28" s="2">
         <v>10</v>
       </c>
-      <c r="B17" s="2">
-        <v>1</v>
-      </c>
-      <c r="C17" s="8" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="18" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A18" s="7" t="s">
-        <v>32</v>
-      </c>
-      <c r="B18" s="2">
-        <v>100</v>
-      </c>
-      <c r="C18" s="8" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="19" spans="1:7" ht="43.8" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A19" s="9" t="s">
-        <v>11</v>
-      </c>
-      <c r="B19" s="16" t="s">
-        <v>62</v>
-      </c>
-      <c r="C19" s="10" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="20" spans="1:7" ht="21.6" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A20" s="21" t="s">
-        <v>34</v>
-      </c>
-      <c r="B20" s="21"/>
-      <c r="C20" s="21"/>
-    </row>
-    <row r="21" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A21" s="5" t="s">
-        <v>35</v>
-      </c>
-      <c r="B21" s="17">
-        <v>1</v>
-      </c>
-      <c r="C21" s="6" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="22" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A22" s="7" t="s">
-        <v>36</v>
-      </c>
-      <c r="B22" s="2">
-        <v>1</v>
-      </c>
-      <c r="C22" s="8" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="23" spans="1:7" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A23" s="9" t="s">
-        <v>38</v>
-      </c>
-      <c r="B23" s="16">
-        <v>0</v>
-      </c>
-      <c r="C23" s="10" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="24" spans="1:7" ht="21.6" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A24" s="19" t="s">
-        <v>29</v>
-      </c>
-      <c r="B24" s="19"/>
-      <c r="C24" s="19"/>
-    </row>
-    <row r="25" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A25" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="B25" s="17" t="s">
-        <v>18</v>
-      </c>
-      <c r="C25" s="6" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="26" spans="1:7" ht="86.4" x14ac:dyDescent="0.3">
-      <c r="A26" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="B26" s="2">
+      <c r="C28" s="13" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" ht="58.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A29" s="9" t="s">
+        <v>43</v>
+      </c>
+      <c r="B29" s="16">
+        <v>0.02</v>
+      </c>
+      <c r="C29" s="14" t="s">
+        <v>44</v>
+      </c>
+      <c r="G29" s="15"/>
+    </row>
+    <row r="30" spans="1:7" ht="21.6" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A30" s="20" t="s">
         <v>30</v>
       </c>
-      <c r="C26" s="13" t="s">
+      <c r="B30" s="20"/>
+      <c r="C30" s="20"/>
+    </row>
+    <row r="31" spans="1:7" ht="72" x14ac:dyDescent="0.3">
+      <c r="A31" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="B31" s="17">
+        <v>15</v>
+      </c>
+      <c r="C31" s="6" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="27" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A27" s="7" t="s">
-        <v>41</v>
-      </c>
-      <c r="B27" s="2">
-        <v>10</v>
-      </c>
-      <c r="C27" s="13" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="28" spans="1:7" ht="58.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A28" s="9" t="s">
-        <v>43</v>
-      </c>
-      <c r="B28" s="16">
-        <v>0.02</v>
-      </c>
-      <c r="C28" s="14" t="s">
-        <v>44</v>
-      </c>
-      <c r="G28" s="15"/>
-    </row>
-    <row r="29" spans="1:7" ht="21.6" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A29" s="20" t="s">
-        <v>30</v>
-      </c>
-      <c r="B29" s="20"/>
-      <c r="C29" s="20"/>
-    </row>
-    <row r="30" spans="1:7" ht="72" x14ac:dyDescent="0.3">
-      <c r="A30" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="B30" s="17">
+    <row r="32" spans="1:7" ht="58.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A32" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="C30" s="6" t="s">
+      <c r="B32" s="16">
+        <v>0.1</v>
+      </c>
+      <c r="C32" s="10" t="s">
         <v>57</v>
-      </c>
-    </row>
-    <row r="31" spans="1:7" ht="58.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A31" s="9" t="s">
-        <v>15</v>
-      </c>
-      <c r="B31" s="16">
-        <v>0.1</v>
-      </c>
-      <c r="C31" s="10" t="s">
-        <v>58</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="6">
-    <mergeCell ref="A24:C24"/>
-    <mergeCell ref="A29:C29"/>
-    <mergeCell ref="A11:C11"/>
-    <mergeCell ref="A9:C9"/>
+    <mergeCell ref="A25:C25"/>
+    <mergeCell ref="A30:C30"/>
+    <mergeCell ref="A12:C12"/>
+    <mergeCell ref="A10:C10"/>
     <mergeCell ref="A6:C6"/>
-    <mergeCell ref="A20:C20"/>
+    <mergeCell ref="A21:C21"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
feat: pairwise testing and boxplots core_addons
</commit_message>
<xml_diff>
--- a/settings.xlsx
+++ b/settings.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://charitede-my.sharepoint.com/personal/lev_petrov_charite_de/Documents/DOCTORATE/Cytomata_data/iahp_panel_1/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="20" documentId="13_ncr:1_{9C262F40-B724-47DA-807B-CA0883A1DDFB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{859FDE1F-19A7-4992-B7F9-0C57C426998A}"/>
+  <xr:revisionPtr revIDLastSave="26" documentId="13_ncr:1_{9C262F40-B724-47DA-807B-CA0883A1DDFB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A0EDFBD9-E490-4A5E-9D63-272ED4A8D50D}"/>
   <bookViews>
     <workbookView xWindow="1440" yWindow="1008" windowWidth="21600" windowHeight="11232" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -216,9 +216,6 @@
     <t>S1.1, S1.2, HC</t>
   </si>
   <si>
-    <t>Monos_and_DCs, CD4_T, CD8_T, B</t>
-  </si>
-  <si>
     <t>norm_mode</t>
   </si>
   <si>
@@ -226,6 +223,9 @@
   </si>
   <si>
     <t>percentile or harmony. Harmony is weird for now, will fix.</t>
+  </si>
+  <si>
+    <t>Monos_and_DCs, CD4_T, CD8_T, B, TCRgd, NK</t>
   </si>
 </sst>
 </file>
@@ -448,6 +448,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -456,9 +459,6 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -742,8 +742,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G32"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C8" sqref="A8:C8"/>
+    <sheetView tabSelected="1" topLeftCell="A14" workbookViewId="0">
+      <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -809,18 +809,18 @@
       </c>
     </row>
     <row r="6" spans="1:3" ht="21.6" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A6" s="20" t="s">
+      <c r="A6" s="21" t="s">
         <v>23</v>
       </c>
-      <c r="B6" s="20"/>
-      <c r="C6" s="20"/>
+      <c r="B6" s="21"/>
+      <c r="C6" s="21"/>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" s="5" t="s">
         <v>25</v>
       </c>
       <c r="B7" s="17">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C7" s="6" t="s">
         <v>24</v>
@@ -828,13 +828,13 @@
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="B8" s="19" t="s">
         <v>64</v>
       </c>
-      <c r="B8" s="22" t="s">
+      <c r="C8" s="8" t="s">
         <v>65</v>
-      </c>
-      <c r="C8" s="8" t="s">
-        <v>66</v>
       </c>
     </row>
     <row r="9" spans="1:3" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
@@ -849,36 +849,36 @@
       </c>
     </row>
     <row r="10" spans="1:3" ht="21.6" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A10" s="20" t="s">
+      <c r="A10" s="21" t="s">
         <v>26</v>
       </c>
-      <c r="B10" s="20"/>
-      <c r="C10" s="20"/>
+      <c r="B10" s="21"/>
+      <c r="C10" s="21"/>
     </row>
     <row r="11" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A11" s="11" t="s">
         <v>27</v>
       </c>
       <c r="B11" s="18">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C11" s="12" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="12" spans="1:3" ht="21.6" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A12" s="20" t="s">
+      <c r="A12" s="21" t="s">
         <v>28</v>
       </c>
-      <c r="B12" s="20"/>
-      <c r="C12" s="20"/>
+      <c r="B12" s="21"/>
+      <c r="C12" s="21"/>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A13" s="5" t="s">
         <v>31</v>
       </c>
       <c r="B13" s="17">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C13" s="6" t="s">
         <v>24</v>
@@ -922,7 +922,7 @@
         <v>9</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
       <c r="C17" s="8" t="s">
         <v>52</v>
@@ -962,11 +962,11 @@
       </c>
     </row>
     <row r="21" spans="1:7" ht="21.6" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A21" s="21" t="s">
+      <c r="A21" s="22" t="s">
         <v>34</v>
       </c>
-      <c r="B21" s="21"/>
-      <c r="C21" s="21"/>
+      <c r="B21" s="22"/>
+      <c r="C21" s="22"/>
     </row>
     <row r="22" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A22" s="5" t="s">
@@ -1002,11 +1002,11 @@
       </c>
     </row>
     <row r="25" spans="1:7" ht="21.6" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A25" s="19" t="s">
+      <c r="A25" s="20" t="s">
         <v>29</v>
       </c>
-      <c r="B25" s="19"/>
-      <c r="C25" s="19"/>
+      <c r="B25" s="20"/>
+      <c r="C25" s="20"/>
     </row>
     <row r="26" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A26" s="5" t="s">
@@ -1054,11 +1054,11 @@
       <c r="G29" s="15"/>
     </row>
     <row r="30" spans="1:7" ht="21.6" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A30" s="20" t="s">
+      <c r="A30" s="21" t="s">
         <v>30</v>
       </c>
-      <c r="B30" s="20"/>
-      <c r="C30" s="20"/>
+      <c r="B30" s="21"/>
+      <c r="C30" s="21"/>
     </row>
     <row r="31" spans="1:7" ht="72" x14ac:dyDescent="0.3">
       <c r="A31" s="5" t="s">

</xml_diff>

<commit_message>
add: treat_NA_as_group setting to automatically drop events with NA value in grouping column from the analysis
</commit_message>
<xml_diff>
--- a/settings.xlsx
+++ b/settings.xlsx
@@ -1,24 +1,35 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24332"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27932"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://charitede-my.sharepoint.com/personal/lev_petrov_charite_de/Documents/DOCTORATE/Cytomata_data/iahp_panel_1/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://charitede-my.sharepoint.com/personal/lev_petrov_charite_de/Documents/DOCTORATE/Cytomata/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="26" documentId="13_ncr:1_{9C262F40-B724-47DA-807B-CA0883A1DDFB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A0EDFBD9-E490-4A5E-9D63-272ED4A8D50D}"/>
+  <xr:revisionPtr revIDLastSave="52" documentId="13_ncr:1_{9C262F40-B724-47DA-807B-CA0883A1DDFB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{3DD45382-447F-4FF1-934C-9EF2565386A3}"/>
   <bookViews>
-    <workbookView xWindow="1440" yWindow="1008" windowWidth="21600" windowHeight="11232" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="8664" yWindow="3324" windowWidth="28776" windowHeight="15288" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -165,15 +176,9 @@
     <t>excluded_channels</t>
   </si>
   <si>
-    <t>B2M, DNA, Bead, LD, Live, Dead, ID, Cell-ID, Cell_ID</t>
-  </si>
-  <si>
     <t>grouping_orders</t>
   </si>
   <si>
-    <t>HC-050</t>
-  </si>
-  <si>
     <t>Patterns present in the names of pre-processing channels that will be used to remove them. Input separated by comma and whitespace (", "). This can be adjusted in the panel.csv file afterwards.</t>
   </si>
   <si>
@@ -201,21 +206,9 @@
     <t>UMAPs min_dist. Lower values lead to clumpier embeddings, higher make them more spread-out. Accepts multiple values, separated by comma and whitespace (", ") of different values are needed for each data_subset. Order is given by data_subset vector.</t>
   </si>
   <si>
-    <t>Control order of groups. Input group names separated by comma and whitespace (", "). For multiple grouping columns - separate by semicolon and whitespace (", "). If you do not want to input order for any specific grouping column - write NA.</t>
-  </si>
-  <si>
     <t>0, 30</t>
   </si>
   <si>
-    <t>iahp_panel_1</t>
-  </si>
-  <si>
-    <t>visit</t>
-  </si>
-  <si>
-    <t>S1.1, S1.2, HC</t>
-  </si>
-  <si>
     <t>norm_mode</t>
   </si>
   <si>
@@ -225,7 +218,25 @@
     <t>percentile or harmony. Harmony is weird for now, will fix.</t>
   </si>
   <si>
-    <t>Monos_and_DCs, CD4_T, CD8_T, B, TCRgd, NK</t>
+    <t>B</t>
+  </si>
+  <si>
+    <t>B2M, DNA, Bead, LD, Live, Dead, ID, Cell-ID, Cell_ID, NA</t>
+  </si>
+  <si>
+    <t>iacs_panel_1</t>
+  </si>
+  <si>
+    <t>HC-04</t>
+  </si>
+  <si>
+    <t>Control order of groups. Input group names separated by comma and whitespace (", "). For multiple grouping columns - separate by semicolon and whitespace ("; "). If you do not want to input order for any specific grouping column - write NA.</t>
+  </si>
+  <si>
+    <t>hc_vs_pc_pre_treat, responder_pre_treat, pre_post, pre_post_w_hc</t>
+  </si>
+  <si>
+    <t>HC, S1.1; yes, no; S1.1, S1.2; HC, S1.1, S1.2</t>
   </si>
 </sst>
 </file>
@@ -742,8 +753,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G32"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A14" workbookViewId="0">
-      <selection activeCell="B16" sqref="B16"/>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="B23" sqref="B23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -780,7 +791,7 @@
         <v>4</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="C3" s="8" t="s">
         <v>21</v>
@@ -802,10 +813,10 @@
         <v>45</v>
       </c>
       <c r="B5" s="16" t="s">
-        <v>46</v>
+        <v>61</v>
       </c>
       <c r="C5" s="10" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
     </row>
     <row r="6" spans="1:3" ht="21.6" thickBot="1" x14ac:dyDescent="0.35">
@@ -828,13 +839,13 @@
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" s="7" t="s">
-        <v>63</v>
+        <v>57</v>
       </c>
       <c r="B8" s="19" t="s">
-        <v>64</v>
+        <v>58</v>
       </c>
       <c r="C8" s="8" t="s">
-        <v>65</v>
+        <v>59</v>
       </c>
     </row>
     <row r="9" spans="1:3" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
@@ -842,10 +853,10 @@
         <v>7</v>
       </c>
       <c r="B9" s="16" t="s">
+        <v>63</v>
+      </c>
+      <c r="C9" s="10" t="s">
         <v>48</v>
-      </c>
-      <c r="C9" s="10" t="s">
-        <v>50</v>
       </c>
     </row>
     <row r="10" spans="1:3" ht="21.6" thickBot="1" x14ac:dyDescent="0.35">
@@ -900,21 +911,21 @@
         <v>8</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>61</v>
+        <v>65</v>
       </c>
       <c r="C15" s="8" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
     </row>
     <row r="16" spans="1:3" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A16" s="7" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>62</v>
+        <v>66</v>
       </c>
       <c r="C16" s="8" t="s">
-        <v>58</v>
+        <v>64</v>
       </c>
     </row>
     <row r="17" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
@@ -922,10 +933,10 @@
         <v>9</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>66</v>
+        <v>60</v>
       </c>
       <c r="C17" s="8" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
     </row>
     <row r="18" spans="1:7" ht="187.2" x14ac:dyDescent="0.3">
@@ -936,7 +947,7 @@
         <v>1</v>
       </c>
       <c r="C18" s="8" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
     </row>
     <row r="19" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
@@ -955,10 +966,10 @@
         <v>11</v>
       </c>
       <c r="B20" s="16" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="C20" s="10" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
     </row>
     <row r="21" spans="1:7" ht="21.6" thickBot="1" x14ac:dyDescent="0.35">
@@ -1027,7 +1038,7 @@
         <v>30</v>
       </c>
       <c r="C27" s="13" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
     </row>
     <row r="28" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
@@ -1046,7 +1057,7 @@
         <v>43</v>
       </c>
       <c r="B29" s="16">
-        <v>0.02</v>
+        <v>7.0000000000000001E-3</v>
       </c>
       <c r="C29" s="14" t="s">
         <v>44</v>
@@ -1068,7 +1079,7 @@
         <v>15</v>
       </c>
       <c r="C31" s="6" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
     </row>
     <row r="32" spans="1:7" ht="58.2" thickBot="1" x14ac:dyDescent="0.35">
@@ -1079,7 +1090,7 @@
         <v>0.1</v>
       </c>
       <c r="C32" s="10" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add: new custom palette, conditional check for analysis_core_addons
</commit_message>
<xml_diff>
--- a/settings.xlsx
+++ b/settings.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27932"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24332"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://charitede-my.sharepoint.com/personal/lev_petrov_charite_de/Documents/DOCTORATE/Cytomata/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://charitede-my.sharepoint.com/personal/lev_petrov_charite_de/Documents/DOCTORATE/Cytomata_data/iacs_panel_1/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="52" documentId="13_ncr:1_{9C262F40-B724-47DA-807B-CA0883A1DDFB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{3DD45382-447F-4FF1-934C-9EF2565386A3}"/>
+  <xr:revisionPtr revIDLastSave="60" documentId="13_ncr:1_{9C262F40-B724-47DA-807B-CA0883A1DDFB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E79D95C2-3479-4A96-AFA4-29FE57FB9764}"/>
   <bookViews>
-    <workbookView xWindow="8664" yWindow="3324" windowWidth="28776" windowHeight="15288" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -27,8 +27,6 @@
         <xcalcf:feature name="microsoft.com:FV"/>
         <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -36,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="69">
   <si>
     <t>setting</t>
   </si>
@@ -218,9 +216,6 @@
     <t>percentile or harmony. Harmony is weird for now, will fix.</t>
   </si>
   <si>
-    <t>B</t>
-  </si>
-  <si>
     <t>B2M, DNA, Bead, LD, Live, Dead, ID, Cell-ID, Cell_ID, NA</t>
   </si>
   <si>
@@ -237,6 +232,15 @@
   </si>
   <si>
     <t>HC, S1.1; yes, no; S1.1, S1.2; HC, S1.1, S1.2</t>
+  </si>
+  <si>
+    <t>treat_NA_as_group</t>
+  </si>
+  <si>
+    <t>0 (off, default) or 1 (on)</t>
+  </si>
+  <si>
+    <t>B, CD4_T</t>
   </si>
 </sst>
 </file>
@@ -751,10 +755,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G32"/>
+  <dimension ref="A1:G33"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="B23" sqref="B23"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="F28" sqref="F28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -791,7 +795,7 @@
         <v>4</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C3" s="8" t="s">
         <v>21</v>
@@ -813,7 +817,7 @@
         <v>45</v>
       </c>
       <c r="B5" s="16" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C5" s="10" t="s">
         <v>47</v>
@@ -853,7 +857,7 @@
         <v>7</v>
       </c>
       <c r="B9" s="16" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C9" s="10" t="s">
         <v>48</v>
@@ -911,7 +915,7 @@
         <v>8</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C15" s="8" t="s">
         <v>49</v>
@@ -922,185 +926,196 @@
         <v>46</v>
       </c>
       <c r="B16" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="C16" s="8" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A17" s="7" t="s">
         <v>66</v>
       </c>
-      <c r="C16" s="8" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="17" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A17" s="7" t="s">
+      <c r="B17" s="2">
+        <v>0</v>
+      </c>
+      <c r="C17" s="8" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A18" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="B17" s="2" t="s">
-        <v>60</v>
-      </c>
-      <c r="C17" s="8" t="s">
+      <c r="B18" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="C18" s="8" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="18" spans="1:7" ht="187.2" x14ac:dyDescent="0.3">
-      <c r="A18" s="7" t="s">
+    <row r="19" spans="1:7" ht="187.2" x14ac:dyDescent="0.3">
+      <c r="A19" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="B18" s="2">
+      <c r="B19" s="2">
         <v>1</v>
       </c>
-      <c r="C18" s="8" t="s">
+      <c r="C19" s="8" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="19" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A19" s="7" t="s">
+    <row r="20" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A20" s="7" t="s">
         <v>32</v>
       </c>
-      <c r="B19" s="2">
+      <c r="B20" s="2">
         <v>100</v>
       </c>
-      <c r="C19" s="8" t="s">
+      <c r="C20" s="8" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="20" spans="1:7" ht="43.8" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A20" s="9" t="s">
+    <row r="21" spans="1:7" ht="43.8" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A21" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="B20" s="16" t="s">
+      <c r="B21" s="16" t="s">
         <v>56</v>
       </c>
-      <c r="C20" s="10" t="s">
+      <c r="C21" s="10" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="21" spans="1:7" ht="21.6" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A21" s="22" t="s">
+    <row r="22" spans="1:7" ht="21.6" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A22" s="22" t="s">
         <v>34</v>
       </c>
-      <c r="B21" s="22"/>
-      <c r="C21" s="22"/>
-    </row>
-    <row r="22" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A22" s="5" t="s">
+      <c r="B22" s="22"/>
+      <c r="C22" s="22"/>
+    </row>
+    <row r="23" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A23" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="B22" s="17">
+      <c r="B23" s="17">
         <v>1</v>
       </c>
-      <c r="C22" s="6" t="s">
+      <c r="C23" s="6" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="23" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A23" s="7" t="s">
+    <row r="24" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A24" s="7" t="s">
         <v>36</v>
       </c>
-      <c r="B23" s="2">
+      <c r="B24" s="2">
         <v>1</v>
       </c>
-      <c r="C23" s="8" t="s">
+      <c r="C24" s="8" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="24" spans="1:7" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A24" s="9" t="s">
+    <row r="25" spans="1:7" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A25" s="9" t="s">
         <v>38</v>
       </c>
-      <c r="B24" s="16">
+      <c r="B25" s="16">
         <v>0</v>
       </c>
-      <c r="C24" s="10" t="s">
+      <c r="C25" s="10" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="25" spans="1:7" ht="21.6" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A25" s="20" t="s">
+    <row r="26" spans="1:7" ht="21.6" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A26" s="20" t="s">
         <v>29</v>
       </c>
-      <c r="B25" s="20"/>
-      <c r="C25" s="20"/>
-    </row>
-    <row r="26" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A26" s="5" t="s">
+      <c r="B26" s="20"/>
+      <c r="C26" s="20"/>
+    </row>
+    <row r="27" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A27" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="B26" s="17" t="s">
+      <c r="B27" s="17" t="s">
         <v>18</v>
       </c>
-      <c r="C26" s="6" t="s">
+      <c r="C27" s="6" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="27" spans="1:7" ht="86.4" x14ac:dyDescent="0.3">
-      <c r="A27" s="7" t="s">
+    <row r="28" spans="1:7" ht="86.4" x14ac:dyDescent="0.3">
+      <c r="A28" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="B27" s="2">
+      <c r="B28" s="2">
         <v>30</v>
       </c>
-      <c r="C27" s="13" t="s">
+      <c r="C28" s="13" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="28" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A28" s="7" t="s">
+    <row r="29" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A29" s="7" t="s">
         <v>41</v>
       </c>
-      <c r="B28" s="2">
+      <c r="B29" s="2">
         <v>10</v>
       </c>
-      <c r="C28" s="13" t="s">
+      <c r="C29" s="13" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="29" spans="1:7" ht="58.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A29" s="9" t="s">
+    <row r="30" spans="1:7" ht="58.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A30" s="9" t="s">
         <v>43</v>
       </c>
-      <c r="B29" s="16">
+      <c r="B30" s="16">
         <v>7.0000000000000001E-3</v>
       </c>
-      <c r="C29" s="14" t="s">
+      <c r="C30" s="14" t="s">
         <v>44</v>
       </c>
-      <c r="G29" s="15"/>
-    </row>
-    <row r="30" spans="1:7" ht="21.6" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A30" s="21" t="s">
+      <c r="G30" s="15"/>
+    </row>
+    <row r="31" spans="1:7" ht="21.6" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A31" s="21" t="s">
         <v>30</v>
       </c>
-      <c r="B30" s="21"/>
-      <c r="C30" s="21"/>
-    </row>
-    <row r="31" spans="1:7" ht="72" x14ac:dyDescent="0.3">
-      <c r="A31" s="5" t="s">
+      <c r="B31" s="21"/>
+      <c r="C31" s="21"/>
+    </row>
+    <row r="32" spans="1:7" ht="72" x14ac:dyDescent="0.3">
+      <c r="A32" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="B31" s="17">
+      <c r="B32" s="17">
         <v>15</v>
       </c>
-      <c r="C31" s="6" t="s">
+      <c r="C32" s="6" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="32" spans="1:7" ht="58.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A32" s="9" t="s">
+    <row r="33" spans="1:3" ht="58.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A33" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="B32" s="16">
+      <c r="B33" s="16">
         <v>0.1</v>
       </c>
-      <c r="C32" s="10" t="s">
+      <c r="C33" s="10" t="s">
         <v>55</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="6">
-    <mergeCell ref="A25:C25"/>
-    <mergeCell ref="A30:C30"/>
+    <mergeCell ref="A26:C26"/>
+    <mergeCell ref="A31:C31"/>
     <mergeCell ref="A12:C12"/>
     <mergeCell ref="A10:C10"/>
     <mergeCell ref="A6:C6"/>
-    <mergeCell ref="A21:C21"/>
+    <mergeCell ref="A22:C22"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
refactor: update batch normalization logic to use meta table for filtering
</commit_message>
<xml_diff>
--- a/settings.xlsx
+++ b/settings.xlsx
@@ -1,40 +1,31 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24332"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27932"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://charitede-my.sharepoint.com/personal/lev_petrov_charite_de/Documents/DOCTORATE/Cytomata_data/iacs_panel_1/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://charitede-my.sharepoint.com/personal/lev_petrov_charite_de/Documents/DOCTORATE/Cytomata/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="60" documentId="13_ncr:1_{9C262F40-B724-47DA-807B-CA0883A1DDFB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E79D95C2-3479-4A96-AFA4-29FE57FB9764}"/>
+  <xr:revisionPtr revIDLastSave="37" documentId="13_ncr:1_{9C262F40-B724-47DA-807B-CA0883A1DDFB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F1A53FD9-25B2-47DA-B102-657616DD89E5}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1260" yWindow="4872" windowWidth="28776" windowHeight="16176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="67">
   <si>
     <t>setting</t>
   </si>
@@ -204,9 +195,15 @@
     <t>UMAPs min_dist. Lower values lead to clumpier embeddings, higher make them more spread-out. Accepts multiple values, separated by comma and whitespace (", ") of different values are needed for each data_subset. Order is given by data_subset vector.</t>
   </si>
   <si>
+    <t>Control order of groups. Input group names separated by comma and whitespace (", "). For multiple grouping columns - separate by semicolon and whitespace (", "). If you do not want to input order for any specific grouping column - write NA.</t>
+  </si>
+  <si>
     <t>0, 30</t>
   </si>
   <si>
+    <t>visit</t>
+  </si>
+  <si>
     <t>norm_mode</t>
   </si>
   <si>
@@ -216,31 +213,19 @@
     <t>percentile or harmony. Harmony is weird for now, will fix.</t>
   </si>
   <si>
+    <t>HC, S1.1, S1.2</t>
+  </si>
+  <si>
+    <t>B</t>
+  </si>
+  <si>
+    <t>dc10</t>
+  </si>
+  <si>
+    <t>Anchor</t>
+  </si>
+  <si>
     <t>B2M, DNA, Bead, LD, Live, Dead, ID, Cell-ID, Cell_ID, NA</t>
-  </si>
-  <si>
-    <t>iacs_panel_1</t>
-  </si>
-  <si>
-    <t>HC-04</t>
-  </si>
-  <si>
-    <t>Control order of groups. Input group names separated by comma and whitespace (", "). For multiple grouping columns - separate by semicolon and whitespace ("; "). If you do not want to input order for any specific grouping column - write NA.</t>
-  </si>
-  <si>
-    <t>hc_vs_pc_pre_treat, responder_pre_treat, pre_post, pre_post_w_hc</t>
-  </si>
-  <si>
-    <t>HC, S1.1; yes, no; S1.1, S1.2; HC, S1.1, S1.2</t>
-  </si>
-  <si>
-    <t>treat_NA_as_group</t>
-  </si>
-  <si>
-    <t>0 (off, default) or 1 (on)</t>
-  </si>
-  <si>
-    <t>B, CD4_T</t>
   </si>
 </sst>
 </file>
@@ -755,10 +740,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G33"/>
+  <dimension ref="A1:G32"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="F28" sqref="F28"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -795,7 +780,7 @@
         <v>4</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>61</v>
+        <v>64</v>
       </c>
       <c r="C3" s="8" t="s">
         <v>21</v>
@@ -817,7 +802,7 @@
         <v>45</v>
       </c>
       <c r="B5" s="16" t="s">
-        <v>60</v>
+        <v>66</v>
       </c>
       <c r="C5" s="10" t="s">
         <v>47</v>
@@ -835,7 +820,7 @@
         <v>25</v>
       </c>
       <c r="B7" s="17">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C7" s="6" t="s">
         <v>24</v>
@@ -843,13 +828,13 @@
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" s="7" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="B8" s="19" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="C8" s="8" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
     </row>
     <row r="9" spans="1:3" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
@@ -857,7 +842,7 @@
         <v>7</v>
       </c>
       <c r="B9" s="16" t="s">
-        <v>62</v>
+        <v>65</v>
       </c>
       <c r="C9" s="10" t="s">
         <v>48</v>
@@ -875,7 +860,7 @@
         <v>27</v>
       </c>
       <c r="B11" s="18">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C11" s="12" t="s">
         <v>24</v>
@@ -893,7 +878,7 @@
         <v>31</v>
       </c>
       <c r="B13" s="17">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C13" s="6" t="s">
         <v>24</v>
@@ -915,7 +900,7 @@
         <v>8</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>64</v>
+        <v>58</v>
       </c>
       <c r="C15" s="8" t="s">
         <v>49</v>
@@ -926,196 +911,185 @@
         <v>46</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="C16" s="8" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A17" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="B17" s="2" t="s">
         <v>63</v>
       </c>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A17" s="7" t="s">
-        <v>66</v>
-      </c>
-      <c r="B17" s="2">
+      <c r="C17" s="8" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" ht="187.2" x14ac:dyDescent="0.3">
+      <c r="A18" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="B18" s="2">
+        <v>1</v>
+      </c>
+      <c r="C18" s="8" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A19" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="B19" s="2">
+        <v>100</v>
+      </c>
+      <c r="C19" s="8" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" ht="43.8" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A20" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="B20" s="16" t="s">
+        <v>57</v>
+      </c>
+      <c r="C20" s="10" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" ht="21.6" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A21" s="22" t="s">
+        <v>34</v>
+      </c>
+      <c r="B21" s="22"/>
+      <c r="C21" s="22"/>
+    </row>
+    <row r="22" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A22" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="B22" s="17">
+        <v>1</v>
+      </c>
+      <c r="C22" s="6" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A23" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="B23" s="2">
+        <v>1</v>
+      </c>
+      <c r="C23" s="8" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A24" s="9" t="s">
+        <v>38</v>
+      </c>
+      <c r="B24" s="16">
         <v>0</v>
       </c>
-      <c r="C17" s="8" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="18" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A18" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="B18" s="2" t="s">
-        <v>68</v>
-      </c>
-      <c r="C18" s="8" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="19" spans="1:7" ht="187.2" x14ac:dyDescent="0.3">
-      <c r="A19" s="7" t="s">
+      <c r="C24" s="10" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" ht="21.6" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A25" s="20" t="s">
+        <v>29</v>
+      </c>
+      <c r="B25" s="20"/>
+      <c r="C25" s="20"/>
+    </row>
+    <row r="26" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A26" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="B26" s="17" t="s">
+        <v>18</v>
+      </c>
+      <c r="C26" s="6" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" ht="86.4" x14ac:dyDescent="0.3">
+      <c r="A27" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="B27" s="2">
+        <v>30</v>
+      </c>
+      <c r="C27" s="13" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A28" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="B28" s="2">
         <v>10</v>
       </c>
-      <c r="B19" s="2">
-        <v>1</v>
-      </c>
-      <c r="C19" s="8" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="20" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A20" s="7" t="s">
-        <v>32</v>
-      </c>
-      <c r="B20" s="2">
-        <v>100</v>
-      </c>
-      <c r="C20" s="8" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="21" spans="1:7" ht="43.8" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A21" s="9" t="s">
-        <v>11</v>
-      </c>
-      <c r="B21" s="16" t="s">
-        <v>56</v>
-      </c>
-      <c r="C21" s="10" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="22" spans="1:7" ht="21.6" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A22" s="22" t="s">
-        <v>34</v>
-      </c>
-      <c r="B22" s="22"/>
-      <c r="C22" s="22"/>
-    </row>
-    <row r="23" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A23" s="5" t="s">
-        <v>35</v>
-      </c>
-      <c r="B23" s="17">
-        <v>1</v>
-      </c>
-      <c r="C23" s="6" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="24" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A24" s="7" t="s">
-        <v>36</v>
-      </c>
-      <c r="B24" s="2">
-        <v>1</v>
-      </c>
-      <c r="C24" s="8" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="25" spans="1:7" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A25" s="9" t="s">
-        <v>38</v>
-      </c>
-      <c r="B25" s="16">
-        <v>0</v>
-      </c>
-      <c r="C25" s="10" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="26" spans="1:7" ht="21.6" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A26" s="20" t="s">
-        <v>29</v>
-      </c>
-      <c r="B26" s="20"/>
-      <c r="C26" s="20"/>
-    </row>
-    <row r="27" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A27" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="B27" s="17" t="s">
-        <v>18</v>
-      </c>
-      <c r="C27" s="6" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="28" spans="1:7" ht="86.4" x14ac:dyDescent="0.3">
-      <c r="A28" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="B28" s="2">
+      <c r="C28" s="13" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" ht="58.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A29" s="9" t="s">
+        <v>43</v>
+      </c>
+      <c r="B29" s="16">
+        <v>7.0000000000000001E-3</v>
+      </c>
+      <c r="C29" s="14" t="s">
+        <v>44</v>
+      </c>
+      <c r="G29" s="15"/>
+    </row>
+    <row r="30" spans="1:7" ht="21.6" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A30" s="21" t="s">
         <v>30</v>
       </c>
-      <c r="C28" s="13" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="29" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A29" s="7" t="s">
-        <v>41</v>
-      </c>
-      <c r="B29" s="2">
-        <v>10</v>
-      </c>
-      <c r="C29" s="13" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="30" spans="1:7" ht="58.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A30" s="9" t="s">
-        <v>43</v>
-      </c>
-      <c r="B30" s="16">
-        <v>7.0000000000000001E-3</v>
-      </c>
-      <c r="C30" s="14" t="s">
-        <v>44</v>
-      </c>
-      <c r="G30" s="15"/>
-    </row>
-    <row r="31" spans="1:7" ht="21.6" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A31" s="21" t="s">
-        <v>30</v>
-      </c>
-      <c r="B31" s="21"/>
-      <c r="C31" s="21"/>
-    </row>
-    <row r="32" spans="1:7" ht="72" x14ac:dyDescent="0.3">
-      <c r="A32" s="5" t="s">
+      <c r="B30" s="21"/>
+      <c r="C30" s="21"/>
+    </row>
+    <row r="31" spans="1:7" ht="72" x14ac:dyDescent="0.3">
+      <c r="A31" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="B32" s="17">
+      <c r="B31" s="17">
         <v>15</v>
       </c>
-      <c r="C32" s="6" t="s">
+      <c r="C31" s="6" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="33" spans="1:3" ht="58.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A33" s="9" t="s">
+    <row r="32" spans="1:7" ht="58.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A32" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="B33" s="16">
+      <c r="B32" s="16">
         <v>0.1</v>
       </c>
-      <c r="C33" s="10" t="s">
+      <c r="C32" s="10" t="s">
         <v>55</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="6">
-    <mergeCell ref="A26:C26"/>
-    <mergeCell ref="A31:C31"/>
+    <mergeCell ref="A25:C25"/>
+    <mergeCell ref="A30:C30"/>
     <mergeCell ref="A12:C12"/>
     <mergeCell ref="A10:C10"/>
     <mergeCell ref="A6:C6"/>
-    <mergeCell ref="A22:C22"/>
+    <mergeCell ref="A21:C21"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
add: Tomi DC10-specific settings and addons, add failsafe to cluster expr heatmaps to prevent crashes when NaNs are present after scaling and cluster_rows is active
</commit_message>
<xml_diff>
--- a/settings.xlsx
+++ b/settings.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27932"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24332"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://charitede-my.sharepoint.com/personal/lev_petrov_charite_de/Documents/DOCTORATE/Cytomata/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="37" documentId="13_ncr:1_{9C262F40-B724-47DA-807B-CA0883A1DDFB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F1A53FD9-25B2-47DA-B102-657616DD89E5}"/>
+  <xr:revisionPtr revIDLastSave="6" documentId="6_{876AA531-D3F9-49D7-A1D5-6BB11379BB13}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{2548AA64-A83A-42F9-8BDE-440C2679FB5D}"/>
   <bookViews>
-    <workbookView xWindow="1260" yWindow="4872" windowWidth="28776" windowHeight="16176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2268" yWindow="2268" windowWidth="17280" windowHeight="8880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="69">
   <si>
     <t>setting</t>
   </si>
@@ -195,15 +195,9 @@
     <t>UMAPs min_dist. Lower values lead to clumpier embeddings, higher make them more spread-out. Accepts multiple values, separated by comma and whitespace (", ") of different values are needed for each data_subset. Order is given by data_subset vector.</t>
   </si>
   <si>
-    <t>Control order of groups. Input group names separated by comma and whitespace (", "). For multiple grouping columns - separate by semicolon and whitespace (", "). If you do not want to input order for any specific grouping column - write NA.</t>
-  </si>
-  <si>
     <t>0, 30</t>
   </si>
   <si>
-    <t>visit</t>
-  </si>
-  <si>
     <t>norm_mode</t>
   </si>
   <si>
@@ -213,12 +207,6 @@
     <t>percentile or harmony. Harmony is weird for now, will fix.</t>
   </si>
   <si>
-    <t>HC, S1.1, S1.2</t>
-  </si>
-  <si>
-    <t>B</t>
-  </si>
-  <si>
     <t>dc10</t>
   </si>
   <si>
@@ -226,6 +214,24 @@
   </si>
   <si>
     <t>B2M, DNA, Bead, LD, Live, Dead, ID, Cell-ID, Cell_ID, NA</t>
+  </si>
+  <si>
+    <t>group, paired_0, paired_0_5, paired_4, paired_24, paired_0_LPS, paired_0_5_LPS, paired_4_LPS, paired_24_LPS</t>
+  </si>
+  <si>
+    <t>Control order of groups. Input group names separated by comma and whitespace (", "). For multiple grouping columns - separate by semicolon and whitespace ("; "). If you do not want to input order for any specific grouping column - write NA.</t>
+  </si>
+  <si>
+    <t>DC</t>
+  </si>
+  <si>
+    <t>DC_0h, DC_0.5h, DC_4h, DC_24h, DC+LPS_0h, DC+LPS_0.5h, DC+LPS_4h, DC+LPS_24h, DC-10_0h, DC-10_0.5h, DC-10_4h, DC-10_24h, DC-10+LPS_0h, DC-10+LPS_0.5h, DC-10+LPS_4h, DC-10+LPS_24h; DC_0h, DC-10_0h; DC_0.5h, DC-10_0.5h; DC_4h, DC-10_4h; DC_24h, DC-10_24h; DC+LPS_0h, DC-10+LPS_0h; DC+LPS_0.5h, DC-10+LPS_0.5h; DC+LPS_4h, DC-10+LPS_4h; DC+LPS_24h, DC-10+LPS_24h</t>
+  </si>
+  <si>
+    <t>treat_NA_as_group</t>
+  </si>
+  <si>
+    <t>0 (off, default) or 1 (on)</t>
   </si>
 </sst>
 </file>
@@ -740,10 +746,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G32"/>
+  <dimension ref="A1:G33"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="B30" sqref="B30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -780,7 +786,7 @@
         <v>4</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="C3" s="8" t="s">
         <v>21</v>
@@ -802,7 +808,7 @@
         <v>45</v>
       </c>
       <c r="B5" s="16" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="C5" s="10" t="s">
         <v>47</v>
@@ -820,7 +826,7 @@
         <v>25</v>
       </c>
       <c r="B7" s="17">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C7" s="6" t="s">
         <v>24</v>
@@ -828,13 +834,13 @@
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" s="7" t="s">
+        <v>57</v>
+      </c>
+      <c r="B8" s="19" t="s">
+        <v>58</v>
+      </c>
+      <c r="C8" s="8" t="s">
         <v>59</v>
-      </c>
-      <c r="B8" s="19" t="s">
-        <v>60</v>
-      </c>
-      <c r="C8" s="8" t="s">
-        <v>61</v>
       </c>
     </row>
     <row r="9" spans="1:3" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
@@ -842,7 +848,7 @@
         <v>7</v>
       </c>
       <c r="B9" s="16" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="C9" s="10" t="s">
         <v>48</v>
@@ -860,7 +866,7 @@
         <v>27</v>
       </c>
       <c r="B11" s="18">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C11" s="12" t="s">
         <v>24</v>
@@ -878,7 +884,7 @@
         <v>31</v>
       </c>
       <c r="B13" s="17">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C13" s="6" t="s">
         <v>24</v>
@@ -900,196 +906,207 @@
         <v>8</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>58</v>
+        <v>63</v>
       </c>
       <c r="C15" s="8" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="16" spans="1:3" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:3" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A16" s="7" t="s">
         <v>46</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>62</v>
+        <v>66</v>
       </c>
       <c r="C16" s="8" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A17" s="7" t="s">
+        <v>67</v>
+      </c>
+      <c r="B17" s="2">
+        <v>0</v>
+      </c>
+      <c r="C17" s="8" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A18" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="B18" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="C18" s="8" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" ht="187.2" x14ac:dyDescent="0.3">
+      <c r="A19" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="B19" s="2">
+        <v>1</v>
+      </c>
+      <c r="C19" s="8" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A20" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="B20" s="2">
+        <v>100</v>
+      </c>
+      <c r="C20" s="8" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" ht="43.8" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A21" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="B21" s="16" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="17" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A17" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="B17" s="2" t="s">
-        <v>63</v>
-      </c>
-      <c r="C17" s="8" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="18" spans="1:7" ht="187.2" x14ac:dyDescent="0.3">
-      <c r="A18" s="7" t="s">
+      <c r="C21" s="10" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" ht="21.6" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A22" s="22" t="s">
+        <v>34</v>
+      </c>
+      <c r="B22" s="22"/>
+      <c r="C22" s="22"/>
+    </row>
+    <row r="23" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A23" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="B23" s="17">
+        <v>1</v>
+      </c>
+      <c r="C23" s="6" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A24" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="B24" s="2">
+        <v>1</v>
+      </c>
+      <c r="C24" s="8" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A25" s="9" t="s">
+        <v>38</v>
+      </c>
+      <c r="B25" s="16">
+        <v>0</v>
+      </c>
+      <c r="C25" s="10" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" ht="21.6" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A26" s="20" t="s">
+        <v>29</v>
+      </c>
+      <c r="B26" s="20"/>
+      <c r="C26" s="20"/>
+    </row>
+    <row r="27" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A27" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="B27" s="17" t="s">
+        <v>18</v>
+      </c>
+      <c r="C27" s="6" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" ht="86.4" x14ac:dyDescent="0.3">
+      <c r="A28" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="B28" s="2">
+        <v>20</v>
+      </c>
+      <c r="C28" s="13" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A29" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="B29" s="2">
         <v>10</v>
       </c>
-      <c r="B18" s="2">
-        <v>1</v>
-      </c>
-      <c r="C18" s="8" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="19" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A19" s="7" t="s">
-        <v>32</v>
-      </c>
-      <c r="B19" s="2">
-        <v>100</v>
-      </c>
-      <c r="C19" s="8" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="20" spans="1:7" ht="43.8" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A20" s="9" t="s">
-        <v>11</v>
-      </c>
-      <c r="B20" s="16" t="s">
-        <v>57</v>
-      </c>
-      <c r="C20" s="10" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="21" spans="1:7" ht="21.6" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A21" s="22" t="s">
-        <v>34</v>
-      </c>
-      <c r="B21" s="22"/>
-      <c r="C21" s="22"/>
-    </row>
-    <row r="22" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A22" s="5" t="s">
-        <v>35</v>
-      </c>
-      <c r="B22" s="17">
-        <v>1</v>
-      </c>
-      <c r="C22" s="6" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="23" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A23" s="7" t="s">
-        <v>36</v>
-      </c>
-      <c r="B23" s="2">
-        <v>1</v>
-      </c>
-      <c r="C23" s="8" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="24" spans="1:7" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A24" s="9" t="s">
-        <v>38</v>
-      </c>
-      <c r="B24" s="16">
-        <v>0</v>
-      </c>
-      <c r="C24" s="10" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="25" spans="1:7" ht="21.6" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A25" s="20" t="s">
-        <v>29</v>
-      </c>
-      <c r="B25" s="20"/>
-      <c r="C25" s="20"/>
-    </row>
-    <row r="26" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A26" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="B26" s="17" t="s">
-        <v>18</v>
-      </c>
-      <c r="C26" s="6" t="s">
+      <c r="C29" s="13" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" ht="58.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A30" s="9" t="s">
+        <v>43</v>
+      </c>
+      <c r="B30" s="16">
+        <v>2.5000000000000001E-2</v>
+      </c>
+      <c r="C30" s="14" t="s">
+        <v>44</v>
+      </c>
+      <c r="G30" s="15"/>
+    </row>
+    <row r="31" spans="1:7" ht="21.6" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A31" s="21" t="s">
+        <v>30</v>
+      </c>
+      <c r="B31" s="21"/>
+      <c r="C31" s="21"/>
+    </row>
+    <row r="32" spans="1:7" ht="72" x14ac:dyDescent="0.3">
+      <c r="A32" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="B32" s="17">
         <v>20</v>
       </c>
-    </row>
-    <row r="27" spans="1:7" ht="86.4" x14ac:dyDescent="0.3">
-      <c r="A27" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="B27" s="2">
-        <v>30</v>
-      </c>
-      <c r="C27" s="13" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="28" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A28" s="7" t="s">
-        <v>41</v>
-      </c>
-      <c r="B28" s="2">
-        <v>10</v>
-      </c>
-      <c r="C28" s="13" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="29" spans="1:7" ht="58.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A29" s="9" t="s">
-        <v>43</v>
-      </c>
-      <c r="B29" s="16">
-        <v>7.0000000000000001E-3</v>
-      </c>
-      <c r="C29" s="14" t="s">
-        <v>44</v>
-      </c>
-      <c r="G29" s="15"/>
-    </row>
-    <row r="30" spans="1:7" ht="21.6" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A30" s="21" t="s">
-        <v>30</v>
-      </c>
-      <c r="B30" s="21"/>
-      <c r="C30" s="21"/>
-    </row>
-    <row r="31" spans="1:7" ht="72" x14ac:dyDescent="0.3">
-      <c r="A31" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="B31" s="17">
+      <c r="C32" s="6" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" ht="58.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A33" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="C31" s="6" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="32" spans="1:7" ht="58.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A32" s="9" t="s">
-        <v>15</v>
-      </c>
-      <c r="B32" s="16">
-        <v>0.1</v>
-      </c>
-      <c r="C32" s="10" t="s">
+      <c r="B33" s="16">
+        <v>0.15</v>
+      </c>
+      <c r="C33" s="10" t="s">
         <v>55</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="6">
-    <mergeCell ref="A25:C25"/>
-    <mergeCell ref="A30:C30"/>
+    <mergeCell ref="A26:C26"/>
+    <mergeCell ref="A31:C31"/>
     <mergeCell ref="A12:C12"/>
     <mergeCell ref="A10:C10"/>
     <mergeCell ref="A6:C6"/>
-    <mergeCell ref="A21:C21"/>
+    <mergeCell ref="A22:C22"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
add: ungroup before rstatix pairwise testing that fixes map() error for some reason
</commit_message>
<xml_diff>
--- a/settings.xlsx
+++ b/settings.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://charitede-my.sharepoint.com/personal/lev_petrov_charite_de/Documents/DOCTORATE/Cytomata/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="6" documentId="6_{876AA531-D3F9-49D7-A1D5-6BB11379BB13}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{2548AA64-A83A-42F9-8BDE-440C2679FB5D}"/>
+  <xr:revisionPtr revIDLastSave="10" documentId="6_{876AA531-D3F9-49D7-A1D5-6BB11379BB13}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{25807F88-EDEF-40CC-902B-B0A2B0B17303}"/>
   <bookViews>
-    <workbookView xWindow="2268" yWindow="2268" windowWidth="17280" windowHeight="8880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2616" yWindow="2616" windowWidth="17280" windowHeight="8880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -225,13 +225,13 @@
     <t>DC</t>
   </si>
   <si>
-    <t>DC_0h, DC_0.5h, DC_4h, DC_24h, DC+LPS_0h, DC+LPS_0.5h, DC+LPS_4h, DC+LPS_24h, DC-10_0h, DC-10_0.5h, DC-10_4h, DC-10_24h, DC-10+LPS_0h, DC-10+LPS_0.5h, DC-10+LPS_4h, DC-10+LPS_24h; DC_0h, DC-10_0h; DC_0.5h, DC-10_0.5h; DC_4h, DC-10_4h; DC_24h, DC-10_24h; DC+LPS_0h, DC-10+LPS_0h; DC+LPS_0.5h, DC-10+LPS_0.5h; DC+LPS_4h, DC-10+LPS_4h; DC+LPS_24h, DC-10+LPS_24h</t>
-  </si>
-  <si>
     <t>treat_NA_as_group</t>
   </si>
   <si>
     <t>0 (off, default) or 1 (on)</t>
+  </si>
+  <si>
+    <t>DC_0h, DC_0_5h, DC_4h, DC_24h, DC_LPS_0h, DC_LPS_0_5h, DC_LPS_4h, DC_LPS_24h, DC10_0h, DC10_0_5h, DC10_4h, DC10_24h, DC10_LPS_0h, DC10_LPS_0_5h, DC10_LPS_4h, DC10_LPS_24h; DC_0h, DC10_0h; DC_0_5h, DC10_0_5h; DC_4h, DC10_4h; DC_24h, DC10_24h; DC_LPS_0h, DC10_LPS_0h; DC_LPS_0_5h, DC10_LPS_0_5h; DC_LPS_4h, DC10_LPS_4h; DC_LPS_24h, DC10_LPS_24h</t>
   </si>
 </sst>
 </file>
@@ -748,8 +748,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G33"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="B30" sqref="B30"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -917,7 +917,7 @@
         <v>46</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="C16" s="8" t="s">
         <v>64</v>
@@ -925,13 +925,13 @@
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A17" s="7" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B17" s="2">
         <v>0</v>
       </c>
       <c r="C17" s="8" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="18" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
add: settings update upon reclustering
</commit_message>
<xml_diff>
--- a/settings.xlsx
+++ b/settings.xlsx
@@ -8,17 +8,26 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://charitede-my.sharepoint.com/personal/lev_petrov_charite_de/Documents/DOCTORATE/Cytomata/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="10" documentId="6_{876AA531-D3F9-49D7-A1D5-6BB11379BB13}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{25807F88-EDEF-40CC-902B-B0A2B0B17303}"/>
+  <xr:revisionPtr revIDLastSave="73" documentId="13_ncr:1_{9C262F40-B724-47DA-807B-CA0883A1DDFB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{AAF093B7-5D07-41EB-94A6-E26478FE079F}"/>
   <bookViews>
-    <workbookView xWindow="2616" yWindow="2616" windowWidth="17280" windowHeight="8880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -207,22 +216,22 @@
     <t>percentile or harmony. Harmony is weird for now, will fix.</t>
   </si>
   <si>
-    <t>dc10</t>
-  </si>
-  <si>
-    <t>Anchor</t>
-  </si>
-  <si>
     <t>B2M, DNA, Bead, LD, Live, Dead, ID, Cell-ID, Cell_ID, NA</t>
   </si>
   <si>
-    <t>group, paired_0, paired_0_5, paired_4, paired_24, paired_0_LPS, paired_0_5_LPS, paired_4_LPS, paired_24_LPS</t>
+    <t>iacs_panel_1</t>
+  </si>
+  <si>
+    <t>HC-04</t>
   </si>
   <si>
     <t>Control order of groups. Input group names separated by comma and whitespace (", "). For multiple grouping columns - separate by semicolon and whitespace ("; "). If you do not want to input order for any specific grouping column - write NA.</t>
   </si>
   <si>
-    <t>DC</t>
+    <t>hc_vs_pc_pre_treat, responder_pre_treat, pre_post, pre_post_w_hc</t>
+  </si>
+  <si>
+    <t>HC, S1.1; yes, no; S1.1, S1.2; HC, S1.1, S1.2</t>
   </si>
   <si>
     <t>treat_NA_as_group</t>
@@ -231,7 +240,7 @@
     <t>0 (off, default) or 1 (on)</t>
   </si>
   <si>
-    <t>DC_0h, DC_0_5h, DC_4h, DC_24h, DC_LPS_0h, DC_LPS_0_5h, DC_LPS_4h, DC_LPS_24h, DC10_0h, DC10_0_5h, DC10_4h, DC10_24h, DC10_LPS_0h, DC10_LPS_0_5h, DC10_LPS_4h, DC10_LPS_24h; DC_0h, DC10_0h; DC_0_5h, DC10_0_5h; DC_4h, DC10_4h; DC_24h, DC10_24h; DC_LPS_0h, DC10_LPS_0h; DC_LPS_0_5h, DC10_LPS_0_5h; DC_LPS_4h, DC10_LPS_4h; DC_LPS_24h, DC10_LPS_24h</t>
+    <t>B</t>
   </si>
 </sst>
 </file>
@@ -748,8 +757,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G33"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="B16" sqref="B16"/>
+    <sheetView tabSelected="1" topLeftCell="A24" workbookViewId="0">
+      <selection activeCell="B30" sqref="B30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -786,7 +795,7 @@
         <v>4</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="C3" s="8" t="s">
         <v>21</v>
@@ -808,7 +817,7 @@
         <v>45</v>
       </c>
       <c r="B5" s="16" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="C5" s="10" t="s">
         <v>47</v>
@@ -848,7 +857,7 @@
         <v>7</v>
       </c>
       <c r="B9" s="16" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="C9" s="10" t="s">
         <v>48</v>
@@ -906,21 +915,21 @@
         <v>8</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="C15" s="8" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="16" spans="1:3" ht="86.4" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:3" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A16" s="7" t="s">
         <v>46</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="C16" s="8" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.3">
@@ -939,7 +948,7 @@
         <v>9</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>65</v>
+        <v>68</v>
       </c>
       <c r="C18" s="8" t="s">
         <v>50</v>
@@ -1041,7 +1050,7 @@
         <v>13</v>
       </c>
       <c r="B28" s="2">
-        <v>20</v>
+        <v>30</v>
       </c>
       <c r="C28" s="13" t="s">
         <v>53</v>
@@ -1063,7 +1072,7 @@
         <v>43</v>
       </c>
       <c r="B30" s="16">
-        <v>2.5000000000000001E-2</v>
+        <v>5.0000000000000001E-3</v>
       </c>
       <c r="C30" s="14" t="s">
         <v>44</v>
@@ -1082,7 +1091,7 @@
         <v>14</v>
       </c>
       <c r="B32" s="17">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="C32" s="6" t="s">
         <v>54</v>
@@ -1093,7 +1102,7 @@
         <v>15</v>
       </c>
       <c r="B33" s="16">
-        <v>0.15</v>
+        <v>0.1</v>
       </c>
       <c r="C33" s="10" t="s">
         <v>55</v>

</xml_diff>

<commit_message>
chore: small fix for nonparametric var=0 testing case
</commit_message>
<xml_diff>
--- a/settings.xlsx
+++ b/settings.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://charitede-my.sharepoint.com/personal/lev_petrov_charite_de/Documents/DOCTORATE/Cytomata/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="73" documentId="13_ncr:1_{9C262F40-B724-47DA-807B-CA0883A1DDFB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{AAF093B7-5D07-41EB-94A6-E26478FE079F}"/>
+  <xr:revisionPtr revIDLastSave="78" documentId="13_ncr:1_{9C262F40-B724-47DA-807B-CA0883A1DDFB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{29FD777F-84A0-4251-87FE-47706A5253AC}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -757,8 +757,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G33"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A24" workbookViewId="0">
-      <selection activeCell="B30" sqref="B30"/>
+    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="B29" sqref="B29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1072,7 +1072,7 @@
         <v>43</v>
       </c>
       <c r="B30" s="16">
-        <v>5.0000000000000001E-3</v>
+        <v>5.4999999999999997E-3</v>
       </c>
       <c r="C30" s="14" t="s">
         <v>44</v>

</xml_diff>

<commit_message>
- change: switch all testing to parametric - add: missing collector$p.adj.signif to parametric testing
</commit_message>
<xml_diff>
--- a/settings.xlsx
+++ b/settings.xlsx
@@ -8,26 +8,17 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://charitede-my.sharepoint.com/personal/lev_petrov_charite_de/Documents/DOCTORATE/Cytomata/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="78" documentId="13_ncr:1_{9C262F40-B724-47DA-807B-CA0883A1DDFB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{29FD777F-84A0-4251-87FE-47706A5253AC}"/>
+  <xr:revisionPtr revIDLastSave="10" documentId="6_{876AA531-D3F9-49D7-A1D5-6BB11379BB13}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{25807F88-EDEF-40CC-902B-B0A2B0B17303}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2616" yWindow="2616" windowWidth="17280" windowHeight="8880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -216,22 +207,22 @@
     <t>percentile or harmony. Harmony is weird for now, will fix.</t>
   </si>
   <si>
+    <t>dc10</t>
+  </si>
+  <si>
+    <t>Anchor</t>
+  </si>
+  <si>
     <t>B2M, DNA, Bead, LD, Live, Dead, ID, Cell-ID, Cell_ID, NA</t>
   </si>
   <si>
-    <t>iacs_panel_1</t>
-  </si>
-  <si>
-    <t>HC-04</t>
+    <t>group, paired_0, paired_0_5, paired_4, paired_24, paired_0_LPS, paired_0_5_LPS, paired_4_LPS, paired_24_LPS</t>
   </si>
   <si>
     <t>Control order of groups. Input group names separated by comma and whitespace (", "). For multiple grouping columns - separate by semicolon and whitespace ("; "). If you do not want to input order for any specific grouping column - write NA.</t>
   </si>
   <si>
-    <t>hc_vs_pc_pre_treat, responder_pre_treat, pre_post, pre_post_w_hc</t>
-  </si>
-  <si>
-    <t>HC, S1.1; yes, no; S1.1, S1.2; HC, S1.1, S1.2</t>
+    <t>DC</t>
   </si>
   <si>
     <t>treat_NA_as_group</t>
@@ -240,7 +231,7 @@
     <t>0 (off, default) or 1 (on)</t>
   </si>
   <si>
-    <t>B</t>
+    <t>DC_0h, DC_0_5h, DC_4h, DC_24h, DC_LPS_0h, DC_LPS_0_5h, DC_LPS_4h, DC_LPS_24h, DC10_0h, DC10_0_5h, DC10_4h, DC10_24h, DC10_LPS_0h, DC10_LPS_0_5h, DC10_LPS_4h, DC10_LPS_24h; DC_0h, DC10_0h; DC_0_5h, DC10_0_5h; DC_4h, DC10_4h; DC_24h, DC10_24h; DC_LPS_0h, DC10_LPS_0h; DC_LPS_0_5h, DC10_LPS_0_5h; DC_LPS_4h, DC10_LPS_4h; DC_LPS_24h, DC10_LPS_24h</t>
   </si>
 </sst>
 </file>
@@ -757,8 +748,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G33"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="B29" sqref="B29"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -795,7 +786,7 @@
         <v>4</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C3" s="8" t="s">
         <v>21</v>
@@ -817,7 +808,7 @@
         <v>45</v>
       </c>
       <c r="B5" s="16" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="C5" s="10" t="s">
         <v>47</v>
@@ -857,7 +848,7 @@
         <v>7</v>
       </c>
       <c r="B9" s="16" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C9" s="10" t="s">
         <v>48</v>
@@ -915,21 +906,21 @@
         <v>8</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C15" s="8" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="16" spans="1:3" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:3" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A16" s="7" t="s">
         <v>46</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>65</v>
+        <v>68</v>
       </c>
       <c r="C16" s="8" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.3">
@@ -948,7 +939,7 @@
         <v>9</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="C18" s="8" t="s">
         <v>50</v>
@@ -1050,7 +1041,7 @@
         <v>13</v>
       </c>
       <c r="B28" s="2">
-        <v>30</v>
+        <v>20</v>
       </c>
       <c r="C28" s="13" t="s">
         <v>53</v>
@@ -1072,7 +1063,7 @@
         <v>43</v>
       </c>
       <c r="B30" s="16">
-        <v>5.4999999999999997E-3</v>
+        <v>2.5000000000000001E-2</v>
       </c>
       <c r="C30" s="14" t="s">
         <v>44</v>
@@ -1091,7 +1082,7 @@
         <v>14</v>
       </c>
       <c r="B32" s="17">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="C32" s="6" t="s">
         <v>54</v>
@@ -1102,7 +1093,7 @@
         <v>15</v>
       </c>
       <c r="B33" s="16">
-        <v>0.1</v>
+        <v>0.15</v>
       </c>
       <c r="C33" s="10" t="s">
         <v>55</v>

</xml_diff>

<commit_message>
feat: non-tested quantile normalization sketch
</commit_message>
<xml_diff>
--- a/settings.xlsx
+++ b/settings.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24332"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27932"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://charitede-my.sharepoint.com/personal/lev_petrov_charite_de/Documents/DOCTORATE/Cytomata/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://charitede-my.sharepoint.com/personal/lev_petrov_charite_de/Documents/DOCTORATE/Cytomata_data/iahp_panel_3/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="10" documentId="6_{876AA531-D3F9-49D7-A1D5-6BB11379BB13}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{25807F88-EDEF-40CC-902B-B0A2B0B17303}"/>
+  <xr:revisionPtr revIDLastSave="33" documentId="13_ncr:1_{9C262F40-B724-47DA-807B-CA0883A1DDFB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B2C91C02-028E-46F2-8FA0-FD0663B1047F}"/>
   <bookViews>
-    <workbookView xWindow="2616" yWindow="2616" windowWidth="17280" windowHeight="8880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="16416" yWindow="3720" windowWidth="29016" windowHeight="15288" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="67">
   <si>
     <t>setting</t>
   </si>
@@ -165,9 +165,15 @@
     <t>excluded_channels</t>
   </si>
   <si>
+    <t>B2M, DNA, Bead, LD, Live, Dead, ID, Cell-ID, Cell_ID</t>
+  </si>
+  <si>
     <t>grouping_orders</t>
   </si>
   <si>
+    <t>HC-050</t>
+  </si>
+  <si>
     <t>Patterns present in the names of pre-processing channels that will be used to remove them. Input separated by comma and whitespace (", "). This can be adjusted in the panel.csv file afterwards.</t>
   </si>
   <si>
@@ -198,40 +204,28 @@
     <t>0, 30</t>
   </si>
   <si>
+    <t>iahp_panel_3</t>
+  </si>
+  <si>
+    <t>percentile</t>
+  </si>
+  <si>
+    <t>percentile or harmony (harmony looks weird, will fix)</t>
+  </si>
+  <si>
     <t>norm_mode</t>
   </si>
   <si>
-    <t>percentile</t>
-  </si>
-  <si>
-    <t>percentile or harmony. Harmony is weird for now, will fix.</t>
-  </si>
-  <si>
-    <t>dc10</t>
-  </si>
-  <si>
-    <t>Anchor</t>
-  </si>
-  <si>
-    <t>B2M, DNA, Bead, LD, Live, Dead, ID, Cell-ID, Cell_ID, NA</t>
-  </si>
-  <si>
-    <t>group, paired_0, paired_0_5, paired_4, paired_24, paired_0_LPS, paired_0_5_LPS, paired_4_LPS, paired_24_LPS</t>
+    <t>Monos_and_DCs, CD4_T, CD8_T, B, TCRgd_T, NK</t>
+  </si>
+  <si>
+    <t>visit, hc_pre, hc_post, pre_post</t>
+  </si>
+  <si>
+    <t>HC, S1.1, S1.2; HC, S1.1; HC, S1.2; S1.1, S1.2</t>
   </si>
   <si>
     <t>Control order of groups. Input group names separated by comma and whitespace (", "). For multiple grouping columns - separate by semicolon and whitespace ("; "). If you do not want to input order for any specific grouping column - write NA.</t>
-  </si>
-  <si>
-    <t>DC</t>
-  </si>
-  <si>
-    <t>treat_NA_as_group</t>
-  </si>
-  <si>
-    <t>0 (off, default) or 1 (on)</t>
-  </si>
-  <si>
-    <t>DC_0h, DC_0_5h, DC_4h, DC_24h, DC_LPS_0h, DC_LPS_0_5h, DC_LPS_4h, DC_LPS_24h, DC10_0h, DC10_0_5h, DC10_4h, DC10_24h, DC10_LPS_0h, DC10_LPS_0_5h, DC10_LPS_4h, DC10_LPS_24h; DC_0h, DC10_0h; DC_0_5h, DC10_0_5h; DC_4h, DC10_4h; DC_24h, DC10_24h; DC_LPS_0h, DC10_LPS_0h; DC_LPS_0_5h, DC10_LPS_0_5h; DC_LPS_4h, DC10_LPS_4h; DC_LPS_24h, DC10_LPS_24h</t>
   </si>
 </sst>
 </file>
@@ -746,10 +740,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G33"/>
+  <dimension ref="A1:G32"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="B16" sqref="B16"/>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="F16" sqref="F16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -786,7 +780,7 @@
         <v>4</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C3" s="8" t="s">
         <v>21</v>
@@ -808,10 +802,10 @@
         <v>45</v>
       </c>
       <c r="B5" s="16" t="s">
-        <v>62</v>
+        <v>46</v>
       </c>
       <c r="C5" s="10" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
     </row>
     <row r="6" spans="1:3" ht="21.6" thickBot="1" x14ac:dyDescent="0.35">
@@ -826,7 +820,7 @@
         <v>25</v>
       </c>
       <c r="B7" s="17">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C7" s="6" t="s">
         <v>24</v>
@@ -834,13 +828,13 @@
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" s="7" t="s">
-        <v>57</v>
+        <v>62</v>
       </c>
       <c r="B8" s="19" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="C8" s="8" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
     </row>
     <row r="9" spans="1:3" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
@@ -848,10 +842,10 @@
         <v>7</v>
       </c>
       <c r="B9" s="16" t="s">
-        <v>61</v>
+        <v>48</v>
       </c>
       <c r="C9" s="10" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
     </row>
     <row r="10" spans="1:3" ht="21.6" thickBot="1" x14ac:dyDescent="0.35">
@@ -866,7 +860,7 @@
         <v>27</v>
       </c>
       <c r="B11" s="18">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C11" s="12" t="s">
         <v>24</v>
@@ -884,7 +878,7 @@
         <v>31</v>
       </c>
       <c r="B13" s="17">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C13" s="6" t="s">
         <v>24</v>
@@ -906,207 +900,196 @@
         <v>8</v>
       </c>
       <c r="B15" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="C15" s="8" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A16" s="7" t="s">
+        <v>47</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="C16" s="8" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A17" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="B17" s="2" t="s">
         <v>63</v>
       </c>
-      <c r="C15" s="8" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" ht="86.4" x14ac:dyDescent="0.3">
-      <c r="A16" s="7" t="s">
-        <v>46</v>
-      </c>
-      <c r="B16" s="2" t="s">
-        <v>68</v>
-      </c>
-      <c r="C16" s="8" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A17" s="7" t="s">
-        <v>66</v>
-      </c>
-      <c r="B17" s="2">
+      <c r="C17" s="8" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" ht="187.2" x14ac:dyDescent="0.3">
+      <c r="A18" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="B18" s="2">
+        <v>1</v>
+      </c>
+      <c r="C18" s="8" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A19" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="B19" s="2">
+        <v>100</v>
+      </c>
+      <c r="C19" s="8" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" ht="43.8" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A20" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="B20" s="16" t="s">
+        <v>58</v>
+      </c>
+      <c r="C20" s="10" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" ht="21.6" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A21" s="22" t="s">
+        <v>34</v>
+      </c>
+      <c r="B21" s="22"/>
+      <c r="C21" s="22"/>
+    </row>
+    <row r="22" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A22" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="B22" s="17">
+        <v>1</v>
+      </c>
+      <c r="C22" s="6" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A23" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="B23" s="2">
+        <v>1</v>
+      </c>
+      <c r="C23" s="8" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A24" s="9" t="s">
+        <v>38</v>
+      </c>
+      <c r="B24" s="16">
         <v>0</v>
       </c>
-      <c r="C17" s="8" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="18" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A18" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="B18" s="2" t="s">
-        <v>65</v>
-      </c>
-      <c r="C18" s="8" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="19" spans="1:7" ht="187.2" x14ac:dyDescent="0.3">
-      <c r="A19" s="7" t="s">
+      <c r="C24" s="10" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" ht="21.6" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A25" s="20" t="s">
+        <v>29</v>
+      </c>
+      <c r="B25" s="20"/>
+      <c r="C25" s="20"/>
+    </row>
+    <row r="26" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A26" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="B26" s="17" t="s">
+        <v>18</v>
+      </c>
+      <c r="C26" s="6" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" ht="86.4" x14ac:dyDescent="0.3">
+      <c r="A27" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="B27" s="2">
+        <v>30</v>
+      </c>
+      <c r="C27" s="13" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A28" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="B28" s="2">
         <v>10</v>
       </c>
-      <c r="B19" s="2">
-        <v>1</v>
-      </c>
-      <c r="C19" s="8" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="20" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A20" s="7" t="s">
-        <v>32</v>
-      </c>
-      <c r="B20" s="2">
-        <v>100</v>
-      </c>
-      <c r="C20" s="8" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="21" spans="1:7" ht="43.8" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A21" s="9" t="s">
-        <v>11</v>
-      </c>
-      <c r="B21" s="16" t="s">
+      <c r="C28" s="13" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" ht="58.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A29" s="9" t="s">
+        <v>43</v>
+      </c>
+      <c r="B29" s="16">
+        <v>7.0000000000000001E-3</v>
+      </c>
+      <c r="C29" s="14" t="s">
+        <v>44</v>
+      </c>
+      <c r="G29" s="15"/>
+    </row>
+    <row r="30" spans="1:7" ht="21.6" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A30" s="21" t="s">
+        <v>30</v>
+      </c>
+      <c r="B30" s="21"/>
+      <c r="C30" s="21"/>
+    </row>
+    <row r="31" spans="1:7" ht="72" x14ac:dyDescent="0.3">
+      <c r="A31" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="B31" s="17">
+        <v>15</v>
+      </c>
+      <c r="C31" s="6" t="s">
         <v>56</v>
       </c>
-      <c r="C21" s="10" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="22" spans="1:7" ht="21.6" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A22" s="22" t="s">
-        <v>34</v>
-      </c>
-      <c r="B22" s="22"/>
-      <c r="C22" s="22"/>
-    </row>
-    <row r="23" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A23" s="5" t="s">
-        <v>35</v>
-      </c>
-      <c r="B23" s="17">
-        <v>1</v>
-      </c>
-      <c r="C23" s="6" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="24" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A24" s="7" t="s">
-        <v>36</v>
-      </c>
-      <c r="B24" s="2">
-        <v>1</v>
-      </c>
-      <c r="C24" s="8" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="25" spans="1:7" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A25" s="9" t="s">
-        <v>38</v>
-      </c>
-      <c r="B25" s="16">
-        <v>0</v>
-      </c>
-      <c r="C25" s="10" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="26" spans="1:7" ht="21.6" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A26" s="20" t="s">
-        <v>29</v>
-      </c>
-      <c r="B26" s="20"/>
-      <c r="C26" s="20"/>
-    </row>
-    <row r="27" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A27" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="B27" s="17" t="s">
-        <v>18</v>
-      </c>
-      <c r="C27" s="6" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="28" spans="1:7" ht="86.4" x14ac:dyDescent="0.3">
-      <c r="A28" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="B28" s="2">
-        <v>20</v>
-      </c>
-      <c r="C28" s="13" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="29" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A29" s="7" t="s">
-        <v>41</v>
-      </c>
-      <c r="B29" s="2">
-        <v>10</v>
-      </c>
-      <c r="C29" s="13" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="30" spans="1:7" ht="58.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A30" s="9" t="s">
-        <v>43</v>
-      </c>
-      <c r="B30" s="16">
-        <v>2.5000000000000001E-2</v>
-      </c>
-      <c r="C30" s="14" t="s">
-        <v>44</v>
-      </c>
-      <c r="G30" s="15"/>
-    </row>
-    <row r="31" spans="1:7" ht="21.6" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A31" s="21" t="s">
-        <v>30</v>
-      </c>
-      <c r="B31" s="21"/>
-      <c r="C31" s="21"/>
-    </row>
-    <row r="32" spans="1:7" ht="72" x14ac:dyDescent="0.3">
-      <c r="A32" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="B32" s="17">
-        <v>20</v>
-      </c>
-      <c r="C32" s="6" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="33" spans="1:3" ht="58.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A33" s="9" t="s">
+    </row>
+    <row r="32" spans="1:7" ht="58.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A32" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="B33" s="16">
-        <v>0.15</v>
-      </c>
-      <c r="C33" s="10" t="s">
-        <v>55</v>
+      <c r="B32" s="16">
+        <v>0.1</v>
+      </c>
+      <c r="C32" s="10" t="s">
+        <v>57</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="6">
-    <mergeCell ref="A26:C26"/>
-    <mergeCell ref="A31:C31"/>
+    <mergeCell ref="A25:C25"/>
+    <mergeCell ref="A30:C30"/>
     <mergeCell ref="A12:C12"/>
     <mergeCell ref="A10:C10"/>
     <mergeCell ref="A6:C6"/>
-    <mergeCell ref="A22:C22"/>
+    <mergeCell ref="A21:C21"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
add: optional marker heatmap ordering for DC project, increase text scaling change: dim reduction plots width and text scaling now changes based on n groups represented
</commit_message>
<xml_diff>
--- a/settings.xlsx
+++ b/settings.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://charitede-my.sharepoint.com/personal/lev_petrov_charite_de/Documents/DOCTORATE/Cytomata/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="86" documentId="13_ncr:1_{9C262F40-B724-47DA-807B-CA0883A1DDFB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{497731B2-7695-4D9C-B51E-4C30D81B17B8}"/>
+  <xr:revisionPtr revIDLastSave="10" documentId="6_{876AA531-D3F9-49D7-A1D5-6BB11379BB13}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{25807F88-EDEF-40CC-902B-B0A2B0B17303}"/>
   <bookViews>
-    <workbookView xWindow="3036" yWindow="3036" windowWidth="17280" windowHeight="8880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2616" yWindow="2616" windowWidth="17280" windowHeight="8880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="76">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="69">
   <si>
     <t>setting</t>
   </si>
@@ -165,15 +165,9 @@
     <t>excluded_channels</t>
   </si>
   <si>
-    <t>B2M, DNA, Bead, LD, Live, Dead, ID, Cell-ID, Cell_ID</t>
-  </si>
-  <si>
     <t>grouping_orders</t>
   </si>
   <si>
-    <t>HC-050</t>
-  </si>
-  <si>
     <t>Patterns present in the names of pre-processing channels that will be used to remove them. Input separated by comma and whitespace (", "). This can be adjusted in the panel.csv file afterwards.</t>
   </si>
   <si>
@@ -207,52 +201,37 @@
     <t>norm_mode</t>
   </si>
   <si>
+    <t>percentile</t>
+  </si>
+  <si>
+    <t>percentile or harmony. Harmony is weird for now, will fix.</t>
+  </si>
+  <si>
+    <t>dc10</t>
+  </si>
+  <si>
+    <t>Anchor</t>
+  </si>
+  <si>
+    <t>B2M, DNA, Bead, LD, Live, Dead, ID, Cell-ID, Cell_ID, NA</t>
+  </si>
+  <si>
+    <t>group, paired_0, paired_0_5, paired_4, paired_24, paired_0_LPS, paired_0_5_LPS, paired_4_LPS, paired_24_LPS</t>
+  </si>
+  <si>
     <t>Control order of groups. Input group names separated by comma and whitespace (", "). For multiple grouping columns - separate by semicolon and whitespace ("; "). If you do not want to input order for any specific grouping column - write NA.</t>
   </si>
   <si>
-    <t>visit, hc_pre, hc_post, pre_post</t>
-  </si>
-  <si>
-    <t>HC, S1.1, S1.2; HC, S1.1; HC, S1.2; S1.1, S1.2</t>
-  </si>
-  <si>
-    <t>B, CD4_T, CD8_T, Monos_and_DCs, NK, TCRgd_T</t>
-  </si>
-  <si>
-    <t>iahp_panel_1_quantile</t>
-  </si>
-  <si>
-    <t>quantile</t>
-  </si>
-  <si>
-    <t>norm_method</t>
-  </si>
-  <si>
-    <t>If quantile mode, can be either sample or channel. sample calculates n_quantiles for each channel and sample and then takes the average for each quantile over all samples to form a target distribution. channel calculates n_quantiles over all events in all reference samples for a given channel to form a target distribution. sample option is much slower, but more traditional.</t>
-  </si>
-  <si>
-    <t>norm_n_quantiles</t>
-  </si>
-  <si>
-    <t>norm_hide_zeroes</t>
-  </si>
-  <si>
-    <t>0 or 1. whether to produce additional density ridges with 0 values hidden for better visibility.</t>
-  </si>
-  <si>
-    <t>norm_ridges_downsampling</t>
-  </si>
-  <si>
-    <t>between 0 and 1. downsampling factor for density ridge plots. Use to speedup compute time.</t>
-  </si>
-  <si>
-    <t>percentile, quantile or harmony. Percentile does linear scaling using automatically estimated optimal anchor sample and optimal percentile for each channel. Quantile maps a spline interpolation function for each batch and adjusts all NON-ZERO values using the spline. NON-ZERO part is important. Harmony is weird for now, will fix at some point.</t>
-  </si>
-  <si>
-    <t>channel</t>
-  </si>
-  <si>
-    <t>how many quantiles to compute (+1). Tested: 100, 10000, 100000. No major difference spotted. Influences runtime by A LOT</t>
+    <t>DC</t>
+  </si>
+  <si>
+    <t>treat_NA_as_group</t>
+  </si>
+  <si>
+    <t>0 (off, default) or 1 (on)</t>
+  </si>
+  <si>
+    <t>DC_0h, DC_0_5h, DC_4h, DC_24h, DC_LPS_0h, DC_LPS_0_5h, DC_LPS_4h, DC_LPS_24h, DC10_0h, DC10_0_5h, DC10_4h, DC10_24h, DC10_LPS_0h, DC10_LPS_0_5h, DC10_LPS_4h, DC10_LPS_24h; DC_0h, DC10_0h; DC_0_5h, DC10_0_5h; DC_4h, DC10_4h; DC_24h, DC10_24h; DC_LPS_0h, DC10_LPS_0h; DC_LPS_0_5h, DC10_LPS_0_5h; DC_LPS_4h, DC10_LPS_4h; DC_LPS_24h, DC10_LPS_24h</t>
   </si>
 </sst>
 </file>
@@ -767,15 +746,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G36"/>
+  <dimension ref="A1:G33"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="24.44140625" style="1" customWidth="1"/>
+    <col min="1" max="1" width="23.109375" style="1" customWidth="1"/>
     <col min="2" max="2" width="71.33203125" style="2" customWidth="1"/>
     <col min="3" max="3" width="59" style="2" customWidth="1"/>
   </cols>
@@ -807,7 +786,7 @@
         <v>4</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="C3" s="8" t="s">
         <v>21</v>
@@ -829,10 +808,10 @@
         <v>45</v>
       </c>
       <c r="B5" s="16" t="s">
-        <v>46</v>
+        <v>62</v>
       </c>
       <c r="C5" s="10" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
     </row>
     <row r="6" spans="1:3" ht="21.6" thickBot="1" x14ac:dyDescent="0.35">
@@ -847,320 +826,287 @@
         <v>25</v>
       </c>
       <c r="B7" s="17">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C7" s="6" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="8" spans="1:3" ht="86.4" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" s="7" t="s">
+        <v>57</v>
+      </c>
+      <c r="B8" s="19" t="s">
+        <v>58</v>
+      </c>
+      <c r="C8" s="8" t="s">
         <v>59</v>
       </c>
-      <c r="B8" s="19" t="s">
+    </row>
+    <row r="9" spans="1:3" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A9" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="B9" s="16" t="s">
+        <v>61</v>
+      </c>
+      <c r="C9" s="10" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" ht="21.6" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A10" s="21" t="s">
+        <v>26</v>
+      </c>
+      <c r="B10" s="21"/>
+      <c r="C10" s="21"/>
+    </row>
+    <row r="11" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A11" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="B11" s="18">
+        <v>0</v>
+      </c>
+      <c r="C11" s="12" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" ht="21.6" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A12" s="21" t="s">
+        <v>28</v>
+      </c>
+      <c r="B12" s="21"/>
+      <c r="C12" s="21"/>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A13" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="B13" s="17">
+        <v>1</v>
+      </c>
+      <c r="C13" s="6" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A14" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="B14" s="2">
+        <v>1</v>
+      </c>
+      <c r="C14" s="8" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A15" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="C15" s="8" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" ht="86.4" x14ac:dyDescent="0.3">
+      <c r="A16" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="C16" s="8" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A17" s="7" t="s">
+        <v>66</v>
+      </c>
+      <c r="B17" s="2">
+        <v>0</v>
+      </c>
+      <c r="C17" s="8" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A18" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="B18" s="2" t="s">
         <v>65</v>
       </c>
-      <c r="C8" s="8" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A9" s="7" t="s">
-        <v>7</v>
-      </c>
-      <c r="B9" s="19" t="s">
-        <v>48</v>
-      </c>
-      <c r="C9" s="8" t="s">
+      <c r="C18" s="8" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="10" spans="1:3" ht="86.4" x14ac:dyDescent="0.3">
-      <c r="A10" s="7" t="s">
-        <v>66</v>
-      </c>
-      <c r="B10" s="19" t="s">
-        <v>74</v>
-      </c>
-      <c r="C10" s="8" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A11" s="7" t="s">
-        <v>68</v>
-      </c>
-      <c r="B11" s="19">
-        <v>50000</v>
-      </c>
-      <c r="C11" s="8" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A12" s="7" t="s">
-        <v>69</v>
-      </c>
-      <c r="B12" s="19">
+    <row r="19" spans="1:7" ht="187.2" x14ac:dyDescent="0.3">
+      <c r="A19" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="B19" s="2">
         <v>1</v>
-      </c>
-      <c r="C12" s="8" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A13" s="9" t="s">
-        <v>71</v>
-      </c>
-      <c r="B13" s="16">
-        <v>0.2</v>
-      </c>
-      <c r="C13" s="10" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" ht="21.6" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A14" s="21" t="s">
-        <v>26</v>
-      </c>
-      <c r="B14" s="21"/>
-      <c r="C14" s="21"/>
-    </row>
-    <row r="15" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A15" s="11" t="s">
-        <v>27</v>
-      </c>
-      <c r="B15" s="18">
-        <v>1</v>
-      </c>
-      <c r="C15" s="12" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" ht="21.6" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A16" s="21" t="s">
-        <v>28</v>
-      </c>
-      <c r="B16" s="21"/>
-      <c r="C16" s="21"/>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A17" s="5" t="s">
-        <v>31</v>
-      </c>
-      <c r="B17" s="17">
-        <v>0</v>
-      </c>
-      <c r="C17" s="6" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A18" s="7" t="s">
-        <v>5</v>
-      </c>
-      <c r="B18" s="2">
-        <v>0</v>
-      </c>
-      <c r="C18" s="8" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A19" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="B19" s="2" t="s">
-        <v>61</v>
       </c>
       <c r="C19" s="8" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="20" spans="1:3" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A20" s="7" t="s">
-        <v>47</v>
-      </c>
-      <c r="B20" s="2" t="s">
-        <v>62</v>
+        <v>32</v>
+      </c>
+      <c r="B20" s="2">
+        <v>100</v>
       </c>
       <c r="C20" s="8" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A21" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="B21" s="2" t="s">
-        <v>63</v>
-      </c>
-      <c r="C21" s="8" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" ht="43.8" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A21" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="B21" s="16" t="s">
+        <v>56</v>
+      </c>
+      <c r="C21" s="10" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="22" spans="1:3" ht="187.2" x14ac:dyDescent="0.3">
-      <c r="A22" s="7" t="s">
+    <row r="22" spans="1:7" ht="21.6" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A22" s="22" t="s">
+        <v>34</v>
+      </c>
+      <c r="B22" s="22"/>
+      <c r="C22" s="22"/>
+    </row>
+    <row r="23" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A23" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="B23" s="17">
+        <v>1</v>
+      </c>
+      <c r="C23" s="6" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A24" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="B24" s="2">
+        <v>1</v>
+      </c>
+      <c r="C24" s="8" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A25" s="9" t="s">
+        <v>38</v>
+      </c>
+      <c r="B25" s="16">
+        <v>0</v>
+      </c>
+      <c r="C25" s="10" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" ht="21.6" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A26" s="20" t="s">
+        <v>29</v>
+      </c>
+      <c r="B26" s="20"/>
+      <c r="C26" s="20"/>
+    </row>
+    <row r="27" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A27" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="B27" s="17" t="s">
+        <v>18</v>
+      </c>
+      <c r="C27" s="6" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" ht="86.4" x14ac:dyDescent="0.3">
+      <c r="A28" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="B28" s="2">
+        <v>20</v>
+      </c>
+      <c r="C28" s="13" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A29" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="B29" s="2">
         <v>10</v>
       </c>
-      <c r="B22" s="2">
-        <v>1</v>
-      </c>
-      <c r="C22" s="8" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A23" s="7" t="s">
-        <v>32</v>
-      </c>
-      <c r="B23" s="2">
-        <v>100</v>
-      </c>
-      <c r="C23" s="8" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3" ht="43.8" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A24" s="9" t="s">
-        <v>11</v>
-      </c>
-      <c r="B24" s="16" t="s">
-        <v>58</v>
-      </c>
-      <c r="C24" s="10" t="s">
+      <c r="C29" s="13" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" ht="58.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A30" s="9" t="s">
+        <v>43</v>
+      </c>
+      <c r="B30" s="16">
+        <v>2.5000000000000001E-2</v>
+      </c>
+      <c r="C30" s="14" t="s">
+        <v>44</v>
+      </c>
+      <c r="G30" s="15"/>
+    </row>
+    <row r="31" spans="1:7" ht="21.6" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A31" s="21" t="s">
+        <v>30</v>
+      </c>
+      <c r="B31" s="21"/>
+      <c r="C31" s="21"/>
+    </row>
+    <row r="32" spans="1:7" ht="72" x14ac:dyDescent="0.3">
+      <c r="A32" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="B32" s="17">
+        <v>20</v>
+      </c>
+      <c r="C32" s="6" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="25" spans="1:3" ht="21.6" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A25" s="22" t="s">
-        <v>34</v>
-      </c>
-      <c r="B25" s="22"/>
-      <c r="C25" s="22"/>
-    </row>
-    <row r="26" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A26" s="5" t="s">
-        <v>35</v>
-      </c>
-      <c r="B26" s="17">
-        <v>1</v>
-      </c>
-      <c r="C26" s="6" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="27" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A27" s="7" t="s">
-        <v>36</v>
-      </c>
-      <c r="B27" s="2">
-        <v>1</v>
-      </c>
-      <c r="C27" s="8" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="28" spans="1:3" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A28" s="9" t="s">
-        <v>38</v>
-      </c>
-      <c r="B28" s="16">
-        <v>0</v>
-      </c>
-      <c r="C28" s="10" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="29" spans="1:3" ht="21.6" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A29" s="20" t="s">
-        <v>29</v>
-      </c>
-      <c r="B29" s="20"/>
-      <c r="C29" s="20"/>
-    </row>
-    <row r="30" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A30" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="B30" s="17" t="s">
-        <v>18</v>
-      </c>
-      <c r="C30" s="6" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="31" spans="1:3" ht="86.4" x14ac:dyDescent="0.3">
-      <c r="A31" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="B31" s="2">
-        <v>30</v>
-      </c>
-      <c r="C31" s="13" t="s">
+    <row r="33" spans="1:3" ht="58.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A33" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="B33" s="16">
+        <v>0.15</v>
+      </c>
+      <c r="C33" s="10" t="s">
         <v>55</v>
-      </c>
-    </row>
-    <row r="32" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A32" s="7" t="s">
-        <v>41</v>
-      </c>
-      <c r="B32" s="2">
-        <v>10</v>
-      </c>
-      <c r="C32" s="13" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="33" spans="1:7" ht="58.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A33" s="9" t="s">
-        <v>43</v>
-      </c>
-      <c r="B33" s="16">
-        <v>7.0000000000000001E-3</v>
-      </c>
-      <c r="C33" s="14" t="s">
-        <v>44</v>
-      </c>
-      <c r="G33" s="15"/>
-    </row>
-    <row r="34" spans="1:7" ht="21.6" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A34" s="21" t="s">
-        <v>30</v>
-      </c>
-      <c r="B34" s="21"/>
-      <c r="C34" s="21"/>
-    </row>
-    <row r="35" spans="1:7" ht="72" x14ac:dyDescent="0.3">
-      <c r="A35" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="B35" s="17">
-        <v>15</v>
-      </c>
-      <c r="C35" s="6" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="36" spans="1:7" ht="58.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A36" s="9" t="s">
-        <v>15</v>
-      </c>
-      <c r="B36" s="16">
-        <v>0.1</v>
-      </c>
-      <c r="C36" s="10" t="s">
-        <v>57</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="6">
-    <mergeCell ref="A29:C29"/>
-    <mergeCell ref="A34:C34"/>
-    <mergeCell ref="A16:C16"/>
-    <mergeCell ref="A14:C14"/>
+    <mergeCell ref="A26:C26"/>
+    <mergeCell ref="A31:C31"/>
+    <mergeCell ref="A12:C12"/>
+    <mergeCell ref="A10:C10"/>
     <mergeCell ref="A6:C6"/>
-    <mergeCell ref="A25:C25"/>
+    <mergeCell ref="A22:C22"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
updated settings file with new settings fields
</commit_message>
<xml_diff>
--- a/settings.xlsx
+++ b/settings.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://charitede-my.sharepoint.com/personal/lev_petrov_charite_de/Documents/DOCTORATE/Cytomata/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://charitede-my.sharepoint.com/personal/lev_petrov_charite_de/Documents/DOCTORATE/Cytomata_data/iahp_panel_1/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="10" documentId="6_{876AA531-D3F9-49D7-A1D5-6BB11379BB13}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{25807F88-EDEF-40CC-902B-B0A2B0B17303}"/>
+  <xr:revisionPtr revIDLastSave="97" documentId="13_ncr:1_{9C262F40-B724-47DA-807B-CA0883A1DDFB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{0978B61A-273A-4D76-AAF9-C850FC64C5D1}"/>
   <bookViews>
-    <workbookView xWindow="2616" yWindow="2616" windowWidth="17280" windowHeight="8880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="78">
   <si>
     <t>setting</t>
   </si>
@@ -165,9 +165,15 @@
     <t>excluded_channels</t>
   </si>
   <si>
+    <t>B2M, DNA, Bead, LD, Live, Dead, ID, Cell-ID, Cell_ID</t>
+  </si>
+  <si>
     <t>grouping_orders</t>
   </si>
   <si>
+    <t>HC-050</t>
+  </si>
+  <si>
     <t>Patterns present in the names of pre-processing channels that will be used to remove them. Input separated by comma and whitespace (", "). This can be adjusted in the panel.csv file afterwards.</t>
   </si>
   <si>
@@ -201,37 +207,58 @@
     <t>norm_mode</t>
   </si>
   <si>
+    <t>Control order of groups. Input group names separated by comma and whitespace (", "). For multiple grouping columns - separate by semicolon and whitespace ("; "). If you do not want to input order for any specific grouping column - write NA.</t>
+  </si>
+  <si>
+    <t>visit, hc_pre, hc_post, pre_post</t>
+  </si>
+  <si>
+    <t>HC, S1.1, S1.2; HC, S1.1; HC, S1.2; S1.1, S1.2</t>
+  </si>
+  <si>
+    <t>B, CD4_T, CD8_T, Monos_and_DCs, NK, TCRgd_T</t>
+  </si>
+  <si>
+    <t>norm_method</t>
+  </si>
+  <si>
+    <t>sample</t>
+  </si>
+  <si>
+    <t>If quantile mode, can be either sample or channel. sample calculates n_quantiles for each channel and sample and then takes the average for each quantile over all samples to form a target distribution. channel calculates n_quantiles over all events in all reference samples for a given channel to form a target distribution. sample option is much slower, but more traditional.</t>
+  </si>
+  <si>
+    <t>norm_n_quantiles</t>
+  </si>
+  <si>
+    <t>norm_hide_zeroes</t>
+  </si>
+  <si>
+    <t>0 or 1. whether to produce additional density ridges with 0 values hidden for better visibility.</t>
+  </si>
+  <si>
+    <t>norm_ridges_downsampling</t>
+  </si>
+  <si>
+    <t>between 0 and 1. downsampling factor for density ridge plots. Use to speedup compute time.</t>
+  </si>
+  <si>
+    <t>how many quantiles to compute (+1). Tested: 100, 100000. No major difference spotted. Influences runtime by A LOT</t>
+  </si>
+  <si>
+    <t>percentile, quantile or harmony. Percentile does linear scaling using automatically estimated optimal anchor sample and optimal percentile for each channel. Quantile maps a spline interpolation function for each batch and adjusts all NON-ZERO values using the spline. NON-ZERO part is important. Harmony is weird for now, will fix at some point.</t>
+  </si>
+  <si>
+    <t>iahp_panel_1</t>
+  </si>
+  <si>
+    <t>treat_NA_as_group</t>
+  </si>
+  <si>
+    <t>0 (off, default) or 1 (on)</t>
+  </si>
+  <si>
     <t>percentile</t>
-  </si>
-  <si>
-    <t>percentile or harmony. Harmony is weird for now, will fix.</t>
-  </si>
-  <si>
-    <t>dc10</t>
-  </si>
-  <si>
-    <t>Anchor</t>
-  </si>
-  <si>
-    <t>B2M, DNA, Bead, LD, Live, Dead, ID, Cell-ID, Cell_ID, NA</t>
-  </si>
-  <si>
-    <t>group, paired_0, paired_0_5, paired_4, paired_24, paired_0_LPS, paired_0_5_LPS, paired_4_LPS, paired_24_LPS</t>
-  </si>
-  <si>
-    <t>Control order of groups. Input group names separated by comma and whitespace (", "). For multiple grouping columns - separate by semicolon and whitespace ("; "). If you do not want to input order for any specific grouping column - write NA.</t>
-  </si>
-  <si>
-    <t>DC</t>
-  </si>
-  <si>
-    <t>treat_NA_as_group</t>
-  </si>
-  <si>
-    <t>0 (off, default) or 1 (on)</t>
-  </si>
-  <si>
-    <t>DC_0h, DC_0_5h, DC_4h, DC_24h, DC_LPS_0h, DC_LPS_0_5h, DC_LPS_4h, DC_LPS_24h, DC10_0h, DC10_0_5h, DC10_4h, DC10_24h, DC10_LPS_0h, DC10_LPS_0_5h, DC10_LPS_4h, DC10_LPS_24h; DC_0h, DC10_0h; DC_0_5h, DC10_0_5h; DC_4h, DC10_4h; DC_24h, DC10_24h; DC_LPS_0h, DC10_LPS_0h; DC_LPS_0_5h, DC10_LPS_0_5h; DC_LPS_4h, DC10_LPS_4h; DC_LPS_24h, DC10_LPS_24h</t>
   </si>
 </sst>
 </file>
@@ -746,15 +773,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G33"/>
+  <dimension ref="A1:G37"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="B16" sqref="B16"/>
+    <sheetView tabSelected="1" topLeftCell="A24" workbookViewId="0">
+      <selection activeCell="B32" sqref="B32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="23.109375" style="1" customWidth="1"/>
+    <col min="1" max="1" width="24.44140625" style="1" customWidth="1"/>
     <col min="2" max="2" width="71.33203125" style="2" customWidth="1"/>
     <col min="3" max="3" width="59" style="2" customWidth="1"/>
   </cols>
@@ -786,7 +813,7 @@
         <v>4</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>60</v>
+        <v>74</v>
       </c>
       <c r="C3" s="8" t="s">
         <v>21</v>
@@ -808,10 +835,10 @@
         <v>45</v>
       </c>
       <c r="B5" s="16" t="s">
-        <v>62</v>
+        <v>46</v>
       </c>
       <c r="C5" s="10" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
     </row>
     <row r="6" spans="1:3" ht="21.6" thickBot="1" x14ac:dyDescent="0.35">
@@ -832,281 +859,325 @@
         <v>24</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:3" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A8" s="7" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="B8" s="19" t="s">
-        <v>58</v>
+        <v>77</v>
       </c>
       <c r="C8" s="8" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A9" s="9" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A9" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="B9" s="16" t="s">
+      <c r="B9" s="19" t="s">
+        <v>48</v>
+      </c>
+      <c r="C9" s="8" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" ht="86.4" x14ac:dyDescent="0.3">
+      <c r="A10" s="7" t="s">
+        <v>64</v>
+      </c>
+      <c r="B10" s="19" t="s">
+        <v>65</v>
+      </c>
+      <c r="C10" s="8" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A11" s="7" t="s">
+        <v>67</v>
+      </c>
+      <c r="B11" s="19">
+        <v>100000</v>
+      </c>
+      <c r="C11" s="8" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A12" s="7" t="s">
+        <v>68</v>
+      </c>
+      <c r="B12" s="19">
+        <v>1</v>
+      </c>
+      <c r="C12" s="8" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A13" s="9" t="s">
+        <v>70</v>
+      </c>
+      <c r="B13" s="16">
+        <v>0.2</v>
+      </c>
+      <c r="C13" s="10" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" ht="21.6" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A14" s="21" t="s">
+        <v>26</v>
+      </c>
+      <c r="B14" s="21"/>
+      <c r="C14" s="21"/>
+    </row>
+    <row r="15" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A15" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="B15" s="18">
+        <v>0</v>
+      </c>
+      <c r="C15" s="12" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" ht="21.6" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A16" s="21" t="s">
+        <v>28</v>
+      </c>
+      <c r="B16" s="21"/>
+      <c r="C16" s="21"/>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A17" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="B17" s="17">
+        <v>1</v>
+      </c>
+      <c r="C17" s="6" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A18" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="B18" s="2">
+        <v>1</v>
+      </c>
+      <c r="C18" s="8" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A19" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="B19" s="2" t="s">
         <v>61</v>
-      </c>
-      <c r="C9" s="10" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" ht="21.6" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A10" s="21" t="s">
-        <v>26</v>
-      </c>
-      <c r="B10" s="21"/>
-      <c r="C10" s="21"/>
-    </row>
-    <row r="11" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A11" s="11" t="s">
-        <v>27</v>
-      </c>
-      <c r="B11" s="18">
-        <v>0</v>
-      </c>
-      <c r="C11" s="12" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" ht="21.6" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A12" s="21" t="s">
-        <v>28</v>
-      </c>
-      <c r="B12" s="21"/>
-      <c r="C12" s="21"/>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A13" s="5" t="s">
-        <v>31</v>
-      </c>
-      <c r="B13" s="17">
-        <v>1</v>
-      </c>
-      <c r="C13" s="6" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A14" s="7" t="s">
-        <v>5</v>
-      </c>
-      <c r="B14" s="2">
-        <v>1</v>
-      </c>
-      <c r="C14" s="8" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A15" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="B15" s="2" t="s">
-        <v>63</v>
-      </c>
-      <c r="C15" s="8" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" ht="86.4" x14ac:dyDescent="0.3">
-      <c r="A16" s="7" t="s">
-        <v>46</v>
-      </c>
-      <c r="B16" s="2" t="s">
-        <v>68</v>
-      </c>
-      <c r="C16" s="8" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A17" s="7" t="s">
-        <v>66</v>
-      </c>
-      <c r="B17" s="2">
-        <v>0</v>
-      </c>
-      <c r="C17" s="8" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="18" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A18" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="B18" s="2" t="s">
-        <v>65</v>
-      </c>
-      <c r="C18" s="8" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="19" spans="1:7" ht="187.2" x14ac:dyDescent="0.3">
-      <c r="A19" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="B19" s="2">
-        <v>1</v>
       </c>
       <c r="C19" s="8" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="20" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:3" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A20" s="7" t="s">
+        <v>47</v>
+      </c>
+      <c r="B20" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="C20" s="8" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A21" s="7" t="s">
+        <v>75</v>
+      </c>
+      <c r="B21" s="2">
+        <v>0</v>
+      </c>
+      <c r="C21" s="8" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A22" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="B22" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="C22" s="8" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" ht="187.2" x14ac:dyDescent="0.3">
+      <c r="A23" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="B23" s="2">
+        <v>1</v>
+      </c>
+      <c r="C23" s="8" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A24" s="7" t="s">
         <v>32</v>
       </c>
-      <c r="B20" s="2">
+      <c r="B24" s="2">
         <v>100</v>
       </c>
-      <c r="C20" s="8" t="s">
+      <c r="C24" s="8" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="21" spans="1:7" ht="43.8" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A21" s="9" t="s">
+    <row r="25" spans="1:3" ht="43.8" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A25" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="B21" s="16" t="s">
+      <c r="B25" s="16" t="s">
+        <v>58</v>
+      </c>
+      <c r="C25" s="10" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" ht="21.6" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A26" s="22" t="s">
+        <v>34</v>
+      </c>
+      <c r="B26" s="22"/>
+      <c r="C26" s="22"/>
+    </row>
+    <row r="27" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A27" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="B27" s="17">
+        <v>1</v>
+      </c>
+      <c r="C27" s="6" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A28" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="B28" s="2">
+        <v>1</v>
+      </c>
+      <c r="C28" s="8" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A29" s="9" t="s">
+        <v>38</v>
+      </c>
+      <c r="B29" s="16">
+        <v>0</v>
+      </c>
+      <c r="C29" s="10" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" ht="21.6" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A30" s="20" t="s">
+        <v>29</v>
+      </c>
+      <c r="B30" s="20"/>
+      <c r="C30" s="20"/>
+    </row>
+    <row r="31" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A31" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="B31" s="17" t="s">
+        <v>18</v>
+      </c>
+      <c r="C31" s="6" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" ht="86.4" x14ac:dyDescent="0.3">
+      <c r="A32" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="B32" s="2">
+        <v>30</v>
+      </c>
+      <c r="C32" s="13" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A33" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="B33" s="2">
+        <v>10</v>
+      </c>
+      <c r="C33" s="13" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" ht="58.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A34" s="9" t="s">
+        <v>43</v>
+      </c>
+      <c r="B34" s="16">
+        <v>7.0000000000000001E-3</v>
+      </c>
+      <c r="C34" s="14" t="s">
+        <v>44</v>
+      </c>
+      <c r="G34" s="15"/>
+    </row>
+    <row r="35" spans="1:7" ht="21.6" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A35" s="21" t="s">
+        <v>30</v>
+      </c>
+      <c r="B35" s="21"/>
+      <c r="C35" s="21"/>
+    </row>
+    <row r="36" spans="1:7" ht="72" x14ac:dyDescent="0.3">
+      <c r="A36" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="B36" s="17">
+        <v>15</v>
+      </c>
+      <c r="C36" s="6" t="s">
         <v>56</v>
       </c>
-      <c r="C21" s="10" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="22" spans="1:7" ht="21.6" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A22" s="22" t="s">
-        <v>34</v>
-      </c>
-      <c r="B22" s="22"/>
-      <c r="C22" s="22"/>
-    </row>
-    <row r="23" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A23" s="5" t="s">
-        <v>35</v>
-      </c>
-      <c r="B23" s="17">
-        <v>1</v>
-      </c>
-      <c r="C23" s="6" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="24" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A24" s="7" t="s">
-        <v>36</v>
-      </c>
-      <c r="B24" s="2">
-        <v>1</v>
-      </c>
-      <c r="C24" s="8" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="25" spans="1:7" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A25" s="9" t="s">
-        <v>38</v>
-      </c>
-      <c r="B25" s="16">
-        <v>0</v>
-      </c>
-      <c r="C25" s="10" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="26" spans="1:7" ht="21.6" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A26" s="20" t="s">
-        <v>29</v>
-      </c>
-      <c r="B26" s="20"/>
-      <c r="C26" s="20"/>
-    </row>
-    <row r="27" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A27" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="B27" s="17" t="s">
-        <v>18</v>
-      </c>
-      <c r="C27" s="6" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="28" spans="1:7" ht="86.4" x14ac:dyDescent="0.3">
-      <c r="A28" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="B28" s="2">
-        <v>20</v>
-      </c>
-      <c r="C28" s="13" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="29" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A29" s="7" t="s">
-        <v>41</v>
-      </c>
-      <c r="B29" s="2">
-        <v>10</v>
-      </c>
-      <c r="C29" s="13" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="30" spans="1:7" ht="58.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A30" s="9" t="s">
-        <v>43</v>
-      </c>
-      <c r="B30" s="16">
-        <v>2.5000000000000001E-2</v>
-      </c>
-      <c r="C30" s="14" t="s">
-        <v>44</v>
-      </c>
-      <c r="G30" s="15"/>
-    </row>
-    <row r="31" spans="1:7" ht="21.6" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A31" s="21" t="s">
-        <v>30</v>
-      </c>
-      <c r="B31" s="21"/>
-      <c r="C31" s="21"/>
-    </row>
-    <row r="32" spans="1:7" ht="72" x14ac:dyDescent="0.3">
-      <c r="A32" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="B32" s="17">
-        <v>20</v>
-      </c>
-      <c r="C32" s="6" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="33" spans="1:3" ht="58.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A33" s="9" t="s">
+    </row>
+    <row r="37" spans="1:7" ht="58.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A37" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="B33" s="16">
-        <v>0.15</v>
-      </c>
-      <c r="C33" s="10" t="s">
-        <v>55</v>
+      <c r="B37" s="16">
+        <v>0.1</v>
+      </c>
+      <c r="C37" s="10" t="s">
+        <v>57</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="6">
+    <mergeCell ref="A30:C30"/>
+    <mergeCell ref="A35:C35"/>
+    <mergeCell ref="A16:C16"/>
+    <mergeCell ref="A14:C14"/>
+    <mergeCell ref="A6:C6"/>
     <mergeCell ref="A26:C26"/>
-    <mergeCell ref="A31:C31"/>
-    <mergeCell ref="A12:C12"/>
-    <mergeCell ref="A10:C10"/>
-    <mergeCell ref="A6:C6"/>
-    <mergeCell ref="A22:C22"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
feat: summary_table csv exporting to output_group folder with added prefix
</commit_message>
<xml_diff>
--- a/settings.xlsx
+++ b/settings.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://charitede-my.sharepoint.com/personal/lev_petrov_charite_de/Documents/DOCTORATE/Cytomata_data/iahp_panel_1/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="97" documentId="13_ncr:1_{9C262F40-B724-47DA-807B-CA0883A1DDFB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{0978B61A-273A-4D76-AAF9-C850FC64C5D1}"/>
+  <xr:revisionPtr revIDLastSave="99" documentId="13_ncr:1_{9C262F40-B724-47DA-807B-CA0883A1DDFB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{03721125-8F97-4ABF-A6EF-FD79164E632C}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -258,7 +258,7 @@
     <t>0 (off, default) or 1 (on)</t>
   </si>
   <si>
-    <t>percentile</t>
+    <t>quantile</t>
   </si>
 </sst>
 </file>
@@ -775,8 +775,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G37"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A24" workbookViewId="0">
-      <selection activeCell="B32" sqref="B32"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -937,7 +937,7 @@
         <v>27</v>
       </c>
       <c r="B15" s="18">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C15" s="12" t="s">
         <v>24</v>

</xml_diff>

<commit_message>
feat: add manually-toggled do_subsetting module, which takes normalized parquet files, extracts backbone markers, does clustering and UMAPs and (optionally, toggled manually) writes subsets as separate FCS files, according to manual annotation to the data subsets folder for downstream analysis
</commit_message>
<xml_diff>
--- a/settings.xlsx
+++ b/settings.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://charitede-my.sharepoint.com/personal/lev_petrov_charite_de/Documents/DOCTORATE/Cytomata_data/iahp_panel_1/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://charitede-my.sharepoint.com/personal/lev_petrov_charite_de/Documents/DOCTORATE/Cytomata_data/iahp_panel_2/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="99" documentId="13_ncr:1_{9C262F40-B724-47DA-807B-CA0883A1DDFB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{03721125-8F97-4ABF-A6EF-FD79164E632C}"/>
+  <xr:revisionPtr revIDLastSave="1" documentId="13_ncr:1_{4072FD5B-943D-4C26-9378-A5CA380F2CD3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{7B0AA230-583C-470D-8818-B113C3E41708}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -216,9 +216,6 @@
     <t>HC, S1.1, S1.2; HC, S1.1; HC, S1.2; S1.1, S1.2</t>
   </si>
   <si>
-    <t>B, CD4_T, CD8_T, Monos_and_DCs, NK, TCRgd_T</t>
-  </si>
-  <si>
     <t>norm_method</t>
   </si>
   <si>
@@ -249,9 +246,6 @@
     <t>percentile, quantile or harmony. Percentile does linear scaling using automatically estimated optimal anchor sample and optimal percentile for each channel. Quantile maps a spline interpolation function for each batch and adjusts all NON-ZERO values using the spline. NON-ZERO part is important. Harmony is weird for now, will fix at some point.</t>
   </si>
   <si>
-    <t>iahp_panel_1</t>
-  </si>
-  <si>
     <t>treat_NA_as_group</t>
   </si>
   <si>
@@ -259,6 +253,12 @@
   </si>
   <si>
     <t>quantile</t>
+  </si>
+  <si>
+    <t>iahp_panel_2</t>
+  </si>
+  <si>
+    <t>Granulos</t>
   </si>
 </sst>
 </file>
@@ -775,8 +775,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G37"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="B22" sqref="B22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -813,7 +813,7 @@
         <v>4</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="C3" s="8" t="s">
         <v>21</v>
@@ -864,10 +864,10 @@
         <v>59</v>
       </c>
       <c r="B8" s="19" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="C8" s="8" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="9" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
@@ -883,46 +883,46 @@
     </row>
     <row r="10" spans="1:3" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A10" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="B10" s="19" t="s">
         <v>64</v>
       </c>
-      <c r="B10" s="19" t="s">
+      <c r="C10" s="8" t="s">
         <v>65</v>
-      </c>
-      <c r="C10" s="8" t="s">
-        <v>66</v>
       </c>
     </row>
     <row r="11" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A11" s="7" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B11" s="19">
         <v>100000</v>
       </c>
       <c r="C11" s="8" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="12" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A12" s="7" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B12" s="19">
         <v>1</v>
       </c>
       <c r="C12" s="8" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="13" spans="1:3" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A13" s="9" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B13" s="16">
         <v>0.2</v>
       </c>
       <c r="C13" s="10" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="14" spans="1:3" ht="21.6" thickBot="1" x14ac:dyDescent="0.35">
@@ -937,7 +937,7 @@
         <v>27</v>
       </c>
       <c r="B15" s="18">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C15" s="12" t="s">
         <v>24</v>
@@ -996,13 +996,13 @@
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A21" s="7" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="B21" s="2">
         <v>0</v>
       </c>
       <c r="C21" s="8" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
     </row>
     <row r="22" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
@@ -1010,7 +1010,7 @@
         <v>9</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>63</v>
+        <v>77</v>
       </c>
       <c r="C22" s="8" t="s">
         <v>52</v>

</xml_diff>

<commit_message>
add: UMAP optimization, better data input, scattermore, subsampling options
</commit_message>
<xml_diff>
--- a/settings.xlsx
+++ b/settings.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://charitede-my.sharepoint.com/personal/lev_petrov_charite_de/Documents/DOCTORATE/Cytomata_data/iahp_panel_2/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://charitede-my.sharepoint.com/personal/lev_petrov_charite_de/Documents/DOCTORATE/Cytomata_data/iahp_panel_3/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1" documentId="13_ncr:1_{4072FD5B-943D-4C26-9378-A5CA380F2CD3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{7B0AA230-583C-470D-8818-B113C3E41708}"/>
+  <xr:revisionPtr revIDLastSave="105" documentId="13_ncr:1_{9C262F40-B724-47DA-807B-CA0883A1DDFB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D1F6F8A5-DD13-4829-ABAD-55A00A56A60F}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1884" yWindow="1884" windowWidth="17280" windowHeight="8880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -216,6 +216,9 @@
     <t>HC, S1.1, S1.2; HC, S1.1; HC, S1.2; S1.1, S1.2</t>
   </si>
   <si>
+    <t>B, CD4_T, CD8_T, Monos_and_DCs, NK, TCRgd_T</t>
+  </si>
+  <si>
     <t>norm_method</t>
   </si>
   <si>
@@ -255,10 +258,7 @@
     <t>quantile</t>
   </si>
   <si>
-    <t>iahp_panel_2</t>
-  </si>
-  <si>
-    <t>Granulos</t>
+    <t>iahp_panel_3</t>
   </si>
 </sst>
 </file>
@@ -775,8 +775,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G37"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="B22" sqref="B22"/>
+    <sheetView tabSelected="1" topLeftCell="A33" workbookViewId="0">
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -813,7 +813,7 @@
         <v>4</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="C3" s="8" t="s">
         <v>21</v>
@@ -864,10 +864,10 @@
         <v>59</v>
       </c>
       <c r="B8" s="19" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="C8" s="8" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
     </row>
     <row r="9" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
@@ -883,46 +883,46 @@
     </row>
     <row r="10" spans="1:3" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A10" s="7" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="B10" s="19" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="C10" s="8" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
     </row>
     <row r="11" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A11" s="7" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="B11" s="19">
         <v>100000</v>
       </c>
       <c r="C11" s="8" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
     </row>
     <row r="12" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A12" s="7" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="B12" s="19">
         <v>1</v>
       </c>
       <c r="C12" s="8" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
     </row>
     <row r="13" spans="1:3" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A13" s="9" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="B13" s="16">
         <v>0.2</v>
       </c>
       <c r="C13" s="10" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
     </row>
     <row r="14" spans="1:3" ht="21.6" thickBot="1" x14ac:dyDescent="0.35">
@@ -996,13 +996,13 @@
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A21" s="7" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="B21" s="2">
         <v>0</v>
       </c>
       <c r="C21" s="8" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
     </row>
     <row r="22" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
@@ -1010,7 +1010,7 @@
         <v>9</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>77</v>
+        <v>63</v>
       </c>
       <c r="C22" s="8" t="s">
         <v>52</v>

</xml_diff>

<commit_message>
Enable UMAP/PCA plots and improve paired analysis with unpaired data removal
- Uncomment UMAP and PCA plot generation in core and exploration modules
- Add remove_unpaired parameter to do_paired_boxplots() to filter incomplete pairs
- Implement paired data validation and unpaired sample removal logic
- Add marker expression analysis for all clusters with paired comparisons
- Optimize plot rendering with improved sampling and visual parameters
- Fix conditional checks for meta_cluster_annotation plotting
</commit_message>
<xml_diff>
--- a/settings.xlsx
+++ b/settings.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://charitede-my.sharepoint.com/personal/lev_petrov_charite_de/Documents/DOCTORATE/Cytomata_data/iahp_panel_3/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://charitede-my.sharepoint.com/personal/lev_petrov_charite_de/Documents/DOCTORATE/Cytomata_data/iahp_panel_2/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="105" documentId="13_ncr:1_{9C262F40-B724-47DA-807B-CA0883A1DDFB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D1F6F8A5-DD13-4829-ABAD-55A00A56A60F}"/>
+  <xr:revisionPtr revIDLastSave="1" documentId="13_ncr:1_{4072FD5B-943D-4C26-9378-A5CA380F2CD3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{7B0AA230-583C-470D-8818-B113C3E41708}"/>
   <bookViews>
-    <workbookView xWindow="1884" yWindow="1884" windowWidth="17280" windowHeight="8880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -216,9 +216,6 @@
     <t>HC, S1.1, S1.2; HC, S1.1; HC, S1.2; S1.1, S1.2</t>
   </si>
   <si>
-    <t>B, CD4_T, CD8_T, Monos_and_DCs, NK, TCRgd_T</t>
-  </si>
-  <si>
     <t>norm_method</t>
   </si>
   <si>
@@ -258,7 +255,10 @@
     <t>quantile</t>
   </si>
   <si>
-    <t>iahp_panel_3</t>
+    <t>iahp_panel_2</t>
+  </si>
+  <si>
+    <t>Granulos</t>
   </si>
 </sst>
 </file>
@@ -775,8 +775,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G37"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A33" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="B22" sqref="B22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -813,7 +813,7 @@
         <v>4</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C3" s="8" t="s">
         <v>21</v>
@@ -864,10 +864,10 @@
         <v>59</v>
       </c>
       <c r="B8" s="19" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C8" s="8" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="9" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
@@ -883,46 +883,46 @@
     </row>
     <row r="10" spans="1:3" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A10" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="B10" s="19" t="s">
         <v>64</v>
       </c>
-      <c r="B10" s="19" t="s">
+      <c r="C10" s="8" t="s">
         <v>65</v>
-      </c>
-      <c r="C10" s="8" t="s">
-        <v>66</v>
       </c>
     </row>
     <row r="11" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A11" s="7" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B11" s="19">
         <v>100000</v>
       </c>
       <c r="C11" s="8" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="12" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A12" s="7" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B12" s="19">
         <v>1</v>
       </c>
       <c r="C12" s="8" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="13" spans="1:3" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A13" s="9" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B13" s="16">
         <v>0.2</v>
       </c>
       <c r="C13" s="10" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="14" spans="1:3" ht="21.6" thickBot="1" x14ac:dyDescent="0.35">
@@ -996,13 +996,13 @@
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A21" s="7" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B21" s="2">
         <v>0</v>
       </c>
       <c r="C21" s="8" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="22" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
@@ -1010,7 +1010,7 @@
         <v>9</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>63</v>
+        <v>77</v>
       </c>
       <c r="C22" s="8" t="s">
         <v>52</v>

</xml_diff>

<commit_message>
fix: pre_post IAHP addon features assignment
</commit_message>
<xml_diff>
--- a/settings.xlsx
+++ b/settings.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24332"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27932"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://charitede-my.sharepoint.com/personal/lev_petrov_charite_de/Documents/DOCTORATE/Cytomata_data/iahp_panel_2/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://charitede-my.sharepoint.com/personal/lev_petrov_charite_de/Documents/DOCTORATE/Cytomata_data/iahp_panel_1/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1" documentId="13_ncr:1_{4072FD5B-943D-4C26-9378-A5CA380F2CD3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{7B0AA230-583C-470D-8818-B113C3E41708}"/>
+  <xr:revisionPtr revIDLastSave="106" documentId="13_ncr:1_{9C262F40-B724-47DA-807B-CA0883A1DDFB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{0C142C15-61FE-4B80-ACAE-6448CE126CDF}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="3780" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -216,6 +216,9 @@
     <t>HC, S1.1, S1.2; HC, S1.1; HC, S1.2; S1.1, S1.2</t>
   </si>
   <si>
+    <t>B, CD4_T, CD8_T, Monos_and_DCs, NK, TCRgd_T</t>
+  </si>
+  <si>
     <t>norm_method</t>
   </si>
   <si>
@@ -246,6 +249,9 @@
     <t>percentile, quantile or harmony. Percentile does linear scaling using automatically estimated optimal anchor sample and optimal percentile for each channel. Quantile maps a spline interpolation function for each batch and adjusts all NON-ZERO values using the spline. NON-ZERO part is important. Harmony is weird for now, will fix at some point.</t>
   </si>
   <si>
+    <t>iahp_panel_1</t>
+  </si>
+  <si>
     <t>treat_NA_as_group</t>
   </si>
   <si>
@@ -253,12 +259,6 @@
   </si>
   <si>
     <t>quantile</t>
-  </si>
-  <si>
-    <t>iahp_panel_2</t>
-  </si>
-  <si>
-    <t>Granulos</t>
   </si>
 </sst>
 </file>
@@ -775,8 +775,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G37"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="B22" sqref="B22"/>
+    <sheetView tabSelected="1" topLeftCell="A29" workbookViewId="0">
+      <selection activeCell="B38" sqref="B38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -813,7 +813,7 @@
         <v>4</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="C3" s="8" t="s">
         <v>21</v>
@@ -864,10 +864,10 @@
         <v>59</v>
       </c>
       <c r="B8" s="19" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="C8" s="8" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
     </row>
     <row r="9" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
@@ -883,46 +883,46 @@
     </row>
     <row r="10" spans="1:3" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A10" s="7" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="B10" s="19" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="C10" s="8" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
     </row>
     <row r="11" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A11" s="7" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="B11" s="19">
         <v>100000</v>
       </c>
       <c r="C11" s="8" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
     </row>
     <row r="12" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A12" s="7" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="B12" s="19">
         <v>1</v>
       </c>
       <c r="C12" s="8" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
     </row>
     <row r="13" spans="1:3" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A13" s="9" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="B13" s="16">
         <v>0.2</v>
       </c>
       <c r="C13" s="10" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
     </row>
     <row r="14" spans="1:3" ht="21.6" thickBot="1" x14ac:dyDescent="0.35">
@@ -996,13 +996,13 @@
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A21" s="7" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="B21" s="2">
         <v>0</v>
       </c>
       <c r="C21" s="8" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
     </row>
     <row r="22" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
@@ -1010,7 +1010,7 @@
         <v>9</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>77</v>
+        <v>63</v>
       </c>
       <c r="C22" s="8" t="s">
         <v>52</v>
@@ -1153,7 +1153,7 @@
         <v>14</v>
       </c>
       <c r="B36" s="17">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="C36" s="6" t="s">
         <v>56</v>
@@ -1164,7 +1164,7 @@
         <v>15</v>
       </c>
       <c r="B37" s="16">
-        <v>0.1</v>
+        <v>0.2</v>
       </c>
       <c r="C37" s="10" t="s">
         <v>57</v>

</xml_diff>

<commit_message>
chore: enable do_subsetting from settings file
</commit_message>
<xml_diff>
--- a/settings.xlsx
+++ b/settings.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27932"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24332"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://charitede-my.sharepoint.com/personal/lev_petrov_charite_de/Documents/DOCTORATE/Cytomata_data/iahp_panel_1/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://charitede-my.sharepoint.com/personal/lev_petrov_charite_de/Documents/DOCTORATE/Cytomata_data/anca_panel_1/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="106" documentId="13_ncr:1_{9C262F40-B724-47DA-807B-CA0883A1DDFB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{0C142C15-61FE-4B80-ACAE-6448CE126CDF}"/>
+  <xr:revisionPtr revIDLastSave="11" documentId="13_ncr:1_{9C262F40-B724-47DA-807B-CA0883A1DDFB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{692FB08E-D1B3-497B-8394-4AD66FE0A642}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="3780" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="78">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="80">
   <si>
     <t>setting</t>
   </si>
@@ -174,6 +174,9 @@
     <t>HC-050</t>
   </si>
   <si>
+    <t>anca_panel_1</t>
+  </si>
+  <si>
     <t>Patterns present in the names of pre-processing channels that will be used to remove them. Input separated by comma and whitespace (", "). This can be adjusted in the panel.csv file afterwards.</t>
   </si>
   <si>
@@ -201,64 +204,67 @@
     <t>UMAPs min_dist. Lower values lead to clumpier embeddings, higher make them more spread-out. Accepts multiple values, separated by comma and whitespace (", ") of different values are needed for each data_subset. Order is given by data_subset vector.</t>
   </si>
   <si>
+    <t>Control order of groups. Input group names separated by comma and whitespace (", "). For multiple grouping columns - separate by semicolon and whitespace (", "). If you do not want to input order for any specific grouping column - write NA.</t>
+  </si>
+  <si>
+    <t>HC, MPO, PR3; HC, ANCA</t>
+  </si>
+  <si>
+    <t>antigen, anca_status</t>
+  </si>
+  <si>
     <t>0, 30</t>
   </si>
   <si>
     <t>norm_mode</t>
   </si>
   <si>
-    <t>Control order of groups. Input group names separated by comma and whitespace (", "). For multiple grouping columns - separate by semicolon and whitespace ("; "). If you do not want to input order for any specific grouping column - write NA.</t>
-  </si>
-  <si>
-    <t>visit, hc_pre, hc_post, pre_post</t>
-  </si>
-  <si>
-    <t>HC, S1.1, S1.2; HC, S1.1; HC, S1.2; S1.1, S1.2</t>
+    <t>quantile</t>
+  </si>
+  <si>
+    <t>percentile, quantile or harmony. Percentile does linear scaling using automatically estimated optimal anchor sample and optimal percentile for each channel. Quantile maps a spline interpolation function for each batch and adjusts all NON-ZERO values using the spline. NON-ZERO part is important. Harmony is weird for now, will fix at some point.</t>
+  </si>
+  <si>
+    <t>norm_method</t>
+  </si>
+  <si>
+    <t>sample</t>
+  </si>
+  <si>
+    <t>If quantile mode, can be either sample or channel. sample calculates n_quantiles for each channel and sample and then takes the average for each quantile over all samples to form a target distribution. channel calculates n_quantiles over all events in all reference samples for a given channel to form a target distribution. sample option is much slower, but more traditional.</t>
+  </si>
+  <si>
+    <t>norm_n_quantiles</t>
+  </si>
+  <si>
+    <t>how many quantiles to compute (+1). Tested: 100, 100000. No major difference spotted. Influences runtime by A LOT</t>
+  </si>
+  <si>
+    <t>norm_hide_zeroes</t>
+  </si>
+  <si>
+    <t>0 or 1. whether to produce additional density ridges with 0 values hidden for better visibility.</t>
+  </si>
+  <si>
+    <t>norm_ridges_downsampling</t>
+  </si>
+  <si>
+    <t>between 0 and 1. downsampling factor for density ridge plots. Use to speedup compute time.</t>
+  </si>
+  <si>
+    <t>full dataset subsetting settings</t>
+  </si>
+  <si>
+    <t>do_subsetting</t>
+  </si>
+  <si>
+    <t>treat_NA_as_group</t>
+  </si>
+  <si>
+    <t>0 (off, default) or 1 (on)</t>
   </si>
   <si>
     <t>B, CD4_T, CD8_T, Monos_and_DCs, NK, TCRgd_T</t>
-  </si>
-  <si>
-    <t>norm_method</t>
-  </si>
-  <si>
-    <t>sample</t>
-  </si>
-  <si>
-    <t>If quantile mode, can be either sample or channel. sample calculates n_quantiles for each channel and sample and then takes the average for each quantile over all samples to form a target distribution. channel calculates n_quantiles over all events in all reference samples for a given channel to form a target distribution. sample option is much slower, but more traditional.</t>
-  </si>
-  <si>
-    <t>norm_n_quantiles</t>
-  </si>
-  <si>
-    <t>norm_hide_zeroes</t>
-  </si>
-  <si>
-    <t>0 or 1. whether to produce additional density ridges with 0 values hidden for better visibility.</t>
-  </si>
-  <si>
-    <t>norm_ridges_downsampling</t>
-  </si>
-  <si>
-    <t>between 0 and 1. downsampling factor for density ridge plots. Use to speedup compute time.</t>
-  </si>
-  <si>
-    <t>how many quantiles to compute (+1). Tested: 100, 100000. No major difference spotted. Influences runtime by A LOT</t>
-  </si>
-  <si>
-    <t>percentile, quantile or harmony. Percentile does linear scaling using automatically estimated optimal anchor sample and optimal percentile for each channel. Quantile maps a spline interpolation function for each batch and adjusts all NON-ZERO values using the spline. NON-ZERO part is important. Harmony is weird for now, will fix at some point.</t>
-  </si>
-  <si>
-    <t>iahp_panel_1</t>
-  </si>
-  <si>
-    <t>treat_NA_as_group</t>
-  </si>
-  <si>
-    <t>0 (off, default) or 1 (on)</t>
-  </si>
-  <si>
-    <t>quantile</t>
   </si>
 </sst>
 </file>
@@ -425,7 +431,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -481,13 +487,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -773,15 +776,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G37"/>
+  <dimension ref="A1:G39"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A29" workbookViewId="0">
-      <selection activeCell="B38" sqref="B38"/>
+    <sheetView tabSelected="1" topLeftCell="A15" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C24" sqref="C24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="24.44140625" style="1" customWidth="1"/>
+    <col min="1" max="1" width="23.109375" style="1" customWidth="1"/>
     <col min="2" max="2" width="71.33203125" style="2" customWidth="1"/>
     <col min="3" max="3" width="59" style="2" customWidth="1"/>
   </cols>
@@ -813,7 +816,7 @@
         <v>4</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>74</v>
+        <v>49</v>
       </c>
       <c r="C3" s="8" t="s">
         <v>21</v>
@@ -838,22 +841,22 @@
         <v>46</v>
       </c>
       <c r="C5" s="10" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
     </row>
     <row r="6" spans="1:3" ht="21.6" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A6" s="21" t="s">
+      <c r="A6" s="19" t="s">
         <v>23</v>
       </c>
-      <c r="B6" s="21"/>
-      <c r="C6" s="21"/>
+      <c r="B6" s="19"/>
+      <c r="C6" s="19"/>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" s="5" t="s">
         <v>25</v>
       </c>
       <c r="B7" s="17">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C7" s="6" t="s">
         <v>24</v>
@@ -861,323 +864,342 @@
     </row>
     <row r="8" spans="1:3" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A8" s="7" t="s">
-        <v>59</v>
-      </c>
-      <c r="B8" s="19" t="s">
-        <v>77</v>
+        <v>63</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>64</v>
       </c>
       <c r="C8" s="8" t="s">
-        <v>73</v>
+        <v>65</v>
       </c>
     </row>
     <row r="9" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A9" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="B9" s="19" t="s">
+      <c r="B9" s="2" t="s">
         <v>48</v>
       </c>
       <c r="C9" s="8" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
     </row>
     <row r="10" spans="1:3" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A10" s="7" t="s">
-        <v>64</v>
-      </c>
-      <c r="B10" s="19" t="s">
-        <v>65</v>
+        <v>66</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>67</v>
       </c>
       <c r="C10" s="8" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
     </row>
     <row r="11" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A11" s="7" t="s">
-        <v>67</v>
-      </c>
-      <c r="B11" s="19">
+        <v>69</v>
+      </c>
+      <c r="B11" s="2">
         <v>100000</v>
       </c>
       <c r="C11" s="8" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
     </row>
     <row r="12" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A12" s="7" t="s">
-        <v>68</v>
-      </c>
-      <c r="B12" s="19">
+        <v>71</v>
+      </c>
+      <c r="B12" s="2">
         <v>1</v>
       </c>
       <c r="C12" s="8" t="s">
-        <v>69</v>
+        <v>72</v>
       </c>
     </row>
     <row r="13" spans="1:3" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A13" s="9" t="s">
-        <v>70</v>
+        <v>73</v>
       </c>
       <c r="B13" s="16">
         <v>0.2</v>
       </c>
       <c r="C13" s="10" t="s">
-        <v>71</v>
+        <v>74</v>
       </c>
     </row>
     <row r="14" spans="1:3" ht="21.6" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A14" s="21" t="s">
+      <c r="A14" s="19" t="s">
         <v>26</v>
       </c>
-      <c r="B14" s="21"/>
-      <c r="C14" s="21"/>
+      <c r="B14" s="19"/>
+      <c r="C14" s="19"/>
     </row>
     <row r="15" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A15" s="11" t="s">
         <v>27</v>
       </c>
       <c r="B15" s="18">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C15" s="12" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="16" spans="1:3" ht="21.6" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A16" s="21" t="s">
+      <c r="A16" s="19" t="s">
+        <v>75</v>
+      </c>
+      <c r="B16" s="19"/>
+      <c r="C16" s="19"/>
+    </row>
+    <row r="17" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A17" s="11" t="s">
+        <v>76</v>
+      </c>
+      <c r="B17" s="18">
+        <v>1</v>
+      </c>
+      <c r="C17" s="12" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" ht="21.6" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A18" s="19" t="s">
         <v>28</v>
       </c>
-      <c r="B16" s="21"/>
-      <c r="C16" s="21"/>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A17" s="5" t="s">
+      <c r="B18" s="19"/>
+      <c r="C18" s="19"/>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A19" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="B17" s="17">
+      <c r="B19" s="17">
         <v>1</v>
       </c>
-      <c r="C17" s="6" t="s">
+      <c r="C19" s="6" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="18" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A18" s="7" t="s">
+    <row r="20" spans="1:3" ht="43.8" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A20" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="B18" s="2">
+      <c r="B20" s="2">
         <v>1</v>
       </c>
-      <c r="C18" s="8" t="s">
+      <c r="C20" s="8" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="19" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A19" s="7" t="s">
+    <row r="21" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A21" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="B19" s="2" t="s">
+      <c r="B21" s="2" t="s">
         <v>61</v>
       </c>
-      <c r="C19" s="8" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A20" s="7" t="s">
+      <c r="C21" s="8" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A22" s="7" t="s">
         <v>47</v>
       </c>
-      <c r="B20" s="2" t="s">
-        <v>62</v>
-      </c>
-      <c r="C20" s="8" t="s">
+      <c r="B22" s="2" t="s">
         <v>60</v>
       </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A21" s="7" t="s">
-        <v>75</v>
-      </c>
-      <c r="B21" s="2">
+      <c r="C22" s="8" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A23" s="7" t="s">
+        <v>77</v>
+      </c>
+      <c r="B23" s="2">
         <v>0</v>
       </c>
-      <c r="C21" s="8" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A22" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="B22" s="2" t="s">
-        <v>63</v>
-      </c>
-      <c r="C22" s="8" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3" ht="187.2" x14ac:dyDescent="0.3">
-      <c r="A23" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="B23" s="2">
-        <v>1</v>
-      </c>
       <c r="C23" s="8" t="s">
-        <v>53</v>
+        <v>78</v>
       </c>
     </row>
     <row r="24" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A24" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="B24" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="C24" s="8" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" ht="187.2" x14ac:dyDescent="0.3">
+      <c r="A25" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="B25" s="2">
+        <v>1</v>
+      </c>
+      <c r="C25" s="8" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A26" s="7" t="s">
         <v>32</v>
       </c>
-      <c r="B24" s="2">
+      <c r="B26" s="2">
         <v>100</v>
       </c>
-      <c r="C24" s="8" t="s">
+      <c r="C26" s="8" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="25" spans="1:3" ht="43.8" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A25" s="9" t="s">
+    <row r="27" spans="1:3" ht="43.8" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A27" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="B25" s="16" t="s">
+      <c r="B27" s="16" t="s">
+        <v>62</v>
+      </c>
+      <c r="C27" s="10" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" ht="21.6" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A28" s="21" t="s">
+        <v>34</v>
+      </c>
+      <c r="B28" s="21"/>
+      <c r="C28" s="21"/>
+    </row>
+    <row r="29" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A29" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="B29" s="17">
+        <v>1</v>
+      </c>
+      <c r="C29" s="6" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A30" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="B30" s="2">
+        <v>1</v>
+      </c>
+      <c r="C30" s="8" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A31" s="9" t="s">
+        <v>38</v>
+      </c>
+      <c r="B31" s="16">
+        <v>0</v>
+      </c>
+      <c r="C31" s="10" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" ht="21.6" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A32" s="20" t="s">
+        <v>29</v>
+      </c>
+      <c r="B32" s="20"/>
+      <c r="C32" s="20"/>
+    </row>
+    <row r="33" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A33" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="B33" s="17" t="s">
+        <v>18</v>
+      </c>
+      <c r="C33" s="6" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" ht="86.4" x14ac:dyDescent="0.3">
+      <c r="A34" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="B34" s="2">
+        <v>30</v>
+      </c>
+      <c r="C34" s="13" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A35" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="B35" s="2">
+        <v>10</v>
+      </c>
+      <c r="C35" s="13" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7" ht="58.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A36" s="9" t="s">
+        <v>43</v>
+      </c>
+      <c r="B36" s="16">
+        <v>7.0000000000000001E-3</v>
+      </c>
+      <c r="C36" s="14" t="s">
+        <v>44</v>
+      </c>
+      <c r="G36" s="15"/>
+    </row>
+    <row r="37" spans="1:7" ht="21.6" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A37" s="19" t="s">
+        <v>30</v>
+      </c>
+      <c r="B37" s="19"/>
+      <c r="C37" s="19"/>
+    </row>
+    <row r="38" spans="1:7" ht="72" x14ac:dyDescent="0.3">
+      <c r="A38" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="B38" s="17">
+        <v>10</v>
+      </c>
+      <c r="C38" s="6" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7" ht="58.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A39" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="B39" s="16">
+        <v>0.2</v>
+      </c>
+      <c r="C39" s="10" t="s">
         <v>58</v>
       </c>
-      <c r="C25" s="10" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="26" spans="1:3" ht="21.6" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A26" s="22" t="s">
-        <v>34</v>
-      </c>
-      <c r="B26" s="22"/>
-      <c r="C26" s="22"/>
-    </row>
-    <row r="27" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A27" s="5" t="s">
-        <v>35</v>
-      </c>
-      <c r="B27" s="17">
-        <v>1</v>
-      </c>
-      <c r="C27" s="6" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="28" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A28" s="7" t="s">
-        <v>36</v>
-      </c>
-      <c r="B28" s="2">
-        <v>1</v>
-      </c>
-      <c r="C28" s="8" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="29" spans="1:3" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A29" s="9" t="s">
-        <v>38</v>
-      </c>
-      <c r="B29" s="16">
-        <v>0</v>
-      </c>
-      <c r="C29" s="10" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="30" spans="1:3" ht="21.6" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A30" s="20" t="s">
-        <v>29</v>
-      </c>
-      <c r="B30" s="20"/>
-      <c r="C30" s="20"/>
-    </row>
-    <row r="31" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A31" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="B31" s="17" t="s">
-        <v>18</v>
-      </c>
-      <c r="C31" s="6" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="32" spans="1:3" ht="86.4" x14ac:dyDescent="0.3">
-      <c r="A32" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="B32" s="2">
-        <v>30</v>
-      </c>
-      <c r="C32" s="13" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="33" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A33" s="7" t="s">
-        <v>41</v>
-      </c>
-      <c r="B33" s="2">
-        <v>10</v>
-      </c>
-      <c r="C33" s="13" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="34" spans="1:7" ht="58.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A34" s="9" t="s">
-        <v>43</v>
-      </c>
-      <c r="B34" s="16">
-        <v>7.0000000000000001E-3</v>
-      </c>
-      <c r="C34" s="14" t="s">
-        <v>44</v>
-      </c>
-      <c r="G34" s="15"/>
-    </row>
-    <row r="35" spans="1:7" ht="21.6" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A35" s="21" t="s">
-        <v>30</v>
-      </c>
-      <c r="B35" s="21"/>
-      <c r="C35" s="21"/>
-    </row>
-    <row r="36" spans="1:7" ht="72" x14ac:dyDescent="0.3">
-      <c r="A36" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="B36" s="17">
-        <v>10</v>
-      </c>
-      <c r="C36" s="6" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="37" spans="1:7" ht="58.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A37" s="9" t="s">
-        <v>15</v>
-      </c>
-      <c r="B37" s="16">
-        <v>0.2</v>
-      </c>
-      <c r="C37" s="10" t="s">
-        <v>57</v>
-      </c>
     </row>
   </sheetData>
-  <mergeCells count="6">
-    <mergeCell ref="A30:C30"/>
-    <mergeCell ref="A35:C35"/>
+  <mergeCells count="7">
+    <mergeCell ref="A6:C6"/>
     <mergeCell ref="A16:C16"/>
+    <mergeCell ref="A32:C32"/>
+    <mergeCell ref="A37:C37"/>
+    <mergeCell ref="A18:C18"/>
     <mergeCell ref="A14:C14"/>
-    <mergeCell ref="A6:C6"/>
-    <mergeCell ref="A26:C26"/>
+    <mergeCell ref="A28:C28"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
chore: add total_data module case for export folder assigment to umap_expressions
</commit_message>
<xml_diff>
--- a/settings.xlsx
+++ b/settings.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://charitede-my.sharepoint.com/personal/lev_petrov_charite_de/Documents/DOCTORATE/Cytomata_data/anca_panel_1/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="11" documentId="13_ncr:1_{9C262F40-B724-47DA-807B-CA0883A1DDFB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{692FB08E-D1B3-497B-8394-4AD66FE0A642}"/>
+  <xr:revisionPtr revIDLastSave="17" documentId="13_ncr:1_{9C262F40-B724-47DA-807B-CA0883A1DDFB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A1005B3A-DE90-4612-B4DF-06226767E48E}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-27360" yWindow="-10155" windowWidth="21600" windowHeight="11235" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -264,7 +264,7 @@
     <t>0 (off, default) or 1 (on)</t>
   </si>
   <si>
-    <t>B, CD4_T, CD8_T, Monos_and_DCs, NK, TCRgd_T</t>
+    <t>CD4_T, CD8_T, TCRgd_T, B, Monos_and_DCs, NK</t>
   </si>
 </sst>
 </file>
@@ -778,8 +778,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G39"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A15" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C24" sqref="C24"/>
+    <sheetView tabSelected="1" topLeftCell="A19" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B24" sqref="B24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -856,7 +856,7 @@
         <v>25</v>
       </c>
       <c r="B7" s="17">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C7" s="6" t="s">
         <v>24</v>
@@ -940,7 +940,7 @@
         <v>27</v>
       </c>
       <c r="B15" s="18">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C15" s="12" t="s">
         <v>24</v>
@@ -958,7 +958,7 @@
         <v>76</v>
       </c>
       <c r="B17" s="18">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C17" s="12" t="s">
         <v>24</v>

</xml_diff>